<commit_message>
Storage state start and end values should work. Also storage_state_reference_value and storage_state_reference_price.
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915369DC-7E2C-43F6-9D46-B66ED24A38DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAD5DBE-0F67-4664-95FB-A333660967A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" activeTab="9" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="457">
   <si>
     <t>commodity</t>
   </si>
@@ -1525,6 +1525,57 @@
   </si>
   <si>
     <t>connection_node_constraint_c</t>
+  </si>
+  <si>
+    <t>storage_binding_method</t>
+  </si>
+  <si>
+    <t>Choice how the storage state will be maintained between periods. 'bind_within_period' will bind the end level to the beginning of the same period. 'bind_between_periods' will bind the end level to the beginning of the next period.</t>
+  </si>
+  <si>
+    <t>storage_state_start</t>
+  </si>
+  <si>
+    <t>[0-1] Relative state of storage at the beginning of the first model solve (irrespective of when the model starts). Constant.</t>
+  </si>
+  <si>
+    <t>storate_state_end</t>
+  </si>
+  <si>
+    <t>[0-1] Relative state of storage at the end of the last model solve (overrides 'storage_state_end_reference'). Constant.</t>
+  </si>
+  <si>
+    <t>[0-1] Relative state of storage at then end of each solve (can be overwritten in the next solve). Constant.</t>
+  </si>
+  <si>
+    <t>storage_start_end_method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choice whether the start and end states of storage are fixed in the beginning and end of the whole model timeline (not between solves). Uses 'storage_state_start' and 'storage_state_end'. </t>
+  </si>
+  <si>
+    <t>storage_solve_horizon_method</t>
+  </si>
+  <si>
+    <t>Choice how to treat storage state at the end of time horizon of each solve. ''free'' lets the model choose the end state. ''use_reference_value'' forces the end state to the specific value set in ''storage_state_reference_value''. ''use_reference_price'' gives the storage state a price in the objective function based on the ''storage_state_reference_price''. '</t>
+  </si>
+  <si>
+    <t>storage_state_reference_value</t>
+  </si>
+  <si>
+    <t>storage_state_reference_price</t>
+  </si>
+  <si>
+    <t>[CUR/MWh] Price for the stored energy at the end of the solve horizon. Requires 'use_reference_price' in 'storage_solve_horizon_method'. Constant or period.</t>
+  </si>
+  <si>
+    <t>fix_start</t>
+  </si>
+  <si>
+    <t>bind_between_timeblocks</t>
+  </si>
+  <si>
+    <t>use_reference_value</t>
   </si>
 </sst>
 </file>
@@ -2538,10 +2589,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="8092152" cy="1395318"/>
     <xdr:sp macro="" textlink="">
@@ -2557,7 +2608,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16392525" y="542925"/>
+          <a:off x="22488525" y="695325"/>
           <a:ext cx="8092152" cy="1395318"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3156,7 +3207,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3514,43 +3567,48 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" customWidth="1"/>
-    <col min="14" max="14" width="10.28515625" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" style="14" customWidth="1"/>
-    <col min="16" max="16" width="9.85546875" style="14" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" style="14" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" style="14" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" customWidth="1"/>
-    <col min="22" max="22" width="18.140625" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10.28515625" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" style="14" customWidth="1"/>
+    <col min="19" max="19" width="9.85546875" style="14" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" style="14" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" style="14" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" customWidth="1"/>
+    <col min="24" max="24" width="8.140625" customWidth="1"/>
+    <col min="25" max="26" width="18.140625" customWidth="1"/>
+    <col min="27" max="27" width="16.85546875" customWidth="1"/>
+    <col min="28" max="29" width="29.140625" customWidth="1"/>
+    <col min="30" max="30" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>250</v>
       </c>
@@ -3571,55 +3629,76 @@
         <v>186</v>
       </c>
       <c r="H1" t="s">
+        <v>441</v>
+      </c>
+      <c r="I1" t="s">
+        <v>448</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="K1" t="s">
         <v>155</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>171</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>367</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>368</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>68</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>71</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>301</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>72</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>302</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>369</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>370</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>371</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>24</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>73</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
+        <v>443</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>453</v>
+      </c>
+      <c r="AD1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3642,55 +3721,76 @@
         <v>11</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="U2" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="Z2" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>451</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>452</v>
+      </c>
+      <c r="AD2" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -3710,14 +3810,14 @@
       <c r="G3" t="s">
         <v>147</v>
       </c>
-      <c r="J3">
+      <c r="M3">
         <v>10000</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>10000</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
@@ -3737,18 +3837,18 @@
       <c r="G4" t="s">
         <v>147</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <f>100*8760</f>
         <v>876000</v>
       </c>
-      <c r="J4">
+      <c r="M4">
         <v>10000</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -3761,14 +3861,14 @@
       <c r="G5" t="s">
         <v>147</v>
       </c>
-      <c r="J5">
+      <c r="M5">
         <v>10000</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -3781,14 +3881,14 @@
       <c r="G6" t="s">
         <v>147</v>
       </c>
-      <c r="J6">
+      <c r="M6">
         <v>10000</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>298</v>
       </c>
@@ -3807,20 +3907,35 @@
       <c r="G7" t="s">
         <v>147</v>
       </c>
-      <c r="J7">
+      <c r="H7" t="s">
+        <v>455</v>
+      </c>
+      <c r="I7" t="s">
+        <v>454</v>
+      </c>
+      <c r="J7" t="s">
+        <v>456</v>
+      </c>
+      <c r="M7">
         <v>12000</v>
       </c>
-      <c r="K7">
+      <c r="N7">
         <v>12000</v>
       </c>
-      <c r="L7">
+      <c r="O7">
         <v>20</v>
       </c>
-      <c r="V7">
+      <c r="Y7">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Z7">
+        <v>0.1</v>
+      </c>
+      <c r="AB7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>404</v>
       </c>
@@ -3833,13 +3948,13 @@
       <c r="G8" t="s">
         <v>147</v>
       </c>
-      <c r="J8">
+      <c r="M8">
         <v>12000</v>
       </c>
-      <c r="K8">
+      <c r="N8">
         <v>12000</v>
       </c>
-      <c r="L8">
+      <c r="O8">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update init alternatives and import more time results
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAD5DBE-0F67-4664-95FB-A333660967A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB35B2E9-E85D-4BBE-811F-52105385FCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" activeTab="9" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="16215" yWindow="2460" windowWidth="23010" windowHeight="13800" tabRatio="1000" activeTab="9" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -1530,9 +1530,6 @@
     <t>storage_binding_method</t>
   </si>
   <si>
-    <t>Choice how the storage state will be maintained between periods. 'bind_within_period' will bind the end level to the beginning of the same period. 'bind_between_periods' will bind the end level to the beginning of the next period.</t>
-  </si>
-  <si>
     <t>storage_state_start</t>
   </si>
   <si>
@@ -1557,9 +1554,6 @@
     <t>storage_solve_horizon_method</t>
   </si>
   <si>
-    <t>Choice how to treat storage state at the end of time horizon of each solve. ''free'' lets the model choose the end state. ''use_reference_value'' forces the end state to the specific value set in ''storage_state_reference_value''. ''use_reference_price'' gives the storage state a price in the objective function based on the ''storage_state_reference_price''. '</t>
-  </si>
-  <si>
     <t>storage_state_reference_value</t>
   </si>
   <si>
@@ -1572,10 +1566,16 @@
     <t>fix_start</t>
   </si>
   <si>
-    <t>bind_between_timeblocks</t>
-  </si>
-  <si>
     <t>use_reference_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Choice how to treat storage state at the end of time horizon of each solve. 'free' lets the model choose the end state. 'use_reference_value' forces the end state to the specific value set in 'storage_state_reference_value'. 'use_reference_price' gives the storage state a price in the objective function based on the 'storage_state_reference_price'. </t>
+  </si>
+  <si>
+    <t>Choice how the storage state will be maintained over discontinuos timelines. Default 'bind_within_timeblocks' will bind the storage end state at the end of the timeblock to the beginning of the timeblock. 'bind_within_period', 'bind_within_solve' and bind_within_model' will act similarly but over increasingly longer time span. Meanwhile 'bind_forward_only' will bind forward over any holes in the used timeline, but will not bind end to the start. Separate parameters (e.g. 'storage_state_start') can force bindings.</t>
+  </si>
+  <si>
+    <t>bind_within_timeblocks</t>
   </si>
 </sst>
 </file>
@@ -3629,13 +3629,13 @@
         <v>186</v>
       </c>
       <c r="H1" t="s">
-        <v>441</v>
+        <v>455</v>
       </c>
       <c r="I1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="K1" t="s">
         <v>155</v>
@@ -3683,16 +3683,16 @@
         <v>73</v>
       </c>
       <c r="Z1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AA1" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="AB1" t="s">
         <v>445</v>
       </c>
-      <c r="AB1" t="s">
-        <v>446</v>
-      </c>
       <c r="AC1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="AD1" t="s">
         <v>74</v>
@@ -3724,10 +3724,10 @@
         <v>440</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>59</v>
@@ -3775,16 +3775,16 @@
         <v>65</v>
       </c>
       <c r="Z2" s="9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AB2" s="9" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>66</v>
@@ -3908,13 +3908,13 @@
         <v>147</v>
       </c>
       <c r="H7" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="I7" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="J7" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="M7">
         <v>12000</v>

</xml_diff>

<commit_message>
Fix profile mistake and add more results.
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAD5DBE-0F67-4664-95FB-A333660967A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86ACC96-05B8-4BCE-BFEE-4E7B883E3AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" activeTab="9" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" firstSheet="11" activeTab="39" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -3569,7 +3569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -6531,14 +6531,14 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="20" customWidth="1"/>
     <col min="5" max="5" width="11.140625" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
@@ -9633,11 +9633,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBE8270-58BA-4E52-BE5C-E66A62EB7AF6}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9754,7 +9754,7 @@
         <v>148</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>406</v>

</xml_diff>

<commit_message>
Added large failure (n-1) reserve method
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86ACC96-05B8-4BCE-BFEE-4E7B883E3AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59471DED-C27B-47EC-91C2-6EFEA8EE4E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" firstSheet="11" activeTab="39" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="38700" windowHeight="15435" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -1071,9 +1071,6 @@
     <t>JustA</t>
   </si>
   <si>
-    <t>Choice of reserve method: no_reserve, timeseries_only, dynamic_only, both</t>
-  </si>
-  <si>
     <t>timeseries_only</t>
   </si>
   <si>
@@ -1576,6 +1573,9 @@
   </si>
   <si>
     <t>use_reference_value</t>
+  </si>
+  <si>
+    <t>Choice of reserve method: no_reserve, timeseries_only, dynamic_only, large_failure_only, timeseries_and_dynamic, timeseries_and_large_failure, dynamic_and_large_failure, all</t>
   </si>
 </sst>
 </file>
@@ -3207,9 +3207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3238,7 +3236,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
@@ -3485,28 +3483,28 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
@@ -3614,13 +3612,13 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D1" t="s">
         <v>183</v>
       </c>
       <c r="E1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F1" t="s">
         <v>184</v>
@@ -3629,13 +3627,13 @@
         <v>186</v>
       </c>
       <c r="H1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="K1" t="s">
         <v>155</v>
@@ -3644,10 +3642,10 @@
         <v>171</v>
       </c>
       <c r="M1" t="s">
+        <v>366</v>
+      </c>
+      <c r="N1" t="s">
         <v>367</v>
-      </c>
-      <c r="N1" t="s">
-        <v>368</v>
       </c>
       <c r="O1" t="s">
         <v>68</v>
@@ -3656,25 +3654,25 @@
         <v>71</v>
       </c>
       <c r="Q1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="R1" t="s">
         <v>72</v>
       </c>
       <c r="S1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="T1" t="s">
+        <v>368</v>
+      </c>
+      <c r="U1" t="s">
         <v>369</v>
-      </c>
-      <c r="U1" t="s">
-        <v>370</v>
       </c>
       <c r="V1" t="s">
         <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="X1" t="s">
         <v>24</v>
@@ -3683,16 +3681,16 @@
         <v>73</v>
       </c>
       <c r="Z1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="AA1" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="AB1" t="s">
         <v>445</v>
       </c>
-      <c r="AB1" t="s">
-        <v>446</v>
-      </c>
       <c r="AC1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="AD1" t="s">
         <v>74</v>
@@ -3706,7 +3704,7 @@
         <v>58</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>60</v>
@@ -3721,13 +3719,13 @@
         <v>11</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>59</v>
@@ -3754,7 +3752,7 @@
         <v>14</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>7</v>
@@ -3775,16 +3773,16 @@
         <v>65</v>
       </c>
       <c r="Z2" s="9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AB2" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="AC2" s="9" t="s">
         <v>451</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>452</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>66</v>
@@ -3804,7 +3802,7 @@
         <v>160</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
@@ -3831,7 +3829,7 @@
         <v>160</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
@@ -3890,7 +3888,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>275</v>
@@ -3908,13 +3906,13 @@
         <v>147</v>
       </c>
       <c r="H7" t="s">
+        <v>454</v>
+      </c>
+      <c r="I7" t="s">
+        <v>453</v>
+      </c>
+      <c r="J7" t="s">
         <v>455</v>
-      </c>
-      <c r="I7" t="s">
-        <v>454</v>
-      </c>
-      <c r="J7" t="s">
-        <v>456</v>
       </c>
       <c r="M7">
         <v>12000</v>
@@ -3937,10 +3935,10 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>160</v>
@@ -4011,19 +4009,19 @@
         <v>70</v>
       </c>
       <c r="G1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I1" t="s">
         <v>372</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>368</v>
+      </c>
+      <c r="K1" t="s">
         <v>373</v>
-      </c>
-      <c r="J1" t="s">
-        <v>369</v>
-      </c>
-      <c r="K1" t="s">
-        <v>374</v>
       </c>
       <c r="L1" t="s">
         <v>21</v>
@@ -4032,7 +4030,7 @@
         <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4061,7 +4059,7 @@
         <v>13</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
@@ -4493,7 +4491,7 @@
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4569,7 +4567,7 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4733,7 +4731,7 @@
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F1" t="s">
         <v>180</v>
@@ -4757,19 +4755,19 @@
         <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="N1" t="s">
         <v>26</v>
       </c>
       <c r="O1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P1" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q1" t="s">
         <v>377</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>378</v>
       </c>
       <c r="R1" t="s">
         <v>21</v>
@@ -4778,10 +4776,10 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
+        <v>378</v>
+      </c>
+      <c r="U1" t="s">
         <v>379</v>
-      </c>
-      <c r="U1" t="s">
-        <v>380</v>
       </c>
       <c r="V1" t="s">
         <v>19</v>
@@ -4801,7 +4799,7 @@
         <v>282</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -4813,7 +4811,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -4831,7 +4829,7 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
@@ -4901,7 +4899,7 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>274</v>
@@ -4933,7 +4931,7 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
@@ -4945,7 +4943,7 @@
         <v>149</v>
       </c>
       <c r="H5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -4994,19 +4992,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H1" t="s">
+        <v>376</v>
+      </c>
+      <c r="I1" t="s">
         <v>377</v>
-      </c>
-      <c r="I1" t="s">
-        <v>378</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -5015,7 +5013,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -5038,7 +5036,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
@@ -5403,10 +5401,10 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E1" t="s">
         <v>181</v>
@@ -5424,19 +5422,19 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M1" t="s">
+        <v>380</v>
+      </c>
+      <c r="N1" t="s">
         <v>381</v>
-      </c>
-      <c r="N1" t="s">
-        <v>382</v>
       </c>
       <c r="O1" t="s">
         <v>21</v>
@@ -5445,7 +5443,7 @@
         <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="R1" t="s">
         <v>172</v>
@@ -5454,10 +5452,10 @@
         <v>111</v>
       </c>
       <c r="T1" t="s">
+        <v>314</v>
+      </c>
+      <c r="U1" t="s">
         <v>315</v>
-      </c>
-      <c r="U1" t="s">
-        <v>316</v>
       </c>
       <c r="V1" t="s">
         <v>199</v>
@@ -5466,7 +5464,7 @@
         <v>200</v>
       </c>
       <c r="X1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5477,7 +5475,7 @@
         <v>125</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>110</v>
@@ -5504,7 +5502,7 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
@@ -5554,7 +5552,7 @@
         <v>160</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E3" s="47" t="s">
         <v>174</v>
@@ -5621,10 +5619,10 @@
         <v>160</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
@@ -5642,27 +5640,27 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>151</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="C7" s="47" t="s">
         <v>160</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E7" s="47" t="s">
         <v>174</v>
@@ -5872,7 +5870,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
@@ -5881,12 +5879,12 @@
         <v>194</v>
       </c>
       <c r="D15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
@@ -5895,12 +5893,12 @@
         <v>194</v>
       </c>
       <c r="D16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
@@ -5909,12 +5907,12 @@
         <v>194</v>
       </c>
       <c r="D17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
@@ -5923,12 +5921,12 @@
         <v>194</v>
       </c>
       <c r="D18" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
@@ -5937,12 +5935,12 @@
         <v>194</v>
       </c>
       <c r="D19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
@@ -5951,12 +5949,12 @@
         <v>194</v>
       </c>
       <c r="D20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
@@ -5965,12 +5963,12 @@
         <v>194</v>
       </c>
       <c r="D21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
@@ -5979,12 +5977,12 @@
         <v>194</v>
       </c>
       <c r="D22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
@@ -5993,12 +5991,12 @@
         <v>194</v>
       </c>
       <c r="D23" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
@@ -6007,12 +6005,12 @@
         <v>194</v>
       </c>
       <c r="D24" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
@@ -6021,12 +6019,12 @@
         <v>194</v>
       </c>
       <c r="D25" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
@@ -6035,12 +6033,12 @@
         <v>194</v>
       </c>
       <c r="D26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B27" s="25">
         <v>44701</v>
@@ -6049,12 +6047,12 @@
         <v>194</v>
       </c>
       <c r="D27" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B28" s="25">
         <v>44712</v>
@@ -6063,12 +6061,12 @@
         <v>194</v>
       </c>
       <c r="D28" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B29" s="25">
         <v>44727</v>
@@ -6077,12 +6075,12 @@
         <v>194</v>
       </c>
       <c r="D29" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B30" s="25">
         <v>44734</v>
@@ -6091,12 +6089,12 @@
         <v>194</v>
       </c>
       <c r="D30" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B31" s="25">
         <v>44741</v>
@@ -6105,7 +6103,7 @@
         <v>194</v>
       </c>
       <c r="D31" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -6152,19 +6150,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H1" t="s">
+        <v>380</v>
+      </c>
+      <c r="I1" t="s">
         <v>381</v>
-      </c>
-      <c r="I1" t="s">
-        <v>382</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -6173,7 +6171,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M1" t="s">
         <v>172</v>
@@ -6199,7 +6197,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
@@ -6564,7 +6562,7 @@
         <v>143</v>
       </c>
       <c r="F1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G1" t="s">
         <v>257</v>
@@ -6576,7 +6574,7 @@
         <v>120</v>
       </c>
       <c r="J1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K1" t="s">
         <v>122</v>
@@ -6585,7 +6583,7 @@
         <v>124</v>
       </c>
       <c r="M1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -6602,7 +6600,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>142</v>
@@ -6611,7 +6609,7 @@
         <v>18</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>113</v>
@@ -6629,7 +6627,7 @@
         <v>123</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -6646,7 +6644,7 @@
         <v>150</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6669,7 +6667,7 @@
         <v>148</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6689,7 +6687,7 @@
         <v>161</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -6706,7 +6704,7 @@
         <v>149</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6726,7 +6724,7 @@
         <v>148</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6737,16 +6735,16 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>161</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -6754,16 +6752,16 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>148</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -6771,16 +6769,16 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>405</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -6856,10 +6854,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>342</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7099,7 +7097,7 @@
         <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7119,7 +7117,7 @@
         <v>276</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7757,16 +7755,16 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C4" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>412</v>
-      </c>
       <c r="E4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -7785,7 +7783,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7817,7 +7815,7 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D1" t="s">
         <v>41</v>
@@ -7826,7 +7824,7 @@
         <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G1" t="s">
         <v>43</v>
@@ -7835,7 +7833,7 @@
         <v>47</v>
       </c>
       <c r="I1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J1" t="s">
         <v>45</v>
@@ -7844,7 +7842,7 @@
         <v>55</v>
       </c>
       <c r="L1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="M1" t="s">
         <v>39</v>
@@ -7856,16 +7854,16 @@
         <v>53</v>
       </c>
       <c r="P1" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q1" t="s">
         <v>347</v>
       </c>
-      <c r="Q1" t="s">
-        <v>348</v>
-      </c>
       <c r="R1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="S1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -7876,7 +7874,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>40</v>
@@ -7885,7 +7883,7 @@
         <v>36</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>42</v>
@@ -7903,7 +7901,7 @@
         <v>54</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>38</v>
@@ -7915,16 +7913,16 @@
         <v>52</v>
       </c>
       <c r="P2" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="Q2" s="9" t="s">
-        <v>346</v>
-      </c>
       <c r="R2" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="S2" s="9" t="s">
         <v>362</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -7960,7 +7958,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>287</v>
@@ -7974,10 +7972,10 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="P6">
         <v>40</v>
@@ -7991,7 +7989,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C7" t="s">
         <v>160</v>
@@ -8056,16 +8054,16 @@
         <v>51</v>
       </c>
       <c r="J1" t="s">
+        <v>346</v>
+      </c>
+      <c r="K1" t="s">
         <v>347</v>
       </c>
-      <c r="K1" t="s">
-        <v>348</v>
-      </c>
       <c r="L1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -8097,16 +8095,16 @@
         <v>50</v>
       </c>
       <c r="J2" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>346</v>
-      </c>
       <c r="L2" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>362</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -8181,7 +8179,7 @@
         <v>250</v>
       </c>
       <c r="B1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8190,42 +8188,42 @@
         <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>324</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>391</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>29</v>
@@ -8266,91 +8264,91 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="F4" t="s">
         <v>323</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>298</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="F4" t="s">
-        <v>324</v>
-      </c>
       <c r="G4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="J4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J5" t="s">
+        <v>389</v>
+      </c>
+      <c r="K5" t="s">
         <v>390</v>
-      </c>
-      <c r="K5" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -8501,7 +8499,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>148</v>
@@ -8509,7 +8507,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>149</v>
@@ -8597,7 +8595,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>151</v>
@@ -8608,7 +8606,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>163</v>
@@ -8696,7 +8694,7 @@
         <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>129</v>
@@ -8719,10 +8717,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>286</v>
@@ -8783,16 +8781,16 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>288</v>
+        <v>456</v>
       </c>
       <c r="F1" t="s">
         <v>138</v>
       </c>
       <c r="G1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -8835,10 +8833,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>286</v>
@@ -8847,7 +8845,7 @@
         <v>287</v>
       </c>
       <c r="E3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -9061,7 +9059,7 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9125,7 +9123,7 @@
         <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>129</v>
@@ -9148,10 +9146,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>286</v>
@@ -9174,10 +9172,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>286</v>
@@ -9200,10 +9198,10 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>286</v>
@@ -9226,10 +9224,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>286</v>
@@ -9252,10 +9250,10 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>286</v>
@@ -9310,7 +9308,7 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E1" t="s">
         <v>158</v>
@@ -9333,7 +9331,7 @@
         <v>156</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>157</v>
@@ -9364,13 +9362,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>406</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>407</v>
       </c>
       <c r="D4" t="s">
         <v>160</v>
@@ -9497,7 +9495,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -9517,7 +9515,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -9537,7 +9535,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>164</v>
@@ -9557,7 +9555,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>35</v>
@@ -9577,7 +9575,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>35</v>
@@ -9597,7 +9595,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>202</v>
@@ -9633,7 +9631,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBE8270-58BA-4E52-BE5C-E66A62EB7AF6}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -9660,7 +9658,7 @@
       <c r="D1" s="3"/>
       <c r="E1"/>
       <c r="F1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -9674,13 +9672,13 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>144</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9694,7 +9692,7 @@
         <v>150</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>178</v>
@@ -9714,7 +9712,7 @@
         <v>148</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>178</v>
@@ -9725,19 +9723,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>161</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -9745,19 +9743,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>148</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -9800,7 +9798,7 @@
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -9817,7 +9815,7 @@
         <v>144</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -9856,10 +9854,10 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
+        <v>427</v>
+      </c>
+      <c r="E1" t="s">
         <v>428</v>
-      </c>
-      <c r="E1" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -9873,10 +9871,10 @@
         <v>144</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>430</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -9914,7 +9912,7 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -9928,7 +9926,7 @@
         <v>144</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -9966,7 +9964,7 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -9980,7 +9978,7 @@
         <v>144</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -10018,10 +10016,10 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10035,7 +10033,7 @@
         <v>169</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -10049,13 +10047,13 @@
         <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>34</v>
@@ -10064,12 +10062,12 @@
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>164</v>
@@ -10078,12 +10076,12 @@
         <v>170</v>
       </c>
       <c r="D5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>35</v>
@@ -10092,12 +10090,12 @@
         <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>202</v>
@@ -10106,51 +10104,51 @@
         <v>170</v>
       </c>
       <c r="D7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>202</v>
       </c>
       <c r="D11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -10284,7 +10282,7 @@
         <v>212</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix timeseries unit outputs. Fix excel importer. Add EV scenario.
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F97E5D-6F3D-467C-B9AF-781013E29D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0901498C-B61B-49BC-B03B-58EA9D517645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="405" yWindow="1905" windowWidth="24900" windowHeight="17970" tabRatio="1000" activeTab="9" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="30" activeTab="41" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1308" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="460">
   <si>
     <t>commodity</t>
   </si>
@@ -1515,9 +1515,6 @@
     <t>15.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Added new sheets for state and capacity constraints. Changed </t>
-  </si>
-  <si>
     <t>connection_node_constraint_c</t>
   </si>
   <si>
@@ -1576,6 +1573,18 @@
   </si>
   <si>
     <t>has_storage</t>
+  </si>
+  <si>
+    <t>Added new sheets for state and capacity constraints. Changed location of unit constraint sheets to the end.</t>
+  </si>
+  <si>
+    <t>16.0</t>
+  </si>
+  <si>
+    <t>In 'node_c' 'has_state' to 'has_storage'. In 'node_c' added 'storage_binding_method', 'storage_start_end_method', 'storage_solve_horizon_method', 'storage_state_start', 'storage_state_end', 'storage_state_reference_value', 'storage_state_reference_price'.</t>
+  </si>
+  <si>
+    <t>foo</t>
   </si>
 </sst>
 </file>
@@ -3208,7 +3217,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3485,7 +3494,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
@@ -3569,11 +3578,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="Z1" sqref="Z1:AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3629,13 +3638,13 @@
         <v>185</v>
       </c>
       <c r="H1" t="s">
+        <v>453</v>
+      </c>
+      <c r="I1" t="s">
         <v>454</v>
       </c>
-      <c r="I1" t="s">
-        <v>455</v>
-      </c>
       <c r="J1" s="5" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K1" t="s">
         <v>154</v>
@@ -3683,16 +3692,16 @@
         <v>72</v>
       </c>
       <c r="Z1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AA1" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="AB1" t="s">
         <v>442</v>
       </c>
-      <c r="AB1" t="s">
-        <v>443</v>
-      </c>
       <c r="AC1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="AD1" t="s">
         <v>73</v>
@@ -3715,19 +3724,19 @@
         <v>265</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>444</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>445</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>59</v>
@@ -3775,16 +3784,16 @@
         <v>64</v>
       </c>
       <c r="Z2" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="AA2" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AB2" s="9" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC2" s="9" t="s">
         <v>447</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>448</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>65</v>
@@ -3908,13 +3917,13 @@
         <v>146</v>
       </c>
       <c r="H7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I7" t="s">
+        <v>449</v>
+      </c>
+      <c r="J7" t="s">
         <v>450</v>
-      </c>
-      <c r="J7" t="s">
-        <v>451</v>
       </c>
       <c r="M7">
         <v>12000</v>
@@ -4698,7 +4707,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5364,10 +5373,10 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="X2" sqref="X1:X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5687,9 +5696,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6105,7 +6116,32 @@
         <v>193</v>
       </c>
       <c r="D31" t="s">
-        <v>436</v>
+        <v>456</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="B32" s="25">
+        <v>44840</v>
+      </c>
+      <c r="C32" t="s">
+        <v>193</v>
+      </c>
+      <c r="D32" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="B33" s="25">
+        <v>44840</v>
+      </c>
+      <c r="C33" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -7785,7 +7821,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8783,7 +8819,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F1" t="s">
         <v>137</v>
@@ -9830,13 +9866,13 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0A3667-1C00-43CD-99E7-8F765FEBD719}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9877,6 +9913,20 @@
       </c>
       <c r="E2" s="9" t="s">
         <v>429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>459</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -9947,7 +9997,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="Q57" sqref="Q57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixing bugs in the Excel import. Adding marginal investment cost.
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0901498C-B61B-49BC-B03B-58EA9D517645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7F03DA-00E3-4261-8F3E-10878A94064B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="30" activeTab="41" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1316" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="459">
   <si>
     <t>commodity</t>
   </si>
@@ -1582,9 +1582,6 @@
   </si>
   <si>
     <t>In 'node_c' 'has_state' to 'has_storage'. In 'node_c' added 'storage_binding_method', 'storage_start_end_method', 'storage_solve_horizon_method', 'storage_state_start', 'storage_state_end', 'storage_state_reference_value', 'storage_state_reference_price'.</t>
-  </si>
-  <si>
-    <t>foo</t>
   </si>
 </sst>
 </file>
@@ -3216,9 +3213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5698,7 +5693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -9866,9 +9861,9 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0A3667-1C00-43CD-99E7-8F765FEBD719}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -9913,20 +9908,6 @@
       </c>
       <c r="E2" s="9" t="s">
         <v>429</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing node_constraint, unit_constraint and connection_constraint importing from FlexTool_import_template.xlsx
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7F03DA-00E3-4261-8F3E-10878A94064B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A3C16C-8353-4065-92ED-727DADB2179D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="463">
   <si>
     <t>commodity</t>
   </si>
@@ -1582,6 +1582,18 @@
   </si>
   <si>
     <t>In 'node_c' 'has_state' to 'has_storage'. In 'node_c' added 'storage_binding_method', 'storage_start_end_method', 'storage_solve_horizon_method', 'storage_state_start', 'storage_state_end', 'storage_state_reference_value', 'storage_state_reference_price'.</t>
+  </si>
+  <si>
+    <t>[MW] Size of single connection - used for investments and some technical limits. If not provided, existing capacity is assumed. Constant.</t>
+  </si>
+  <si>
+    <t>Added 'virtual_unitsize' to 'connection_c'</t>
+  </si>
+  <si>
+    <t>16.1</t>
+  </si>
+  <si>
+    <t>battery_tie_kW_kWh</t>
   </si>
 </sst>
 </file>
@@ -2805,7 +2817,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -3213,7 +3225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3571,13 +3583,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
-  <dimension ref="A1:AD8"/>
+  <dimension ref="A1:AD9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Z1" sqref="Z1:AC2"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3960,6 +3972,32 @@
       </c>
       <c r="O8">
         <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="G9" t="s">
+        <v>324</v>
+      </c>
+      <c r="P9">
+        <v>800</v>
+      </c>
+      <c r="T9" s="14">
+        <v>200</v>
+      </c>
+      <c r="V9" s="14">
+        <v>0.05</v>
+      </c>
+      <c r="X9">
+        <v>10</v>
+      </c>
+      <c r="AD9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4556,7 +4594,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4696,7 +4734,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44D2B2-1DE7-400D-8C40-2CD59BEE6EC3}">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
@@ -4727,9 +4765,10 @@
     <col min="20" max="20" width="10.5703125" customWidth="1"/>
     <col min="21" max="21" width="13.140625" customWidth="1"/>
     <col min="22" max="22" width="10" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>249</v>
       </c>
@@ -4790,8 +4829,11 @@
       <c r="V1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -4858,8 +4900,11 @@
       <c r="V2" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W2" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -4890,20 +4935,8 @@
       <c r="K3">
         <v>100</v>
       </c>
-      <c r="L3">
-        <v>100</v>
-      </c>
-      <c r="P3">
-        <v>500</v>
-      </c>
-      <c r="R3">
-        <v>0.05</v>
-      </c>
-      <c r="S3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>296</v>
       </c>
@@ -4935,7 +4968,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>322</v>
       </c>
@@ -4950,6 +4983,53 @@
       </c>
       <c r="H5" t="s">
         <v>324</v>
+      </c>
+      <c r="L5">
+        <v>100</v>
+      </c>
+      <c r="P5">
+        <v>500</v>
+      </c>
+      <c r="R5">
+        <v>0.05</v>
+      </c>
+      <c r="S5">
+        <v>50</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="H6" t="s">
+        <v>324</v>
+      </c>
+      <c r="L6">
+        <v>100</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0.05</v>
+      </c>
+      <c r="S6">
+        <v>20</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4969,7 +5049,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5368,10 +5448,10 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="X2" sqref="X1:X2"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5693,13 +5773,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6128,15 +6209,18 @@
         <v>458</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="B33" s="25">
-        <v>44840</v>
+        <v>44850</v>
       </c>
       <c r="C33" t="s">
         <v>193</v>
+      </c>
+      <c r="D33" t="s">
+        <v>460</v>
       </c>
     </row>
   </sheetData>
@@ -6562,7 +6646,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6833,7 +6917,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7104,7 +7188,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7575,7 +7659,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7816,7 +7900,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8044,7 +8128,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8198,7 +8282,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9317,19 +9401,19 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C017E3-B844-46CF-8B82-D76F5D9D7ACD}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
     <col min="4" max="9" width="11.5703125" customWidth="1"/>
   </cols>
@@ -9407,6 +9491,23 @@
         <v>159</v>
       </c>
       <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5">
         <v>0</v>
       </c>
     </row>
@@ -9426,7 +9527,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9810,7 +9911,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9861,20 +9962,20 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF0A3667-1C00-43CD-99E7-8F765FEBD719}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="11.5703125" customWidth="1"/>
@@ -9908,6 +10009,20 @@
       </c>
       <c r="E2" s="9" t="s">
         <v>429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -9972,20 +10087,20 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D55AA85F-4B1E-49C3-94EB-B0A94205CD7C}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q57" sqref="Q57"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="20" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="11.5703125" customWidth="1"/>
   </cols>
@@ -10012,6 +10127,20 @@
       </c>
       <c r="D2" s="9" t="s">
         <v>429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="D3">
+        <v>-8</v>
       </c>
     </row>
   </sheetData>
@@ -10030,7 +10159,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Remove outputting of utilization and unit cost (for now). Update template to fix wrong storage binding method name in description.
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A3C16C-8353-4065-92ED-727DADB2179D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05485BB-8A58-49E7-9C81-7E55AD0A5D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" activeTab="9" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -1566,9 +1566,6 @@
     <t>bind_within_period</t>
   </si>
   <si>
-    <t>Choice how the storage state will be maintained over discontinuos timelines. Default 'bind_between_timeblocks' will bind the storage end state at the end of the timeblock to the beginning of the timeblock. 'bind_within_period', 'bind_within_solve' and bind_within_model' will act similarly but over increasingly longer time span. Meanwhile 'bind_forward_only' will bind forward over any holes in the used timeline, but will not bind end to the start. Separate parameters (e.g. 'storage_state_start') can force bindings.</t>
-  </si>
-  <si>
     <t>Choice whether the start and end states of storage are fixed in the beginning and end of the whole model timeline (not between solves). Uses 'storage_state_start' and 'storage_state_end'. Options: 'fix_nothing', 'fix_start', 'fix_end', 'fix_start_end'.</t>
   </si>
   <si>
@@ -1594,6 +1591,9 @@
   </si>
   <si>
     <t>battery_tie_kW_kWh</t>
+  </si>
+  <si>
+    <t>Choice how the storage state will be maintained over discontinuos timelines. Default 'bind_within_timeblock' will bind the storage end state at the end of the timeblock to the beginning of the timeblock. 'bind_within_period', 'bind_within_solve' and bind_within_model' will act similarly but over increasingly longer time span. Meanwhile 'bind_forward_only' will bind forward over any holes in the used timeline, but will not bind end to the start. Separate parameters (e.g. 'storage_state_start') can force bindings.</t>
   </si>
 </sst>
 </file>
@@ -3225,7 +3225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3585,11 +3585,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3645,10 +3645,10 @@
         <v>185</v>
       </c>
       <c r="H1" t="s">
+        <v>462</v>
+      </c>
+      <c r="I1" t="s">
         <v>453</v>
-      </c>
-      <c r="I1" t="s">
-        <v>454</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>445</v>
@@ -3731,7 +3731,7 @@
         <v>265</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>11</v>
@@ -4830,7 +4830,7 @@
         <v>19</v>
       </c>
       <c r="W1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -6192,12 +6192,12 @@
         <v>193</v>
       </c>
       <c r="D31" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B32" s="25">
         <v>44840</v>
@@ -6206,12 +6206,12 @@
         <v>193</v>
       </c>
       <c r="D32" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B33" s="25">
         <v>44850</v>
@@ -6220,7 +6220,7 @@
         <v>193</v>
       </c>
       <c r="D33" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -9499,7 +9499,7 @@
         <v>322</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>405</v>
@@ -10019,7 +10019,7 @@
         <v>274</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -10137,7 +10137,7 @@
         <v>273</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D3">
         <v>-8</v>

</xml_diff>

<commit_message>
Add new investment methods. Fix group based investments and add the new methods there too. Add HiGHS parameter choices (presolve, method and parallel).
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05485BB-8A58-49E7-9C81-7E55AD0A5D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC54E0B-D651-4B61-9105-7A2E1F98F0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" activeTab="9" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="3" activeTab="4" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="476">
   <si>
     <t>commodity</t>
   </si>
@@ -762,9 +762,6 @@
     <t>Choice between minimum up- and downtimes (&lt;empty&gt;, min_downtime, min_uptime, both).</t>
   </si>
   <si>
-    <t>Choice of investment method (only_invest, only_retire, invest_and_retire, not_allowed).</t>
-  </si>
-  <si>
     <t>Can the unit provide this reserve. Empty indicates not allowed. Use 'yes' to indicate true.</t>
   </si>
   <si>
@@ -1179,9 +1176,6 @@
     <t>4solves</t>
   </si>
   <si>
-    <t>only_invest</t>
-  </si>
-  <si>
     <t>alternative_1</t>
   </si>
   <si>
@@ -1594,6 +1588,51 @@
   </si>
   <si>
     <t>Choice how the storage state will be maintained over discontinuos timelines. Default 'bind_within_timeblock' will bind the storage end state at the end of the timeblock to the beginning of the timeblock. 'bind_within_period', 'bind_within_solve' and bind_within_model' will act similarly but over increasingly longer time span. Meanwhile 'bind_forward_only' will bind forward over any holes in the used timeline, but will not bind end to the start. Separate parameters (e.g. 'storage_state_start') can force bindings.</t>
+  </si>
+  <si>
+    <t>invest_total</t>
+  </si>
+  <si>
+    <t>Choice of investment method: not_allowed, invest and retire indicate availability of investment and retirement. no_limit removes all limits even if there are limiting values set. period uses values set in invest/retire_max/min_period. total uses values set in invest/retire_max/min_total.</t>
+  </si>
+  <si>
+    <t>invest_period</t>
+  </si>
+  <si>
+    <t>17.0</t>
+  </si>
+  <si>
+    <t>Changed invest_method choices in node_c, connection_c and unit_c (removed only_invest, only_period and both, added invest_no_limit, invest_period, invest_total, invest_period_total, retire_no_limit, retire_period, retire_total, retire_period_total, invest_retire_no_limit, invest_retire_period, invest_retire_period, invest_retire_period_total)</t>
+  </si>
+  <si>
+    <t>18.0</t>
+  </si>
+  <si>
+    <t>Invest_method for group</t>
+  </si>
+  <si>
+    <t>highs_parallel</t>
+  </si>
+  <si>
+    <t>HiGHS uses presolve ('on') or not ('off'). Useful when solves are large.</t>
+  </si>
+  <si>
+    <t>highs_presolve</t>
+  </si>
+  <si>
+    <t>highs_method</t>
+  </si>
+  <si>
+    <t>HiGHS solver method ('simplex' or 'ipm' which is interior point method)</t>
+  </si>
+  <si>
+    <t>HiGHS parallelises single solves or not ('on' or 'off'). It can be better to turn HiGHS parallel off when executing multiple scnearios in parallel.</t>
+  </si>
+  <si>
+    <t>off</t>
+  </si>
+  <si>
+    <t>simplex</t>
   </si>
 </sst>
 </file>
@@ -2145,10 +2184,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>923925</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5573770" cy="1581459"/>
     <xdr:sp macro="" textlink="">
@@ -2164,7 +2203,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3743325" y="590550"/>
+          <a:off x="7734300" y="638175"/>
           <a:ext cx="5573770" cy="1581459"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3236,74 +3275,74 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>281</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>283</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>282</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>284</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="E4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="E6" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
@@ -3313,65 +3352,65 @@
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="E9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="C10" s="31" t="s">
         <v>218</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>220</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>221</v>
       </c>
       <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="C13" s="31" t="s">
         <v>224</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>242</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="C14" s="31" t="s">
         <v>243</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="31" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3383,26 +3422,26 @@
       <c r="A17" s="39"/>
       <c r="B17" s="39"/>
       <c r="C17" s="40" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B19" s="45"/>
       <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
@@ -3414,45 +3453,45 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="B22" s="34" t="s">
         <v>238</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>239</v>
       </c>
       <c r="C22" s="34"/>
       <c r="D22" s="28"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
@@ -3464,65 +3503,65 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="42"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B30" s="36"/>
       <c r="C30" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
@@ -3585,11 +3624,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3626,32 +3665,32 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D1" t="s">
         <v>182</v>
       </c>
       <c r="E1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F1" t="s">
         <v>183</v>
       </c>
       <c r="G1" t="s">
-        <v>185</v>
+        <v>462</v>
       </c>
       <c r="H1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="I1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="K1" t="s">
         <v>154</v>
@@ -3660,10 +3699,10 @@
         <v>170</v>
       </c>
       <c r="M1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="N1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="O1" t="s">
         <v>67</v>
@@ -3672,25 +3711,25 @@
         <v>70</v>
       </c>
       <c r="Q1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="R1" t="s">
         <v>71</v>
       </c>
       <c r="S1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="T1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="U1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="V1" t="s">
         <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="X1" t="s">
         <v>24</v>
@@ -3699,16 +3738,16 @@
         <v>72</v>
       </c>
       <c r="Z1" t="s">
+        <v>437</v>
+      </c>
+      <c r="AA1" s="5" t="s">
         <v>439</v>
       </c>
-      <c r="AA1" s="5" t="s">
-        <v>441</v>
-      </c>
       <c r="AB1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="AC1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="AD1" t="s">
         <v>73</v>
@@ -3722,28 +3761,28 @@
         <v>58</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>59</v>
@@ -3770,13 +3809,13 @@
         <v>14</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="U2" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="V2" s="9" t="s">
         <v>6</v>
@@ -3791,16 +3830,16 @@
         <v>64</v>
       </c>
       <c r="Z2" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="AA2" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="AA2" s="9" t="s">
-        <v>440</v>
-      </c>
       <c r="AB2" s="9" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="AD2" s="9" t="s">
         <v>65</v>
@@ -3820,7 +3859,7 @@
         <v>159</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
@@ -3847,7 +3886,7 @@
         <v>159</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
@@ -3906,10 +3945,10 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>159</v>
@@ -3924,13 +3963,13 @@
         <v>146</v>
       </c>
       <c r="H7" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="I7" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="J7" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="M7">
         <v>12000</v>
@@ -3953,10 +3992,10 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>159</v>
@@ -3976,13 +4015,13 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G9" t="s">
-        <v>324</v>
+        <v>461</v>
       </c>
       <c r="P9">
         <v>800</v>
@@ -4017,7 +4056,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4039,7 +4078,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4053,19 +4092,19 @@
         <v>69</v>
       </c>
       <c r="G1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H1" t="s">
+        <v>368</v>
+      </c>
+      <c r="I1" t="s">
+        <v>369</v>
+      </c>
+      <c r="J1" t="s">
+        <v>365</v>
+      </c>
+      <c r="K1" t="s">
         <v>370</v>
-      </c>
-      <c r="I1" t="s">
-        <v>371</v>
-      </c>
-      <c r="J1" t="s">
-        <v>367</v>
-      </c>
-      <c r="K1" t="s">
-        <v>372</v>
       </c>
       <c r="L1" t="s">
         <v>21</v>
@@ -4074,7 +4113,7 @@
         <v>24</v>
       </c>
       <c r="N1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4103,13 +4142,13 @@
         <v>13</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>6</v>
@@ -4159,7 +4198,7 @@
         <v>147</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D5">
         <f>250*8760*1.1</f>
@@ -4195,7 +4234,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4528,14 +4567,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
         <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4606,12 +4645,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4664,7 +4703,7 @@
         <v>161</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -4740,7 +4779,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4770,13 +4809,13 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F1" t="s">
         <v>179</v>
@@ -4785,7 +4824,7 @@
         <v>180</v>
       </c>
       <c r="H1" t="s">
-        <v>185</v>
+        <v>462</v>
       </c>
       <c r="I1" t="s">
         <v>181</v>
@@ -4800,19 +4839,19 @@
         <v>23</v>
       </c>
       <c r="M1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N1" t="s">
         <v>26</v>
       </c>
       <c r="O1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="Q1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="R1" t="s">
         <v>21</v>
@@ -4821,16 +4860,16 @@
         <v>24</v>
       </c>
       <c r="T1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="U1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="V1" t="s">
         <v>19</v>
       </c>
       <c r="W1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -4841,13 +4880,13 @@
         <v>27</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>281</v>
-      </c>
       <c r="E2" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -4859,7 +4898,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -4877,13 +4916,13 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>6</v>
@@ -4938,16 +4977,16 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E4" t="s">
         <v>159</v>
@@ -4970,7 +5009,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
@@ -4982,7 +5021,7 @@
         <v>148</v>
       </c>
       <c r="H5" t="s">
-        <v>324</v>
+        <v>461</v>
       </c>
       <c r="L5">
         <v>100</v>
@@ -5002,19 +5041,19 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H6" t="s">
-        <v>324</v>
+        <v>461</v>
       </c>
       <c r="L6">
         <v>100</v>
@@ -5070,7 +5109,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5078,19 +5117,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="I1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -5099,7 +5138,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -5122,13 +5161,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -5176,7 +5215,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -5211,7 +5250,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5451,7 +5490,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="G1" sqref="G1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5483,14 +5522,14 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E1" t="s">
         <v>180</v>
@@ -5499,7 +5538,7 @@
         <v>184</v>
       </c>
       <c r="G1" t="s">
-        <v>185</v>
+        <v>462</v>
       </c>
       <c r="H1" t="s">
         <v>20</v>
@@ -5508,19 +5547,19 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K1" t="s">
         <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="O1" t="s">
         <v>21</v>
@@ -5529,7 +5568,7 @@
         <v>24</v>
       </c>
       <c r="Q1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="R1" t="s">
         <v>171</v>
@@ -5538,19 +5577,19 @@
         <v>110</v>
       </c>
       <c r="T1" t="s">
+        <v>312</v>
+      </c>
+      <c r="U1" t="s">
         <v>313</v>
       </c>
-      <c r="U1" t="s">
-        <v>314</v>
-      </c>
       <c r="V1" t="s">
+        <v>197</v>
+      </c>
+      <c r="W1" t="s">
         <v>198</v>
       </c>
-      <c r="W1" t="s">
-        <v>199</v>
-      </c>
       <c r="X1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5561,7 +5600,7 @@
         <v>124</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>109</v>
@@ -5588,13 +5627,13 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O2" s="24" t="s">
         <v>6</v>
@@ -5638,7 +5677,7 @@
         <v>159</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E3" s="47" t="s">
         <v>173</v>
@@ -5678,7 +5717,7 @@
         <v>159</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E4" s="47" t="s">
         <v>173</v>
@@ -5705,10 +5744,10 @@
         <v>159</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
@@ -5726,27 +5765,27 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>150</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>324</v>
+        <v>463</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C7" s="47" t="s">
         <v>159</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E7" s="47" t="s">
         <v>173</v>
@@ -5771,10 +5810,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5786,441 +5825,469 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C3" t="s">
         <v>191</v>
       </c>
-      <c r="C3" t="s">
-        <v>192</v>
-      </c>
       <c r="D3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B6" s="25">
         <v>44600</v>
       </c>
       <c r="C6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B7" s="25">
         <v>44602</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
       </c>
       <c r="C8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
       </c>
       <c r="C9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B10" s="25">
         <v>44602</v>
       </c>
       <c r="C10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
       </c>
       <c r="C11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
       </c>
       <c r="C12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
       </c>
       <c r="C13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
       </c>
       <c r="C14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
       </c>
       <c r="C15" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
       </c>
       <c r="C16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
       </c>
       <c r="C17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
       </c>
       <c r="C18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
       </c>
       <c r="C19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D19" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
       </c>
       <c r="C20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D20" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
       </c>
       <c r="C21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D21" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
       </c>
       <c r="C22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D22" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
       </c>
       <c r="C23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D23" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
       </c>
       <c r="C24" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D24" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
       </c>
       <c r="C25" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D25" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
       </c>
       <c r="C26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D26" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B27" s="25">
         <v>44701</v>
       </c>
       <c r="C27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D27" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B28" s="25">
         <v>44712</v>
       </c>
       <c r="C28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D28" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B29" s="25">
         <v>44727</v>
       </c>
       <c r="C29" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D29" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B30" s="25">
         <v>44734</v>
       </c>
       <c r="C30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D30" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B31" s="25">
         <v>44741</v>
       </c>
       <c r="C31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D31" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B32" s="25">
         <v>44840</v>
       </c>
       <c r="C32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D32" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B33" s="25">
         <v>44850</v>
       </c>
       <c r="C33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D33" t="s">
-        <v>459</v>
+        <v>457</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="B34" s="25">
+        <v>44875</v>
+      </c>
+      <c r="C34" t="s">
+        <v>192</v>
+      </c>
+      <c r="D34" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="B35" s="25">
+        <v>44876</v>
+      </c>
+      <c r="C35" t="s">
+        <v>192</v>
+      </c>
+      <c r="D35" t="s">
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -6259,7 +6326,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6267,19 +6334,19 @@
         <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="J1" t="s">
         <v>21</v>
@@ -6288,7 +6355,7 @@
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M1" t="s">
         <v>171</v>
@@ -6314,13 +6381,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -6371,7 +6438,7 @@
         <v>150</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D5">
         <v>75</v>
@@ -6406,7 +6473,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6670,7 +6737,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6679,19 +6746,19 @@
         <v>142</v>
       </c>
       <c r="F1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I1" t="s">
         <v>119</v>
       </c>
       <c r="J1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="K1" t="s">
         <v>121</v>
@@ -6700,7 +6767,7 @@
         <v>123</v>
       </c>
       <c r="M1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -6717,7 +6784,7 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>141</v>
@@ -6726,7 +6793,7 @@
         <v>18</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>112</v>
@@ -6744,7 +6811,7 @@
         <v>122</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -6761,7 +6828,7 @@
         <v>149</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6784,7 +6851,7 @@
         <v>147</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6804,7 +6871,7 @@
         <v>160</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -6821,7 +6888,7 @@
         <v>148</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6841,7 +6908,7 @@
         <v>147</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -6852,16 +6919,16 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>160</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -6869,16 +6936,16 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -6886,16 +6953,16 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -6930,7 +6997,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6971,10 +7038,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7214,7 +7281,7 @@
         <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7228,13 +7295,13 @@
         <v>145</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7673,12 +7740,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7706,10 +7773,10 @@
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>274</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>275</v>
       </c>
       <c r="D3" t="s">
         <v>176</v>
@@ -7745,12 +7812,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7781,7 +7848,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D3" t="s">
         <v>176</v>
@@ -7818,13 +7885,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -7872,16 +7939,16 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E4" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -7894,13 +7961,13 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7918,21 +7985,22 @@
     <col min="11" max="11" width="22" customWidth="1"/>
     <col min="12" max="12" width="24.140625" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" customWidth="1"/>
-    <col min="16" max="17" width="20.85546875" customWidth="1"/>
-    <col min="18" max="19" width="16.7109375" customWidth="1"/>
-    <col min="20" max="20" width="16.42578125" customWidth="1"/>
-    <col min="21" max="25" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="15.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="18" width="20.85546875" customWidth="1"/>
+    <col min="19" max="20" width="16.7109375" customWidth="1"/>
+    <col min="21" max="21" width="16.42578125" customWidth="1"/>
+    <col min="22" max="26" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D1" t="s">
         <v>41</v>
@@ -7941,7 +8009,7 @@
         <v>37</v>
       </c>
       <c r="F1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="G1" t="s">
         <v>43</v>
@@ -7950,7 +8018,7 @@
         <v>47</v>
       </c>
       <c r="I1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J1" t="s">
         <v>45</v>
@@ -7959,31 +8027,34 @@
         <v>55</v>
       </c>
       <c r="L1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="M1" t="s">
         <v>39</v>
       </c>
       <c r="N1" t="s">
+        <v>462</v>
+      </c>
+      <c r="O1" t="s">
         <v>49</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>53</v>
       </c>
-      <c r="P1" t="s">
-        <v>345</v>
-      </c>
       <c r="Q1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="R1" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="S1" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="T1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -7991,7 +8062,7 @@
         <v>57</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>40</v>
@@ -8000,7 +8071,7 @@
         <v>36</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>42</v>
@@ -8018,31 +8089,34 @@
         <v>54</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="P2" s="9" t="s">
-        <v>343</v>
-      </c>
       <c r="Q2" s="9" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>360</v>
+        <v>342</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -8052,13 +8126,14 @@
       <c r="E3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N3" s="47"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H4">
         <v>200</v>
@@ -8073,12 +8148,12 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="G5" t="s">
         <v>159</v>
@@ -8087,26 +8162,26 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="P6">
+        <v>346</v>
+      </c>
+      <c r="Q6">
         <v>40</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C7" t="s">
         <v>159</v>
@@ -8148,7 +8223,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8171,16 +8246,16 @@
         <v>51</v>
       </c>
       <c r="J1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="K1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="M1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -8212,16 +8287,16 @@
         <v>50</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -8260,7 +8335,7 @@
         <v>153</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -8293,10 +8368,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8305,42 +8380,42 @@
         <v>29</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>322</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>322</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>389</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>29</v>
@@ -8381,91 +8456,91 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="F4" t="s">
         <v>321</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>323</v>
-      </c>
-      <c r="F4" t="s">
-        <v>322</v>
-      </c>
       <c r="G4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="I4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="M4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="K5" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -8608,7 +8683,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>147</v>
@@ -8616,7 +8691,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>147</v>
@@ -8624,7 +8699,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>148</v>
@@ -8712,7 +8787,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>150</v>
@@ -8723,7 +8798,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>162</v>
@@ -8766,14 +8841,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G1" t="s">
         <v>129</v>
@@ -8811,7 +8886,7 @@
         <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>128</v>
@@ -8834,13 +8909,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>32</v>
@@ -8892,22 +8967,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F1" t="s">
         <v>137</v>
       </c>
       <c r="G1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -8950,19 +9025,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" t="s">
         <v>286</v>
-      </c>
-      <c r="E3" t="s">
-        <v>287</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -9003,7 +9078,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -9195,14 +9270,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G1" t="s">
         <v>129</v>
@@ -9240,7 +9315,7 @@
         <v>58</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>128</v>
@@ -9263,13 +9338,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>150</v>
@@ -9289,13 +9364,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>151</v>
@@ -9315,13 +9390,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>150</v>
@@ -9341,13 +9416,13 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>162</v>
@@ -9367,13 +9442,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>150</v>
@@ -9420,12 +9495,12 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E1" t="s">
         <v>157</v>
@@ -9448,7 +9523,7 @@
         <v>155</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>156</v>
@@ -9479,13 +9554,13 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>404</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D4" t="s">
         <v>159</v>
@@ -9496,13 +9571,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D5" t="s">
         <v>159</v>
@@ -9544,7 +9619,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -9572,16 +9647,16 @@
         <v>33</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>158</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>205</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -9629,7 +9704,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>34</v>
@@ -9649,7 +9724,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -9669,7 +9744,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>163</v>
@@ -9689,7 +9764,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>35</v>
@@ -9709,13 +9784,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D9" t="s">
         <v>167</v>
@@ -9729,10 +9804,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>79</v>
@@ -9785,14 +9860,14 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" s="3"/>
       <c r="E1"/>
       <c r="F1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -9806,13 +9881,13 @@
         <v>58</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>143</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9826,7 +9901,7 @@
         <v>149</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>177</v>
@@ -9846,7 +9921,7 @@
         <v>147</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>177</v>
@@ -9857,19 +9932,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>160</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -9877,19 +9952,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -9926,13 +10001,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -9949,7 +10024,7 @@
         <v>143</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -9983,15 +10058,15 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10005,21 +10080,21 @@
         <v>143</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -10055,12 +10130,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10074,7 +10149,7 @@
         <v>143</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -10107,12 +10182,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10126,18 +10201,18 @@
         <v>143</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D3">
         <v>-8</v>
@@ -10153,9 +10228,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640D032-37A5-47CC-8407-C4F7168BB93B}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -10167,24 +10242,35 @@
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" customWidth="1"/>
-    <col min="6" max="15" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="15" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D1" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+      <c r="E1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F1" t="s">
+        <v>472</v>
+      </c>
+      <c r="G1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -10195,10 +10281,19 @@
         <v>168</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -10209,13 +10304,21 @@
         <v>80</v>
       </c>
       <c r="D3" t="s">
-        <v>392</v>
-      </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+      <c r="E3" t="s">
+        <v>474</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G3" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>34</v>
@@ -10224,12 +10327,21 @@
         <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+      <c r="E4" t="s">
+        <v>474</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>163</v>
@@ -10238,12 +10350,21 @@
         <v>169</v>
       </c>
       <c r="D5" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+      <c r="E5" t="s">
+        <v>474</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G5" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>35</v>
@@ -10252,65 +10373,119 @@
         <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+      <c r="E6" t="s">
+        <v>474</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G6" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7" t="s">
         <v>169</v>
       </c>
       <c r="D7" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>390</v>
+      </c>
+      <c r="E7" t="s">
+        <v>474</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G7" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+      <c r="E8" t="s">
+        <v>474</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G8" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>163</v>
       </c>
       <c r="D9" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+      <c r="E9" t="s">
+        <v>474</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G9" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>398</v>
+      </c>
+      <c r="E10" t="s">
+        <v>474</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G10" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D11" t="s">
-        <v>400</v>
+        <v>398</v>
+      </c>
+      <c r="E11" t="s">
+        <v>474</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="G11" t="s">
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -10344,7 +10519,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -10357,13 +10532,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>82</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10425,12 +10600,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10441,10 +10616,10 @@
         <v>105</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10816,7 +10991,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -10873,7 +11048,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Added a check for storage nodes (they must use has_balance as well). Updates gas_export case in Excel input
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC54E0B-D651-4B61-9105-7A2E1F98F0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164F0560-B68C-4EEA-9DA0-7D15BBBA3C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="3" activeTab="4" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="3" activeTab="9" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="476">
   <si>
     <t>commodity</t>
   </si>
@@ -3624,11 +3624,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4000,9 +4000,18 @@
       <c r="C8" s="14" t="s">
         <v>159</v>
       </c>
+      <c r="D8" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" t="s">
+        <v>159</v>
+      </c>
       <c r="G8" t="s">
         <v>146</v>
       </c>
+      <c r="I8" t="s">
+        <v>447</v>
+      </c>
       <c r="M8">
         <v>12000</v>
       </c>
@@ -4010,7 +4019,10 @@
         <v>12000</v>
       </c>
       <c r="O8">
-        <v>1000</v>
+        <v>10000000</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
@@ -10230,7 +10242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640D032-37A5-47CC-8407-C4F7168BB93B}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>

<commit_message>
Add bind_between_periods as a working option. Change some outputs (remove '_d' from the parameter names)
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164F0560-B68C-4EEA-9DA0-7D15BBBA3C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0359BA10-CA20-4745-9612-FA620450DE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="3" activeTab="9" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="2" activeTab="2" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="477">
   <si>
     <t>commodity</t>
   </si>
@@ -1633,6 +1633,9 @@
   </si>
   <si>
     <t>simplex</t>
+  </si>
+  <si>
+    <t>bind_forward_only</t>
   </si>
 </sst>
 </file>
@@ -3624,11 +3627,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4008,6 +4011,9 @@
       </c>
       <c r="G8" t="s">
         <v>146</v>
+      </c>
+      <c r="H8" t="s">
+        <v>476</v>
       </c>
       <c r="I8" t="s">
         <v>447</v>
@@ -8365,11 +8371,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6AC2C8-7B82-4BFA-94A3-ECFAF63F0D5D}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8499,7 +8505,7 @@
         <v>385</v>
       </c>
       <c r="L4" t="s">
-        <v>397</v>
+        <v>322</v>
       </c>
       <c r="M4" t="s">
         <v>400</v>
@@ -8518,6 +8524,9 @@
       </c>
       <c r="K5" t="s">
         <v>387</v>
+      </c>
+      <c r="L5" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -10430,15 +10439,7 @@
       <c r="D8" t="s">
         <v>398</v>
       </c>
-      <c r="E8" t="s">
-        <v>474</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="G8" t="s">
-        <v>474</v>
-      </c>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -10450,15 +10451,7 @@
       <c r="D9" t="s">
         <v>398</v>
       </c>
-      <c r="E9" t="s">
-        <v>474</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="G9" t="s">
-        <v>474</v>
-      </c>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -10470,15 +10463,7 @@
       <c r="D10" t="s">
         <v>398</v>
       </c>
-      <c r="E10" t="s">
-        <v>474</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="G10" t="s">
-        <v>474</v>
-      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -10490,15 +10475,7 @@
       <c r="D11" t="s">
         <v>398</v>
       </c>
-      <c r="E11" t="s">
-        <v>474</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="G11" t="s">
-        <v>474</v>
-      </c>
+      <c r="F11" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Add period based 'other_operational_cost' for connections. User has to be careful - index name needs to be period or time.
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4A53AB-C756-4A17-8D67-AA481D8A182D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B965210E-F230-4C72-89D2-1986E387FE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="1" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="1" activeTab="15" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -121,7 +121,7 @@
           </rPr>
           <t xml:space="preserve">Possible parameters
 efficiency: [factor] Efficiency of a unit. Constant or time.
-other_operational_cost: [CUR/MWh] Other variable operational cost. Fuel and CO2 cost can be given through separate means. Constant or time.
+other_operational_cost: [CUR/MWh] Other variable operational cost. Fuel and CO2 cost can be given through separate means. Constant, period or time.
 </t>
         </r>
       </text>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="479">
   <si>
     <t>commodity</t>
   </si>
@@ -1638,10 +1638,10 @@
     <t>[CUR/MWh] Other operational cost for energy flows. Constant or time.</t>
   </si>
   <si>
-    <t>[CUR/MWh] Other variable operational cost for transferring over the connection. Constant or time.</t>
-  </si>
-  <si>
     <t>Change variable_cost to other_operational_cost in connection_c, connection_t, unit_node_c, and unit_node_t</t>
+  </si>
+  <si>
+    <t>[CUR/MWh] Other variable operational cost for transferring over the connection. Constant, period or time.</t>
   </si>
 </sst>
 </file>
@@ -4799,7 +4799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44D2B2-1DE7-400D-8C40-2CD59BEE6EC3}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -4887,7 +4887,7 @@
         <v>374</v>
       </c>
       <c r="U1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="V1" t="s">
         <v>18</v>
@@ -5106,7 +5106,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C5CDA4-FFE3-4938-9213-CC2F8772241C}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -5129,9 +5129,10 @@
     <col min="10" max="10" width="12.5703125" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>247</v>
       </c>
@@ -5164,8 +5165,11 @@
       <c r="L1" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -5202,8 +5206,11 @@
       <c r="L2" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="9" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -5217,7 +5224,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -5231,7 +5238,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -5836,7 +5843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6323,7 +6330,7 @@
         <v>191</v>
       </c>
       <c r="D36" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add possibility to scale inflow time series according both annual_flow and peak_inflow parameters (note that peak_inflow needs to have the same sign as the peak in the original time series. annual_flow is signless - always positive).
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B965210E-F230-4C72-89D2-1986E387FE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7206BFBB-42CC-4A22-96D8-B7B8892C3E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="1" activeTab="15" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="30360" yWindow="0" windowWidth="21240" windowHeight="21000" tabRatio="1000" firstSheet="1" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="483">
   <si>
     <t>commodity</t>
   </si>
@@ -666,9 +666,6 @@
     <t>Commodity_nodes</t>
   </si>
   <si>
-    <t>[MWh] Annual flow in energy units (always positive, the sign of inflow defines in/out). Inflow time series is scaled to match annual flow. Default value is calculated from the absolute of inflow time series. Constant or period.</t>
-  </si>
-  <si>
     <t>sense</t>
   </si>
   <si>
@@ -1425,12 +1422,6 @@
     <t>Gas_export_profile</t>
   </si>
   <si>
-    <t>scale_to_annual_flow</t>
-  </si>
-  <si>
-    <t>Choice how to treat inflow time series. Empty defaults to 'use_original', which does not scale the time series. 'no_inflow' ignores the inflow time series. 'scale_to_annual_flow' will scale the time series to match the 'annual_flow' so that the sum of inflow is multiplied by 8760/'hours_in_solve'. 'scale_in_proprotion' calculates a scaling factor by dividing 'annual_flow' with the sum of time series inflow (after it has been annualized using 'timeline_duration_in_years').</t>
-  </si>
-  <si>
     <t>max_relative_capacity</t>
   </si>
   <si>
@@ -1642,6 +1633,27 @@
   </si>
   <si>
     <t>[CUR/MWh] Other variable operational cost for transferring over the connection. Constant, period or time.</t>
+  </si>
+  <si>
+    <t>[MWh] Annual flow in energy units (always positive, the sign of inflow defines in/out). Inflow time series can be scaled to match annual flow. By default, there is no scaling of inflow. Constant or period.</t>
+  </si>
+  <si>
+    <t>[MWh] Highest absolute flow in scaled inflow. Used only with inflow_method scale_to_annual_and_peak_flow. Constant or period.</t>
+  </si>
+  <si>
+    <t>Choice how to treat inflow time series. Empty defaults to 'use_original', which does not scale the time series. 'no_inflow' ignores the inflow time series. 'scale_to_annual_flow' will scale the time series to match the 'annual_flow' so that the sum of inflow is multiplied by 8760/'hours_in_solve'. 'scale_in_proprotion' calculates a scaling factor by dividing 'annual_flow' with the sum of time series inflow (after it has been annualized using 'timeline_duration_in_years'). 'scale_to_annual_and_peak_flow' scales the inflow to match both the annual flow and the peak flow parameters (be careful, can lead to negative numbers).</t>
+  </si>
+  <si>
+    <t>scale_to_annual_and_peak_flow</t>
+  </si>
+  <si>
+    <t>peak_inflow</t>
+  </si>
+  <si>
+    <t>19.1</t>
+  </si>
+  <si>
+    <t>Add scale_to_annual_and_peak_flow to inflow methods as well as peak_inflow parameter to node_c and node_d</t>
   </si>
 </sst>
 </file>
@@ -2655,7 +2667,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -3284,74 +3296,74 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>281</v>
+      </c>
+      <c r="C1" s="46" t="s">
         <v>280</v>
-      </c>
-      <c r="B1" s="46" t="s">
-        <v>282</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="E4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="E6" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
@@ -3361,65 +3373,65 @@
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="E9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="B10" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="C10" s="31" t="s">
         <v>216</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>218</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>219</v>
       </c>
       <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
+        <v>220</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="C13" s="31" t="s">
         <v>222</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
+        <v>239</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>240</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="C14" s="31" t="s">
         <v>241</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3431,26 +3443,26 @@
       <c r="A17" s="39"/>
       <c r="B17" s="39"/>
       <c r="C17" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B19" s="45"/>
       <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
@@ -3462,45 +3474,45 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" s="34" t="s">
         <v>236</v>
-      </c>
-      <c r="B22" s="34" t="s">
-        <v>237</v>
       </c>
       <c r="C22" s="34"/>
       <c r="D22" s="28"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
@@ -3512,65 +3524,65 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="42"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B30" s="36"/>
       <c r="C30" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
@@ -3631,7 +3643,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
-  <dimension ref="A1:AD9"/>
+  <dimension ref="A1:AE9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
@@ -3652,117 +3664,121 @@
     <col min="8" max="8" width="23.140625" customWidth="1"/>
     <col min="9" max="9" width="25.140625" customWidth="1"/>
     <col min="10" max="10" width="29.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" customWidth="1"/>
-    <col min="17" max="17" width="10.28515625" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" style="14" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" style="14" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" style="14" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" style="14" customWidth="1"/>
-    <col min="23" max="23" width="10.5703125" customWidth="1"/>
-    <col min="24" max="24" width="8.140625" customWidth="1"/>
-    <col min="25" max="26" width="18.140625" customWidth="1"/>
-    <col min="27" max="27" width="16.85546875" customWidth="1"/>
-    <col min="28" max="29" width="29.140625" customWidth="1"/>
-    <col min="30" max="30" width="14.7109375" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" style="14" customWidth="1"/>
+    <col min="20" max="20" width="9.85546875" style="14" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" style="14" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" customWidth="1"/>
+    <col min="23" max="23" width="12.7109375" style="14" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" customWidth="1"/>
+    <col min="25" max="25" width="8.140625" customWidth="1"/>
+    <col min="26" max="27" width="18.140625" customWidth="1"/>
+    <col min="28" max="28" width="16.85546875" customWidth="1"/>
+    <col min="29" max="30" width="29.140625" customWidth="1"/>
+    <col min="31" max="31" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="E1" t="s">
-        <v>407</v>
-      </c>
-      <c r="F1" t="s">
-        <v>182</v>
-      </c>
       <c r="G1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="H1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="I1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="K1" t="s">
+        <v>168</v>
+      </c>
+      <c r="L1" t="s">
+        <v>476</v>
+      </c>
+      <c r="M1" t="s">
+        <v>477</v>
+      </c>
+      <c r="N1" t="s">
+        <v>361</v>
+      </c>
+      <c r="O1" t="s">
+        <v>362</v>
+      </c>
+      <c r="P1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>69</v>
+      </c>
+      <c r="R1" t="s">
+        <v>296</v>
+      </c>
+      <c r="S1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" t="s">
+        <v>297</v>
+      </c>
+      <c r="U1" t="s">
+        <v>363</v>
+      </c>
+      <c r="V1" t="s">
+        <v>364</v>
+      </c>
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" t="s">
+        <v>365</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>431</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>434</v>
+      </c>
+      <c r="AD1" t="s">
         <v>440</v>
       </c>
-      <c r="K1" t="s">
-        <v>153</v>
-      </c>
-      <c r="L1" t="s">
-        <v>169</v>
-      </c>
-      <c r="M1" t="s">
-        <v>362</v>
-      </c>
-      <c r="N1" t="s">
-        <v>363</v>
-      </c>
-      <c r="O1" t="s">
-        <v>66</v>
-      </c>
-      <c r="P1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>297</v>
-      </c>
-      <c r="R1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S1" t="s">
-        <v>298</v>
-      </c>
-      <c r="T1" t="s">
-        <v>364</v>
-      </c>
-      <c r="U1" t="s">
-        <v>365</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>366</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>434</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>437</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>443</v>
-      </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3770,91 +3786,94 @@
         <v>57</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>59</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="W2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="AB2" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="AC2" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="AD2" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="U2" s="24" t="s">
-        <v>251</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="Z2" s="9" t="s">
-        <v>433</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>435</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>441</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>442</v>
-      </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AE2" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -3862,26 +3881,26 @@
         <v>146</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>406</v>
+        <v>479</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
         <v>145</v>
       </c>
-      <c r="M3">
-        <v>10000</v>
-      </c>
       <c r="N3">
         <v>10000</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -3889,30 +3908,30 @@
         <v>147</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
         <v>145</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <f>100*8760</f>
         <v>876000</v>
       </c>
-      <c r="M4">
-        <v>10000</v>
-      </c>
       <c r="N4">
         <v>10000</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -3920,146 +3939,146 @@
         <v>148</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G5" t="s">
         <v>145</v>
       </c>
-      <c r="M5">
-        <v>10000</v>
-      </c>
       <c r="N5">
         <v>10000</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G6" t="s">
         <v>145</v>
       </c>
-      <c r="M6">
-        <v>10000</v>
-      </c>
       <c r="N6">
         <v>10000</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G7" t="s">
         <v>145</v>
       </c>
       <c r="H7" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="I7" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="J7" t="s">
-        <v>445</v>
-      </c>
-      <c r="M7">
-        <v>12000</v>
+        <v>442</v>
       </c>
       <c r="N7">
         <v>12000</v>
       </c>
       <c r="O7">
+        <v>12000</v>
+      </c>
+      <c r="P7">
         <v>20</v>
       </c>
-      <c r="Y7">
+      <c r="Z7">
         <v>0.01</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <v>0.1</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G8" t="s">
         <v>145</v>
       </c>
       <c r="H8" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="I8" t="s">
-        <v>444</v>
-      </c>
-      <c r="M8">
-        <v>12000</v>
+        <v>441</v>
       </c>
       <c r="N8">
         <v>12000</v>
       </c>
       <c r="O8">
+        <v>12000</v>
+      </c>
+      <c r="P8">
         <v>10000000</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G9" t="s">
-        <v>458</v>
-      </c>
-      <c r="P9">
+        <v>455</v>
+      </c>
+      <c r="Q9">
         <v>800</v>
       </c>
-      <c r="T9" s="14">
+      <c r="U9" s="14">
         <v>200</v>
       </c>
-      <c r="V9" s="14">
+      <c r="W9" s="14">
         <v>0.05</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>10</v>
       </c>
-      <c r="AD9">
+      <c r="AE9">
         <v>1</v>
       </c>
     </row>
@@ -4074,13 +4093,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51F2ED7-E82A-4D3D-A4CE-E6A52C2211BA}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4088,21 +4107,21 @@
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4110,37 +4129,40 @@
         <v>65</v>
       </c>
       <c r="E1" t="s">
+        <v>477</v>
+      </c>
+      <c r="F1" t="s">
         <v>67</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>68</v>
       </c>
-      <c r="G1" t="s">
-        <v>305</v>
-      </c>
       <c r="H1" t="s">
+        <v>304</v>
+      </c>
+      <c r="I1" t="s">
+        <v>366</v>
+      </c>
+      <c r="J1" t="s">
         <v>367</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>363</v>
+      </c>
+      <c r="L1" t="s">
         <v>368</v>
       </c>
-      <c r="J1" t="s">
-        <v>364</v>
-      </c>
-      <c r="K1" t="s">
-        <v>369</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>23</v>
       </c>
-      <c r="N1" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -4154,37 +4176,40 @@
         <v>58</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="9" t="s">
-        <v>303</v>
-      </c>
       <c r="J2" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="24" t="s">
-        <v>251</v>
-      </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -4198,8 +4223,11 @@
         <f>250*8760*0.9</f>
         <v>1971000</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>-600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -4213,8 +4241,11 @@
         <f>250*8760*1</f>
         <v>2190000</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>-650</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -4222,11 +4253,14 @@
         <v>146</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5">
         <f>250*8760*1.1</f>
         <v>2409000</v>
+      </c>
+      <c r="E5">
+        <v>-700</v>
       </c>
     </row>
   </sheetData>
@@ -4258,7 +4292,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4273,7 +4307,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>60</v>
@@ -4591,14 +4625,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
         <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4634,7 +4668,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C4">
         <v>0.2</v>
@@ -4669,12 +4703,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4696,7 +4730,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>77</v>
@@ -4710,7 +4744,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>78</v>
@@ -4724,10 +4758,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -4784,10 +4818,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -4799,7 +4833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44D2B2-1DE7-400D-8C40-2CD59BEE6EC3}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -4833,28 +4867,28 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1" t="s">
         <v>178</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>456</v>
+      </c>
+      <c r="I1" t="s">
         <v>179</v>
       </c>
-      <c r="H1" t="s">
-        <v>459</v>
-      </c>
-      <c r="I1" t="s">
-        <v>180</v>
-      </c>
       <c r="J1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K1" t="s">
         <v>19</v>
@@ -4863,19 +4897,19 @@
         <v>22</v>
       </c>
       <c r="M1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N1" t="s">
         <v>25</v>
       </c>
       <c r="O1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P1" t="s">
+        <v>371</v>
+      </c>
+      <c r="Q1" t="s">
         <v>372</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>373</v>
       </c>
       <c r="R1" t="s">
         <v>20</v>
@@ -4884,16 +4918,16 @@
         <v>23</v>
       </c>
       <c r="T1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="U1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="V1" t="s">
         <v>18</v>
       </c>
       <c r="W1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -4904,13 +4938,13 @@
         <v>26</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>279</v>
-      </c>
       <c r="E2" s="24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -4922,7 +4956,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -4940,13 +4974,13 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>6</v>
@@ -4958,7 +4992,7 @@
         <v>5</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="V2" s="9" t="s">
         <v>3</v>
@@ -4981,19 +5015,19 @@
         <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F3" t="s">
+        <v>170</v>
+      </c>
+      <c r="G3" t="s">
         <v>171</v>
-      </c>
-      <c r="G3" t="s">
-        <v>172</v>
       </c>
       <c r="H3" t="s">
         <v>145</v>
       </c>
       <c r="I3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K3">
         <v>100</v>
@@ -5001,25 +5035,25 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G4" t="s">
         <v>171</v>
-      </c>
-      <c r="G4" t="s">
-        <v>172</v>
       </c>
       <c r="H4" t="s">
         <v>145</v>
@@ -5033,7 +5067,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>31</v>
@@ -5045,7 +5079,7 @@
         <v>147</v>
       </c>
       <c r="H5" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L5">
         <v>100</v>
@@ -5065,19 +5099,19 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H6" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="L6">
         <v>100</v>
@@ -5134,7 +5168,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5142,19 +5176,19 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F1" t="s">
         <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I1" t="s">
         <v>372</v>
-      </c>
-      <c r="I1" t="s">
-        <v>373</v>
       </c>
       <c r="J1" t="s">
         <v>20</v>
@@ -5163,10 +5197,10 @@
         <v>23</v>
       </c>
       <c r="L1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="M1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -5189,13 +5223,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -5207,7 +5241,7 @@
         <v>5</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -5246,7 +5280,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -5281,7 +5315,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5293,7 +5327,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -5553,23 +5587,23 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="H1" t="s">
         <v>19</v>
@@ -5578,19 +5612,19 @@
         <v>22</v>
       </c>
       <c r="J1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K1" t="s">
         <v>25</v>
       </c>
       <c r="L1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M1" t="s">
+        <v>374</v>
+      </c>
+      <c r="N1" t="s">
         <v>375</v>
-      </c>
-      <c r="N1" t="s">
-        <v>376</v>
       </c>
       <c r="O1" t="s">
         <v>20</v>
@@ -5599,28 +5633,28 @@
         <v>23</v>
       </c>
       <c r="Q1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="R1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="S1" t="s">
         <v>109</v>
       </c>
       <c r="T1" t="s">
+        <v>310</v>
+      </c>
+      <c r="U1" t="s">
         <v>311</v>
       </c>
-      <c r="U1" t="s">
-        <v>312</v>
-      </c>
       <c r="V1" t="s">
+        <v>195</v>
+      </c>
+      <c r="W1" t="s">
         <v>196</v>
       </c>
-      <c r="W1" t="s">
-        <v>197</v>
-      </c>
       <c r="X1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5631,7 +5665,7 @@
         <v>123</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>108</v>
@@ -5658,13 +5692,13 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O2" s="24" t="s">
         <v>6</v>
@@ -5705,13 +5739,13 @@
         <v>149</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F3" s="47"/>
       <c r="G3" s="47" t="s">
@@ -5745,13 +5779,13 @@
         <v>150</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="47" t="s">
@@ -5769,16 +5803,16 @@
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
@@ -5796,30 +5830,30 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>149</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>398</v>
-      </c>
       <c r="C7" s="47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G7" s="47" t="s">
         <v>145</v>
@@ -5841,9 +5875,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5854,483 +5890,497 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B3" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" t="s">
         <v>189</v>
       </c>
-      <c r="C3" t="s">
-        <v>190</v>
-      </c>
       <c r="D3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6" s="25">
         <v>44600</v>
       </c>
       <c r="C6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B7" s="25">
         <v>44602</v>
       </c>
       <c r="C7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
       </c>
       <c r="C8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B10" s="25">
         <v>44602</v>
       </c>
       <c r="C10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
       </c>
       <c r="C11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
       </c>
       <c r="C12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
       </c>
       <c r="C13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
       </c>
       <c r="C14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
       </c>
       <c r="C15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
       </c>
       <c r="C16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
       </c>
       <c r="C17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
       </c>
       <c r="C18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
       </c>
       <c r="C19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
       </c>
       <c r="C20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
       </c>
       <c r="C21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D21" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
       </c>
       <c r="C22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
       </c>
       <c r="C23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D23" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
       </c>
       <c r="C24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D24" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
       </c>
       <c r="C25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D25" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
       </c>
       <c r="C26" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D26" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B27" s="25">
         <v>44701</v>
       </c>
       <c r="C27" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D27" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B28" s="25">
         <v>44712</v>
       </c>
       <c r="C28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D28" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B29" s="25">
         <v>44727</v>
       </c>
       <c r="C29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D29" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B30" s="25">
         <v>44734</v>
       </c>
       <c r="C30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D30" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B31" s="25">
         <v>44741</v>
       </c>
       <c r="C31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D31" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B32" s="25">
         <v>44840</v>
       </c>
       <c r="C32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D32" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B33" s="25">
         <v>44850</v>
       </c>
       <c r="C33" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D33" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B34" s="25">
         <v>44875</v>
       </c>
       <c r="C34" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D34" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B35" s="25">
         <v>44876</v>
       </c>
       <c r="C35" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D35" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="B36" s="25">
         <v>44889</v>
       </c>
       <c r="C36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D36" t="s">
-        <v>477</v>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="B37" s="25">
+        <v>44893</v>
+      </c>
+      <c r="C37" t="s">
+        <v>190</v>
+      </c>
+      <c r="D37" t="s">
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -6369,7 +6419,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6377,19 +6427,19 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F1" t="s">
         <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I1" t="s">
         <v>375</v>
-      </c>
-      <c r="I1" t="s">
-        <v>376</v>
       </c>
       <c r="J1" t="s">
         <v>20</v>
@@ -6398,10 +6448,10 @@
         <v>23</v>
       </c>
       <c r="L1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="M1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6424,13 +6474,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -6481,7 +6531,7 @@
         <v>149</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5">
         <v>75</v>
@@ -6516,7 +6566,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6528,7 +6578,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -6542,7 +6592,7 @@
         <v>123</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -6780,7 +6830,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6789,19 +6839,19 @@
         <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="G1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I1" t="s">
         <v>118</v>
       </c>
       <c r="J1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="K1" t="s">
         <v>120</v>
@@ -6810,7 +6860,7 @@
         <v>122</v>
       </c>
       <c r="M1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -6827,16 +6877,16 @@
         <v>57</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>140</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>111</v>
@@ -6854,7 +6904,7 @@
         <v>121</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -6871,7 +6921,7 @@
         <v>148</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6894,7 +6944,7 @@
         <v>146</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6908,13 +6958,13 @@
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -6925,13 +6975,13 @@
         <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -6951,27 +7001,27 @@
         <v>146</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>398</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -6979,16 +7029,16 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>398</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -6996,16 +7046,16 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>398</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -7040,7 +7090,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -7052,10 +7102,10 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7064,7 +7114,7 @@
         <v>123</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -7073,7 +7123,7 @@
         <v>57</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7081,10 +7131,10 @@
         <v>27</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>337</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7324,7 +7374,7 @@
         <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7338,13 +7388,13 @@
         <v>144</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7783,12 +7833,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7802,7 +7852,7 @@
         <v>143</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -7816,13 +7866,13 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>273</v>
-      </c>
       <c r="D3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -7855,12 +7905,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7874,7 +7924,7 @@
         <v>143</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -7891,10 +7941,10 @@
         <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -7928,13 +7978,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -7951,7 +8001,7 @@
         <v>143</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -7974,7 +8024,7 @@
         <v>144</v>
       </c>
       <c r="E3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -7982,16 +8032,16 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C4" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>405</v>
-      </c>
       <c r="E4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -8039,11 +8089,11 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D1" t="s">
         <v>40</v>
@@ -8052,7 +8102,7 @@
         <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="G1" t="s">
         <v>42</v>
@@ -8061,7 +8111,7 @@
         <v>46</v>
       </c>
       <c r="I1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J1" t="s">
         <v>44</v>
@@ -8070,13 +8120,13 @@
         <v>54</v>
       </c>
       <c r="L1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="M1" t="s">
         <v>38</v>
       </c>
       <c r="N1" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="O1" t="s">
         <v>48</v>
@@ -8085,16 +8135,16 @@
         <v>52</v>
       </c>
       <c r="Q1" t="s">
+        <v>341</v>
+      </c>
+      <c r="R1" t="s">
         <v>342</v>
       </c>
-      <c r="R1" t="s">
-        <v>343</v>
-      </c>
       <c r="S1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="T1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
@@ -8105,7 +8155,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>39</v>
@@ -8114,7 +8164,7 @@
         <v>35</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>41</v>
@@ -8132,7 +8182,7 @@
         <v>53</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>37</v>
@@ -8147,16 +8197,16 @@
         <v>51</v>
       </c>
       <c r="Q2" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="R2" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="R2" s="9" t="s">
-        <v>341</v>
-      </c>
       <c r="S2" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="T2" s="9" t="s">
         <v>357</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -8176,7 +8226,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H4">
         <v>200</v>
@@ -8193,24 +8243,24 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="Q6">
         <v>40</v>
@@ -8224,10 +8274,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -8266,7 +8316,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8289,16 +8339,16 @@
         <v>50</v>
       </c>
       <c r="J1" t="s">
+        <v>341</v>
+      </c>
+      <c r="K1" t="s">
         <v>342</v>
       </c>
-      <c r="K1" t="s">
-        <v>343</v>
-      </c>
       <c r="L1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -8330,16 +8380,16 @@
         <v>49</v>
       </c>
       <c r="J2" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>341</v>
-      </c>
       <c r="L2" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>357</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -8378,7 +8428,7 @@
         <v>152</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -8411,10 +8461,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8423,42 +8473,42 @@
         <v>28</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>320</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>382</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>384</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>28</v>
@@ -8499,94 +8549,94 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="F4" t="s">
         <v>319</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>321</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>293</v>
+      </c>
+      <c r="H4" t="s">
+        <v>344</v>
+      </c>
+      <c r="I4" t="s">
+        <v>381</v>
+      </c>
+      <c r="J4" t="s">
+        <v>381</v>
+      </c>
+      <c r="K4" t="s">
+        <v>381</v>
+      </c>
+      <c r="L4" t="s">
         <v>320</v>
       </c>
-      <c r="G4" t="s">
-        <v>294</v>
-      </c>
-      <c r="H4" t="s">
-        <v>345</v>
-      </c>
-      <c r="I4" t="s">
-        <v>382</v>
-      </c>
-      <c r="J4" t="s">
-        <v>382</v>
-      </c>
-      <c r="K4" t="s">
-        <v>382</v>
-      </c>
-      <c r="L4" t="s">
-        <v>321</v>
-      </c>
       <c r="M4" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J5" t="s">
+        <v>382</v>
+      </c>
+      <c r="K5" t="s">
         <v>383</v>
       </c>
-      <c r="K5" t="s">
-        <v>384</v>
-      </c>
       <c r="L5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -8724,12 +8774,12 @@
         <v>152</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>146</v>
@@ -8737,7 +8787,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>146</v>
@@ -8745,7 +8795,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>147</v>
@@ -8833,7 +8883,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>149</v>
@@ -8844,10 +8894,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>147</v>
@@ -8887,14 +8937,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G1" t="s">
         <v>128</v>
@@ -8932,7 +8982,7 @@
         <v>57</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>127</v>
@@ -8955,13 +9005,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>31</v>
@@ -8970,7 +9020,7 @@
         <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -9013,22 +9063,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="F1" t="s">
         <v>136</v>
       </c>
       <c r="G1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -9071,19 +9121,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="E3" t="s">
         <v>284</v>
-      </c>
-      <c r="E3" t="s">
-        <v>285</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -9124,7 +9174,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -9153,7 +9203,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -9316,14 +9366,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G1" t="s">
         <v>128</v>
@@ -9361,7 +9411,7 @@
         <v>57</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>127</v>
@@ -9384,13 +9434,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>149</v>
@@ -9399,7 +9449,7 @@
         <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I3">
         <v>0.5</v>
@@ -9410,13 +9460,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>150</v>
@@ -9425,7 +9475,7 @@
         <v>146</v>
       </c>
       <c r="F4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -9436,13 +9486,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>149</v>
@@ -9451,7 +9501,7 @@
         <v>146</v>
       </c>
       <c r="F5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I5">
         <v>0.01</v>
@@ -9462,22 +9512,22 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>147</v>
       </c>
       <c r="F6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I6">
         <v>0.5</v>
@@ -9488,13 +9538,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>149</v>
@@ -9503,7 +9553,7 @@
         <v>146</v>
       </c>
       <c r="F7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I7">
         <v>0.01</v>
@@ -9541,15 +9591,15 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -9566,13 +9616,13 @@
         <v>142</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>154</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>155</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -9586,13 +9636,13 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>177</v>
-      </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -9600,16 +9650,16 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>400</v>
-      </c>
       <c r="D4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -9617,16 +9667,16 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9665,15 +9715,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" t="s">
         <v>163</v>
-      </c>
-      <c r="E1" t="s">
-        <v>164</v>
       </c>
       <c r="F1" t="s">
         <v>75</v>
@@ -9693,16 +9743,16 @@
         <v>32</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>203</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -9716,16 +9766,16 @@
         <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -9739,18 +9789,18 @@
         <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>33</v>
@@ -9759,18 +9809,18 @@
         <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>33</v>
@@ -9779,38 +9829,38 @@
         <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>34</v>
@@ -9819,53 +9869,53 @@
         <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E9">
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -9906,14 +9956,14 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" s="3"/>
       <c r="E1"/>
       <c r="F1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -9927,13 +9977,13 @@
         <v>57</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>142</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -9947,10 +9997,10 @@
         <v>148</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -9967,10 +10017,10 @@
         <v>146</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F4">
         <v>-0.1</v>
@@ -9978,19 +10028,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>398</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>338</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>399</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -9998,19 +10048,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>398</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -10047,13 +10097,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10070,7 +10120,7 @@
         <v>142</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -10104,15 +10154,15 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="E1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10126,21 +10176,21 @@
         <v>142</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -10176,12 +10226,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10195,7 +10245,7 @@
         <v>142</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -10228,12 +10278,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10247,18 +10297,18 @@
         <v>142</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D3">
         <v>-8</v>
@@ -10297,23 +10347,23 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E1" t="s">
+        <v>463</v>
+      </c>
+      <c r="F1" t="s">
         <v>466</v>
       </c>
-      <c r="F1" t="s">
-        <v>469</v>
-      </c>
       <c r="G1" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10324,19 +10374,19 @@
         <v>76</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -10350,21 +10400,21 @@
         <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E3" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="G3" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>33</v>
@@ -10373,44 +10423,44 @@
         <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E4" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="G4" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E5" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="G5" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -10419,86 +10469,86 @@
         <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E6" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="G6" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E7" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="G7" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D9" t="s">
         <v>394</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" t="s">
-        <v>395</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D11" t="s">
         <v>394</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D11" t="s">
-        <v>395</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -10533,7 +10583,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -10546,13 +10596,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>81</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10560,7 +10610,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -10574,7 +10624,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>29</v>
@@ -10614,12 +10664,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10630,10 +10680,10 @@
         <v>104</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -11005,7 +11055,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -11062,7 +11112,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>104</v>
@@ -11070,7 +11120,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>105</v>
@@ -11078,7 +11128,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Added CO2 method as well as CO2 limits and an example to init.sqlite
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7206BFBB-42CC-4A22-96D8-B7B8892C3E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8847FA-9772-4139-99DA-C95158972008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30360" yWindow="0" windowWidth="21240" windowHeight="21000" tabRatio="1000" firstSheet="1" activeTab="1" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="9" activeTab="27" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="491">
   <si>
     <t>commodity</t>
   </si>
@@ -1654,6 +1654,30 @@
   </si>
   <si>
     <t>Add scale_to_annual_and_peak_flow to inflow methods as well as peak_inflow parameter to node_c and node_d</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>Added CO2 method and limit parameters to ghe 'group_c' (and group_p)</t>
+  </si>
+  <si>
+    <t>[tCO2] Maximum limit for emitted CO2 in the whole solve.</t>
+  </si>
+  <si>
+    <t>co2_method</t>
+  </si>
+  <si>
+    <t>co2_max_total</t>
+  </si>
+  <si>
+    <t>[tCO2] Maximum limit for emitted CO2 in each period.</t>
+  </si>
+  <si>
+    <t>co2_max_period</t>
+  </si>
+  <si>
+    <t>Choice of the CO2 method: no_method, price, period, total, price_period, price_total, period_total, price_period_total</t>
   </si>
 </sst>
 </file>
@@ -5875,10 +5899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6381,6 +6405,20 @@
       </c>
       <c r="D37" t="s">
         <v>482</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="B38" s="25">
+        <v>44903</v>
+      </c>
+      <c r="C38" t="s">
+        <v>190</v>
+      </c>
+      <c r="D38" t="s">
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -8054,13 +8092,13 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8077,17 +8115,19 @@
     <col min="10" max="10" width="21" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
     <col min="12" max="12" width="24.140625" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1"/>
-    <col min="17" max="18" width="20.85546875" customWidth="1"/>
-    <col min="19" max="20" width="16.7109375" customWidth="1"/>
-    <col min="21" max="21" width="16.42578125" customWidth="1"/>
-    <col min="22" max="26" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" customWidth="1"/>
+    <col min="19" max="20" width="20.85546875" customWidth="1"/>
+    <col min="21" max="22" width="16.7109375" customWidth="1"/>
+    <col min="23" max="23" width="16.42578125" customWidth="1"/>
+    <col min="24" max="28" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>246</v>
       </c>
@@ -8123,31 +8163,37 @@
         <v>409</v>
       </c>
       <c r="M1" t="s">
+        <v>490</v>
+      </c>
+      <c r="N1" t="s">
         <v>38</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>485</v>
+      </c>
+      <c r="P1" t="s">
         <v>456</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>48</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>341</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>342</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>351</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -8185,31 +8231,37 @@
         <v>289</v>
       </c>
       <c r="M2" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="O2" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="P2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -8219,9 +8271,9 @@
       <c r="E3">
         <v>10</v>
       </c>
-      <c r="N3" s="47"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="P3" s="47"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -8241,7 +8293,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>318</v>
       </c>
@@ -8255,21 +8307,21 @@
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>344</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>40</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -8290,7 +8342,7 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA54FD9A-FB2F-4111-AC75-F20843B34F53}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
@@ -8308,13 +8360,14 @@
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
-    <col min="10" max="11" width="20.85546875" customWidth="1"/>
-    <col min="12" max="13" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="12" width="20.85546875" customWidth="1"/>
+    <col min="13" max="14" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>246</v>
       </c>
@@ -8333,25 +8386,28 @@
         <v>38</v>
       </c>
       <c r="H1" t="s">
+        <v>488</v>
+      </c>
+      <c r="I1" t="s">
         <v>47</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>341</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>342</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>351</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -8374,25 +8430,28 @@
         <v>37</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -8406,7 +8465,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -8420,7 +8479,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Update highs_method description and changed default to choose (using Simplex or IPM with a MIP model will not work - it will be solved as LP)
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8847FA-9772-4139-99DA-C95158972008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A74194-F64F-471E-B9C1-BB27369EC1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30360" windowHeight="21000" tabRatio="1000" firstSheet="9" activeTab="27" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21240" windowHeight="21000" tabRatio="1000" firstSheet="3" activeTab="4" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -1605,9 +1605,6 @@
     <t>highs_method</t>
   </si>
   <si>
-    <t>HiGHS solver method ('simplex' or 'ipm' which is interior point method)</t>
-  </si>
-  <si>
     <t>HiGHS parallelises single solves or not ('on' or 'off'). It can be better to turn HiGHS parallel off when executing multiple scnearios in parallel.</t>
   </si>
   <si>
@@ -1678,6 +1675,9 @@
   </si>
   <si>
     <t>Choice of the CO2 method: no_method, price, period, total, price_period, price_total, period_total, price_period_total</t>
+  </si>
+  <si>
+    <t>HiGHS solver method (use 'choose' for MIP models, for LP models it's possible to choose 'simplex' or 'ipm' which is interior point method)</t>
   </si>
 </sst>
 </file>
@@ -3721,7 +3721,7 @@
         <v>180</v>
       </c>
       <c r="E1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F1" t="s">
         <v>181</v>
@@ -3742,10 +3742,10 @@
         <v>168</v>
       </c>
       <c r="L1" t="s">
+        <v>475</v>
+      </c>
+      <c r="M1" t="s">
         <v>476</v>
-      </c>
-      <c r="M1" t="s">
-        <v>477</v>
       </c>
       <c r="N1" t="s">
         <v>361</v>
@@ -3840,7 +3840,7 @@
         <v>58</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>61</v>
@@ -3911,7 +3911,7 @@
         <v>157</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
@@ -4062,7 +4062,7 @@
         <v>145</v>
       </c>
       <c r="H8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I8" t="s">
         <v>441</v>
@@ -4153,7 +4153,7 @@
         <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F1" t="s">
         <v>67</v>
@@ -4200,7 +4200,7 @@
         <v>58</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>8</v>
@@ -4945,7 +4945,7 @@
         <v>373</v>
       </c>
       <c r="U1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="V1" t="s">
         <v>18</v>
@@ -5016,7 +5016,7 @@
         <v>5</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="V2" s="9" t="s">
         <v>3</v>
@@ -5224,7 +5224,7 @@
         <v>373</v>
       </c>
       <c r="M1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -5265,7 +5265,7 @@
         <v>5</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6381,7 +6381,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B36" s="25">
         <v>44889</v>
@@ -6390,12 +6390,12 @@
         <v>190</v>
       </c>
       <c r="D36" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B37" s="25">
         <v>44893</v>
@@ -6404,12 +6404,12 @@
         <v>190</v>
       </c>
       <c r="D37" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B38" s="25">
         <v>44903</v>
@@ -6418,7 +6418,7 @@
         <v>190</v>
       </c>
       <c r="D38" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -6877,7 +6877,7 @@
         <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G1" t="s">
         <v>253</v>
@@ -6921,7 +6921,7 @@
         <v>140</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>286</v>
@@ -7143,7 +7143,7 @@
         <v>172</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -8094,7 +8094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -8163,13 +8163,13 @@
         <v>409</v>
       </c>
       <c r="M1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N1" t="s">
         <v>38</v>
       </c>
       <c r="O1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="P1" t="s">
         <v>456</v>
@@ -8231,13 +8231,13 @@
         <v>289</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>37</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="P2" s="24" t="s">
         <v>11</v>
@@ -8386,7 +8386,7 @@
         <v>38</v>
       </c>
       <c r="H1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I1" t="s">
         <v>47</v>
@@ -8430,7 +8430,7 @@
         <v>37</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>9</v>
@@ -10385,7 +10385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640D032-37A5-47CC-8407-C4F7168BB93B}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -10419,10 +10419,10 @@
         <v>463</v>
       </c>
       <c r="F1" t="s">
+        <v>490</v>
+      </c>
+      <c r="G1" t="s">
         <v>466</v>
-      </c>
-      <c r="G1" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10462,13 +10462,13 @@
         <v>386</v>
       </c>
       <c r="E3" t="s">
+        <v>467</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>469</v>
-      </c>
       <c r="G3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -10485,13 +10485,13 @@
         <v>386</v>
       </c>
       <c r="E4" t="s">
+        <v>467</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>469</v>
-      </c>
       <c r="G4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -10508,13 +10508,13 @@
         <v>386</v>
       </c>
       <c r="E5" t="s">
+        <v>467</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>469</v>
-      </c>
       <c r="G5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -10531,13 +10531,13 @@
         <v>386</v>
       </c>
       <c r="E6" t="s">
+        <v>467</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>469</v>
-      </c>
       <c r="G6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -10554,13 +10554,13 @@
         <v>386</v>
       </c>
       <c r="E7" t="s">
+        <v>467</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>468</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>469</v>
-      </c>
       <c r="G7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Some cleanup for investment hard end
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A74194-F64F-471E-B9C1-BB27369EC1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75839A2-811A-499F-898B-77E44AD3286E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21240" windowHeight="21000" tabRatio="1000" firstSheet="3" activeTab="4" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -675,9 +675,6 @@
     <t>Constraints and the sense of the constraint (greater_than, equal, less_than) as well as a constant factor for the constraint equation.</t>
   </si>
   <si>
-    <t>discount_years</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -696,9 +693,6 @@
     <t>Name of timeblock set associated with the period.</t>
   </si>
   <si>
-    <t>How many years from the solve to the different periods included in the solve. Used for discounting.</t>
-  </si>
-  <si>
     <t>half_day</t>
   </si>
   <si>
@@ -1678,6 +1672,12 @@
   </si>
   <si>
     <t>HiGHS solver method (use 'choose' for MIP models, for LP models it's possible to choose 'simplex' or 'ipm' which is interior point method)</t>
+  </si>
+  <si>
+    <t>years_represented</t>
+  </si>
+  <si>
+    <t>How many years the period represents before the next period in the solve. Used for discounting. Can be below one (multiple periods in one year). Index: period, value: years.</t>
   </si>
 </sst>
 </file>
@@ -3309,7 +3309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3320,74 +3320,74 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="46" t="s">
-        <v>281</v>
-      </c>
       <c r="C1" s="46" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="E4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="E6" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="29" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
@@ -3397,65 +3397,65 @@
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
       <c r="E9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" s="31" t="s">
         <v>214</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>215</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C11" s="32"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>219</v>
+      </c>
+      <c r="C13" s="31" t="s">
         <v>220</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>221</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14" s="31" t="s">
         <v>239</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>240</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3467,26 +3467,26 @@
       <c r="A17" s="39"/>
       <c r="B17" s="39"/>
       <c r="C17" s="40" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B19" s="45"/>
       <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
@@ -3498,45 +3498,45 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C22" s="34"/>
       <c r="D22" s="28"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B23" s="41"/>
       <c r="C23" s="41"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
@@ -3548,65 +3548,65 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="42"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B30" s="36"/>
       <c r="C30" s="35" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="48" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
@@ -3711,47 +3711,47 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="M1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="N1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="O1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="P1" t="s">
         <v>66</v>
@@ -3760,25 +3760,25 @@
         <v>69</v>
       </c>
       <c r="R1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="S1" t="s">
         <v>70</v>
       </c>
       <c r="T1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="U1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="V1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="W1" t="s">
         <v>20</v>
       </c>
       <c r="X1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="Y1" t="s">
         <v>23</v>
@@ -3787,16 +3787,16 @@
         <v>71</v>
       </c>
       <c r="AA1" t="s">
+        <v>429</v>
+      </c>
+      <c r="AB1" s="5" t="s">
         <v>431</v>
       </c>
-      <c r="AB1" s="5" t="s">
-        <v>433</v>
-      </c>
       <c r="AC1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AD1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="AE1" t="s">
         <v>72</v>
@@ -3810,28 +3810,28 @@
         <v>57</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>59</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>60</v>
@@ -3840,7 +3840,7 @@
         <v>58</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>61</v>
@@ -3861,13 +3861,13 @@
         <v>14</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="U2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="V2" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>6</v>
@@ -3882,16 +3882,16 @@
         <v>63</v>
       </c>
       <c r="AA2" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="AB2" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="AB2" s="9" t="s">
-        <v>432</v>
-      </c>
       <c r="AC2" s="9" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="AD2" s="9" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="AE2" s="9" t="s">
         <v>64</v>
@@ -3905,13 +3905,13 @@
         <v>146</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
@@ -3932,13 +3932,13 @@
         <v>147</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
@@ -3963,7 +3963,7 @@
         <v>148</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G5" t="s">
         <v>145</v>
@@ -3980,10 +3980,10 @@
         <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G6" t="s">
         <v>145</v>
@@ -3997,31 +3997,31 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G7" t="s">
         <v>145</v>
       </c>
       <c r="H7" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="J7" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="N7">
         <v>12000</v>
@@ -4044,28 +4044,28 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G8" t="s">
         <v>145</v>
       </c>
       <c r="H8" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I8" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="N8">
         <v>12000</v>
@@ -4082,13 +4082,13 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G9" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="Q9">
         <v>800</v>
@@ -4145,7 +4145,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4153,7 +4153,7 @@
         <v>65</v>
       </c>
       <c r="E1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F1" t="s">
         <v>67</v>
@@ -4162,19 +4162,19 @@
         <v>68</v>
       </c>
       <c r="H1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="I1" t="s">
+        <v>364</v>
+      </c>
+      <c r="J1" t="s">
+        <v>365</v>
+      </c>
+      <c r="K1" t="s">
+        <v>361</v>
+      </c>
+      <c r="L1" t="s">
         <v>366</v>
-      </c>
-      <c r="J1" t="s">
-        <v>367</v>
-      </c>
-      <c r="K1" t="s">
-        <v>363</v>
-      </c>
-      <c r="L1" t="s">
-        <v>368</v>
       </c>
       <c r="M1" t="s">
         <v>20</v>
@@ -4183,7 +4183,7 @@
         <v>23</v>
       </c>
       <c r="O1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4200,7 +4200,7 @@
         <v>58</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>8</v>
@@ -4215,13 +4215,13 @@
         <v>13</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>6</v>
@@ -4277,7 +4277,7 @@
         <v>146</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D5">
         <f>250*8760*1.1</f>
@@ -4316,7 +4316,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4331,7 +4331,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>60</v>
@@ -4649,14 +4649,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
         <v>73</v>
       </c>
       <c r="D1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4692,7 +4692,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4">
         <v>0.2</v>
@@ -4727,12 +4727,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4754,7 +4754,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>77</v>
@@ -4768,7 +4768,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>78</v>
@@ -4782,10 +4782,10 @@
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -4842,10 +4842,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -4891,28 +4891,28 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" t="s">
+        <v>176</v>
+      </c>
+      <c r="H1" t="s">
+        <v>454</v>
+      </c>
+      <c r="I1" t="s">
         <v>177</v>
       </c>
-      <c r="G1" t="s">
-        <v>178</v>
-      </c>
-      <c r="H1" t="s">
-        <v>456</v>
-      </c>
-      <c r="I1" t="s">
-        <v>179</v>
-      </c>
       <c r="J1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K1" t="s">
         <v>19</v>
@@ -4921,19 +4921,19 @@
         <v>22</v>
       </c>
       <c r="M1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="N1" t="s">
         <v>25</v>
       </c>
       <c r="O1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="P1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="Q1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="R1" t="s">
         <v>20</v>
@@ -4942,16 +4942,16 @@
         <v>23</v>
       </c>
       <c r="T1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="U1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="V1" t="s">
         <v>18</v>
       </c>
       <c r="W1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -4962,13 +4962,13 @@
         <v>26</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -4980,7 +4980,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -4998,13 +4998,13 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>6</v>
@@ -5016,7 +5016,7 @@
         <v>5</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="V2" s="9" t="s">
         <v>3</v>
@@ -5039,19 +5039,19 @@
         <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H3" t="s">
         <v>145</v>
       </c>
       <c r="I3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K3">
         <v>100</v>
@@ -5059,25 +5059,25 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H4" t="s">
         <v>145</v>
@@ -5091,7 +5091,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>31</v>
@@ -5103,7 +5103,7 @@
         <v>147</v>
       </c>
       <c r="H5" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L5">
         <v>100</v>
@@ -5123,19 +5123,19 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H6" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L6">
         <v>100</v>
@@ -5192,7 +5192,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5200,19 +5200,19 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F1" t="s">
         <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J1" t="s">
         <v>20</v>
@@ -5221,10 +5221,10 @@
         <v>23</v>
       </c>
       <c r="L1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="M1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -5247,13 +5247,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -5265,7 +5265,7 @@
         <v>5</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -5304,7 +5304,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -5339,7 +5339,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5351,7 +5351,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -5611,23 +5611,23 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H1" t="s">
         <v>19</v>
@@ -5636,19 +5636,19 @@
         <v>22</v>
       </c>
       <c r="J1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="K1" t="s">
         <v>25</v>
       </c>
       <c r="L1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="M1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="N1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="O1" t="s">
         <v>20</v>
@@ -5657,28 +5657,28 @@
         <v>23</v>
       </c>
       <c r="Q1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="R1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="S1" t="s">
         <v>109</v>
       </c>
       <c r="T1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="U1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="V1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="W1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="X1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5689,7 +5689,7 @@
         <v>123</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>108</v>
@@ -5716,13 +5716,13 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="O2" s="24" t="s">
         <v>6</v>
@@ -5763,13 +5763,13 @@
         <v>149</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F3" s="47"/>
       <c r="G3" s="47" t="s">
@@ -5803,13 +5803,13 @@
         <v>150</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="47" t="s">
@@ -5827,16 +5827,16 @@
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
@@ -5854,30 +5854,30 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>149</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G7" s="47" t="s">
         <v>145</v>
@@ -5914,511 +5914,511 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" t="s">
         <v>186</v>
       </c>
-      <c r="B3" t="s">
-        <v>188</v>
-      </c>
       <c r="C3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" t="s">
         <v>189</v>
-      </c>
-      <c r="D3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" t="s">
         <v>190</v>
-      </c>
-      <c r="D4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B6" s="25">
         <v>44600</v>
       </c>
       <c r="C6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B7" s="25">
         <v>44602</v>
       </c>
       <c r="C7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
       </c>
       <c r="C8" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
       </c>
       <c r="C9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B10" s="25">
         <v>44602</v>
       </c>
       <c r="C10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D10" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
       </c>
       <c r="C11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
       </c>
       <c r="C12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D12" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
       </c>
       <c r="C13" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
       </c>
       <c r="C14" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
       </c>
       <c r="C15" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D15" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
       </c>
       <c r="C16" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D16" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
       </c>
       <c r="C17" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D17" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
       </c>
       <c r="C18" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
       </c>
       <c r="C19" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D19" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
       </c>
       <c r="C20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D20" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
       </c>
       <c r="C21" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D21" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
       </c>
       <c r="C22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D22" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
       </c>
       <c r="C23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D23" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
       </c>
       <c r="C24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
       </c>
       <c r="C25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D25" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
       </c>
       <c r="C26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D26" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B27" s="25">
         <v>44701</v>
       </c>
       <c r="C27" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D27" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B28" s="25">
         <v>44712</v>
       </c>
       <c r="C28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D28" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B29" s="25">
         <v>44727</v>
       </c>
       <c r="C29" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D29" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B30" s="25">
         <v>44734</v>
       </c>
       <c r="C30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D30" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B31" s="25">
         <v>44741</v>
       </c>
       <c r="C31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D31" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B32" s="25">
         <v>44840</v>
       </c>
       <c r="C32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D32" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B33" s="25">
         <v>44850</v>
       </c>
       <c r="C33" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D33" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B34" s="25">
         <v>44875</v>
       </c>
       <c r="C34" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D34" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B35" s="25">
         <v>44876</v>
       </c>
       <c r="C35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D35" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B36" s="25">
         <v>44889</v>
       </c>
       <c r="C36" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D36" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B37" s="25">
         <v>44893</v>
       </c>
       <c r="C37" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D37" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B38" s="25">
         <v>44903</v>
       </c>
       <c r="C38" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D38" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -6457,7 +6457,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6465,19 +6465,19 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F1" t="s">
         <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="J1" t="s">
         <v>20</v>
@@ -6486,10 +6486,10 @@
         <v>23</v>
       </c>
       <c r="L1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="M1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6512,13 +6512,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -6569,7 +6569,7 @@
         <v>149</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D5">
         <v>75</v>
@@ -6604,7 +6604,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6616,7 +6616,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -6630,7 +6630,7 @@
         <v>123</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -6868,7 +6868,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6877,19 +6877,19 @@
         <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I1" t="s">
         <v>118</v>
       </c>
       <c r="J1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="K1" t="s">
         <v>120</v>
@@ -6898,7 +6898,7 @@
         <v>122</v>
       </c>
       <c r="M1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -6915,16 +6915,16 @@
         <v>57</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>140</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>111</v>
@@ -6942,7 +6942,7 @@
         <v>121</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
@@ -6959,7 +6959,7 @@
         <v>148</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6982,7 +6982,7 @@
         <v>146</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -6996,13 +6996,13 @@
         <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -7013,13 +7013,13 @@
         <v>28</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>147</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -7039,27 +7039,27 @@
         <v>146</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -7067,16 +7067,16 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -7084,16 +7084,16 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -7128,7 +7128,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -7140,10 +7140,10 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7152,7 +7152,7 @@
         <v>123</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -7161,7 +7161,7 @@
         <v>57</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7169,10 +7169,10 @@
         <v>27</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7412,7 +7412,7 @@
         <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7426,13 +7426,13 @@
         <v>144</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7871,12 +7871,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7890,7 +7890,7 @@
         <v>143</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -7904,13 +7904,13 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -7943,12 +7943,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7962,7 +7962,7 @@
         <v>143</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -7979,10 +7979,10 @@
         <v>31</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -8016,13 +8016,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -8039,7 +8039,7 @@
         <v>143</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -8062,7 +8062,7 @@
         <v>144</v>
       </c>
       <c r="E3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -8070,16 +8070,16 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E4" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -8129,11 +8129,11 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D1" t="s">
         <v>40</v>
@@ -8142,7 +8142,7 @@
         <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="G1" t="s">
         <v>42</v>
@@ -8151,7 +8151,7 @@
         <v>46</v>
       </c>
       <c r="I1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="J1" t="s">
         <v>44</v>
@@ -8160,19 +8160,19 @@
         <v>54</v>
       </c>
       <c r="L1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="M1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="N1" t="s">
         <v>38</v>
       </c>
       <c r="O1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="P1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="Q1" t="s">
         <v>48</v>
@@ -8181,16 +8181,16 @@
         <v>52</v>
       </c>
       <c r="S1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="T1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="U1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="V1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -8201,7 +8201,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>39</v>
@@ -8210,7 +8210,7 @@
         <v>35</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>41</v>
@@ -8228,16 +8228,16 @@
         <v>53</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>37</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="P2" s="24" t="s">
         <v>11</v>
@@ -8249,16 +8249,16 @@
         <v>51</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -8278,7 +8278,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H4">
         <v>200</v>
@@ -8295,24 +8295,24 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="S6">
         <v>40</v>
@@ -8326,10 +8326,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -8369,7 +8369,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8386,7 +8386,7 @@
         <v>38</v>
       </c>
       <c r="H1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="I1" t="s">
         <v>47</v>
@@ -8395,16 +8395,16 @@
         <v>50</v>
       </c>
       <c r="K1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="L1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="M1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="N1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -8430,7 +8430,7 @@
         <v>37</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>9</v>
@@ -8439,16 +8439,16 @@
         <v>49</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -8487,7 +8487,7 @@
         <v>152</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -8520,10 +8520,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8532,42 +8532,42 @@
         <v>28</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>318</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>320</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>383</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>28</v>
@@ -8608,94 +8608,94 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>320</v>
-      </c>
       <c r="F4" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="K4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="M4" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="J5" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="K5" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -8833,12 +8833,12 @@
         <v>152</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>146</v>
@@ -8846,7 +8846,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>146</v>
@@ -8854,7 +8854,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>147</v>
@@ -8942,7 +8942,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>149</v>
@@ -8953,10 +8953,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>147</v>
@@ -8996,14 +8996,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G1" t="s">
         <v>128</v>
@@ -9041,7 +9041,7 @@
         <v>57</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>127</v>
@@ -9064,13 +9064,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>31</v>
@@ -9079,7 +9079,7 @@
         <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -9122,22 +9122,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F1" t="s">
         <v>136</v>
       </c>
       <c r="G1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="H1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -9180,19 +9180,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>281</v>
+      </c>
+      <c r="E3" t="s">
         <v>282</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>283</v>
-      </c>
-      <c r="E3" t="s">
-        <v>284</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -9233,7 +9233,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -9262,7 +9262,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -9425,14 +9425,14 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G1" t="s">
         <v>128</v>
@@ -9470,7 +9470,7 @@
         <v>57</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>127</v>
@@ -9493,13 +9493,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>149</v>
@@ -9508,7 +9508,7 @@
         <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I3">
         <v>0.5</v>
@@ -9519,13 +9519,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>150</v>
@@ -9534,7 +9534,7 @@
         <v>146</v>
       </c>
       <c r="F4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -9545,13 +9545,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>149</v>
@@ -9560,7 +9560,7 @@
         <v>146</v>
       </c>
       <c r="F5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I5">
         <v>0.01</v>
@@ -9571,22 +9571,22 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>147</v>
       </c>
       <c r="F6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I6">
         <v>0.5</v>
@@ -9597,13 +9597,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>149</v>
@@ -9612,7 +9612,7 @@
         <v>146</v>
       </c>
       <c r="F7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I7">
         <v>0.01</v>
@@ -9650,12 +9650,12 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E1" t="s">
         <v>155</v>
@@ -9678,7 +9678,7 @@
         <v>153</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>154</v>
@@ -9695,13 +9695,13 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -9709,16 +9709,16 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>398</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -9726,16 +9726,16 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9765,8 +9765,8 @@
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="14" width="11.5703125" customWidth="1"/>
@@ -9774,15 +9774,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E1" t="s">
-        <v>163</v>
+        <v>490</v>
       </c>
       <c r="F1" t="s">
         <v>75</v>
@@ -9802,16 +9802,16 @@
         <v>32</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>156</v>
+        <v>489</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -9825,16 +9825,16 @@
         <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -9848,18 +9848,18 @@
         <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>33</v>
@@ -9868,18 +9868,18 @@
         <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>33</v>
@@ -9888,38 +9888,38 @@
         <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>34</v>
@@ -9928,53 +9928,53 @@
         <v>78</v>
       </c>
       <c r="D8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E9">
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>78</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -10015,14 +10015,14 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" s="3"/>
       <c r="E1"/>
       <c r="F1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -10036,13 +10036,13 @@
         <v>57</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>142</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -10056,10 +10056,10 @@
         <v>148</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -10076,10 +10076,10 @@
         <v>146</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F4">
         <v>-0.1</v>
@@ -10087,19 +10087,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>396</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>337</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>398</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -10107,19 +10107,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>146</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -10156,13 +10156,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10179,7 +10179,7 @@
         <v>142</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -10213,15 +10213,15 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10235,21 +10235,21 @@
         <v>142</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -10285,12 +10285,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10304,7 +10304,7 @@
         <v>142</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -10337,12 +10337,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10356,18 +10356,18 @@
         <v>142</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D3">
         <v>-8</v>
@@ -10385,7 +10385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640D032-37A5-47CC-8407-C4F7168BB93B}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -10406,23 +10406,23 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="E1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="G1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10433,19 +10433,19 @@
         <v>76</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -10459,21 +10459,21 @@
         <v>79</v>
       </c>
       <c r="D3" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>33</v>
@@ -10482,44 +10482,44 @@
         <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G5" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
@@ -10528,86 +10528,86 @@
         <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="E7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D9" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -10642,7 +10642,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -10655,13 +10655,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>81</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10669,7 +10669,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>29</v>
@@ -10683,7 +10683,7 @@
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>29</v>
@@ -10723,12 +10723,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10739,10 +10739,10 @@
         <v>104</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -11114,7 +11114,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -11171,7 +11171,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>104</v>
@@ -11179,7 +11179,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>105</v>
@@ -11187,7 +11187,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Update input files again (discount_years had somehow remained there)
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{356184BC-A55F-4E3D-8367-ECA4BF70C6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38742156-D32F-47E5-A5F4-B83F865A266F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="504">
   <si>
     <t>commodity</t>
   </si>
@@ -651,9 +651,6 @@
     <t>Constraints and the sense of the constraint (greater_than, equal, less_than) as well as a constant factor for the constraint equation.</t>
   </si>
   <si>
-    <t>discount_years</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -672,9 +669,6 @@
     <t>Name of timeblock set associated with the period.</t>
   </si>
   <si>
-    <t>How many years from the solve to the different periods included in the solve. Used for discounting.</t>
-  </si>
-  <si>
     <t>half_day</t>
   </si>
   <si>
@@ -1719,16 +1713,10 @@
     <t>solver_argument_9</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>test this</t>
-  </si>
-  <si>
-    <t>test this too</t>
-  </si>
-  <si>
-    <t>foo</t>
+    <t>years_represented</t>
+  </si>
+  <si>
+    <t>How many years the period represents before the next period in the solve. Used for discounting. Can be below one (multiple periods in one year). Index: period, value: years.</t>
   </si>
 </sst>
 </file>
@@ -3350,81 +3338,81 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>268</v>
       </c>
-      <c r="B1" s="46" t="s">
-        <v>270</v>
-      </c>
       <c r="C1" s="46" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="E4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="E6" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="43"/>
@@ -3434,65 +3422,65 @@
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
       <c r="E10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="C11" s="31" t="s">
         <v>203</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C12" s="32"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14" s="31" t="s">
         <v>209</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>227</v>
+      </c>
+      <c r="C15" s="31" t="s">
         <v>228</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>229</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B16" s="32"/>
       <c r="C16" s="31" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3504,26 +3492,26 @@
       <c r="A18" s="39"/>
       <c r="B18" s="39"/>
       <c r="C18" s="40" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B19" s="45"/>
       <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
@@ -3535,45 +3523,45 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B23" s="34" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C23" s="34"/>
       <c r="D23" s="28"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B24" s="41"/>
       <c r="C24" s="41"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
@@ -3585,65 +3573,65 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="42"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B31" s="36"/>
       <c r="C31" s="35" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B32" s="42"/>
       <c r="C32" s="42"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="48" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B39" s="48"/>
       <c r="C39" s="48"/>
@@ -3749,47 +3737,47 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="I1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="K1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="M1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="N1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="O1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="P1" t="s">
         <v>65</v>
@@ -3798,25 +3786,25 @@
         <v>68</v>
       </c>
       <c r="R1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="S1" t="s">
         <v>69</v>
       </c>
       <c r="T1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="U1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="V1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="W1" t="s">
         <v>19</v>
       </c>
       <c r="X1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="Y1" t="s">
         <v>22</v>
@@ -3825,19 +3813,19 @@
         <v>70</v>
       </c>
       <c r="AA1" t="s">
+        <v>414</v>
+      </c>
+      <c r="AB1" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="AB1" s="5" t="s">
-        <v>418</v>
-      </c>
       <c r="AC1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AD1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="AE1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3848,28 +3836,28 @@
         <v>56</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>59</v>
@@ -3878,7 +3866,7 @@
         <v>57</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>60</v>
@@ -3899,13 +3887,13 @@
         <v>14</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="U2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="V2" s="24" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>6</v>
@@ -3920,16 +3908,16 @@
         <v>62</v>
       </c>
       <c r="AA2" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="AB2" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="AB2" s="9" t="s">
-        <v>417</v>
-      </c>
       <c r="AC2" s="9" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="AD2" s="9" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="AE2" s="9" t="s">
         <v>63</v>
@@ -3943,13 +3931,13 @@
         <v>138</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
@@ -3970,13 +3958,13 @@
         <v>139</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
@@ -4001,7 +3989,7 @@
         <v>140</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G5" t="s">
         <v>137</v>
@@ -4018,10 +4006,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G6" t="s">
         <v>137</v>
@@ -4035,31 +4023,31 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G7" t="s">
         <v>137</v>
       </c>
       <c r="H7" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I7" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="J7" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="N7">
         <v>12000</v>
@@ -4082,28 +4070,28 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G8" t="s">
         <v>137</v>
       </c>
       <c r="H8" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I8" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="N8">
         <v>12000</v>
@@ -4120,13 +4108,13 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="G9" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="Q9">
         <v>800</v>
@@ -4183,7 +4171,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4191,7 +4179,7 @@
         <v>64</v>
       </c>
       <c r="E1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F1" t="s">
         <v>66</v>
@@ -4200,19 +4188,19 @@
         <v>67</v>
       </c>
       <c r="H1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I1" t="s">
+        <v>352</v>
+      </c>
+      <c r="J1" t="s">
+        <v>353</v>
+      </c>
+      <c r="K1" t="s">
+        <v>349</v>
+      </c>
+      <c r="L1" t="s">
         <v>354</v>
-      </c>
-      <c r="J1" t="s">
-        <v>355</v>
-      </c>
-      <c r="K1" t="s">
-        <v>351</v>
-      </c>
-      <c r="L1" t="s">
-        <v>356</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
@@ -4221,7 +4209,7 @@
         <v>22</v>
       </c>
       <c r="O1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4238,7 +4226,7 @@
         <v>57</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>8</v>
@@ -4253,13 +4241,13 @@
         <v>13</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>6</v>
@@ -4315,7 +4303,7 @@
         <v>138</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D5">
         <f>250*8760*1.1</f>
@@ -4354,7 +4342,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -4369,7 +4357,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>59</v>
@@ -4687,14 +4675,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
         <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4730,7 +4718,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4">
         <v>0.2</v>
@@ -4765,12 +4753,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4792,7 +4780,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>75</v>
@@ -4806,7 +4794,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>76</v>
@@ -4820,10 +4808,10 @@
         <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -4880,10 +4868,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -4929,28 +4917,28 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="J1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K1" t="s">
         <v>18</v>
@@ -4959,19 +4947,19 @@
         <v>21</v>
       </c>
       <c r="M1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="N1" t="s">
         <v>24</v>
       </c>
       <c r="O1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="P1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="Q1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="R1" t="s">
         <v>19</v>
@@ -4980,16 +4968,16 @@
         <v>22</v>
       </c>
       <c r="T1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="U1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="V1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="W1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -5000,13 +4988,13 @@
         <v>25</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -5018,7 +5006,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>15</v>
@@ -5036,13 +5024,13 @@
         <v>14</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="R2" s="9" t="s">
         <v>6</v>
@@ -5054,7 +5042,7 @@
         <v>5</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="V2" s="9" t="s">
         <v>3</v>
@@ -5077,19 +5065,19 @@
         <v>139</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H3" t="s">
         <v>137</v>
       </c>
       <c r="I3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K3">
         <v>100</v>
@@ -5097,25 +5085,25 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H4" t="s">
         <v>137</v>
@@ -5129,7 +5117,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>30</v>
@@ -5141,7 +5129,7 @@
         <v>139</v>
       </c>
       <c r="H5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="L5">
         <v>100</v>
@@ -5161,19 +5149,19 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="L6">
         <v>100</v>
@@ -5230,7 +5218,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5238,19 +5226,19 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F1" t="s">
         <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="I1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="J1" t="s">
         <v>19</v>
@@ -5259,10 +5247,10 @@
         <v>22</v>
       </c>
       <c r="L1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="M1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -5285,13 +5273,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -5303,7 +5291,7 @@
         <v>5</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -5342,7 +5330,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -5377,7 +5365,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5389,7 +5377,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -5649,23 +5637,23 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
@@ -5674,19 +5662,19 @@
         <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K1" t="s">
         <v>24</v>
       </c>
       <c r="L1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="M1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="N1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="O1" t="s">
         <v>19</v>
@@ -5695,28 +5683,28 @@
         <v>22</v>
       </c>
       <c r="Q1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="R1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="S1" t="s">
         <v>106</v>
       </c>
       <c r="T1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="U1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="V1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="W1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="X1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -5727,7 +5715,7 @@
         <v>117</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>105</v>
@@ -5754,13 +5742,13 @@
         <v>14</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="M2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O2" s="24" t="s">
         <v>6</v>
@@ -5801,13 +5789,13 @@
         <v>141</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E3" s="47" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F3" s="47"/>
       <c r="G3" s="47" t="s">
@@ -5841,13 +5829,13 @@
         <v>142</v>
       </c>
       <c r="C4" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="47" t="s">
@@ -5865,16 +5853,16 @@
         <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
@@ -5892,30 +5880,30 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>141</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G7" s="47" t="s">
         <v>137</v>
@@ -5950,511 +5938,511 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
         <v>175</v>
       </c>
-      <c r="B3" t="s">
-        <v>177</v>
-      </c>
       <c r="C3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" t="s">
         <v>178</v>
-      </c>
-      <c r="D3" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" t="s">
         <v>179</v>
-      </c>
-      <c r="D4" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B6" s="25">
         <v>44600</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B7" s="25">
         <v>44602</v>
       </c>
       <c r="C7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
       </c>
       <c r="C8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
       </c>
       <c r="C9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B10" s="25">
         <v>44602</v>
       </c>
       <c r="C10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
       </c>
       <c r="C11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D11" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
       </c>
       <c r="C12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D12" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
       </c>
       <c r="C13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D13" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
       </c>
       <c r="C14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
       </c>
       <c r="C15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D15" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
       </c>
       <c r="C16" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
       </c>
       <c r="C17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D17" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D18" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
       </c>
       <c r="C19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D19" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
       </c>
       <c r="C20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D20" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
       </c>
       <c r="C21" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D21" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
       </c>
       <c r="C22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D22" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
       </c>
       <c r="C23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
       </c>
       <c r="C24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D24" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
       </c>
       <c r="C25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D25" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
       </c>
       <c r="C26" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D26" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B27" s="25">
         <v>44701</v>
       </c>
       <c r="C27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D27" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B28" s="25">
         <v>44712</v>
       </c>
       <c r="C28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D28" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B29" s="25">
         <v>44727</v>
       </c>
       <c r="C29" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D29" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B30" s="25">
         <v>44734</v>
       </c>
       <c r="C30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D30" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B31" s="25">
         <v>44741</v>
       </c>
       <c r="C31" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D31" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B32" s="25">
         <v>44840</v>
       </c>
       <c r="C32" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D32" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B33" s="25">
         <v>44850</v>
       </c>
       <c r="C33" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D33" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B34" s="25">
         <v>44875</v>
       </c>
       <c r="C34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D34" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B35" s="25">
         <v>44876</v>
       </c>
       <c r="C35" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D35" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B36" s="25">
         <v>44889</v>
       </c>
       <c r="C36" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D36" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B37" s="25">
         <v>44893</v>
       </c>
       <c r="C37" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D37" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B38" s="25">
         <v>44903</v>
       </c>
       <c r="C38" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D38" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -6493,7 +6481,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6501,19 +6489,19 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F1" t="s">
         <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="I1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="J1" t="s">
         <v>19</v>
@@ -6522,10 +6510,10 @@
         <v>22</v>
       </c>
       <c r="L1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="M1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -6548,13 +6536,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -6605,7 +6593,7 @@
         <v>141</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D5">
         <v>75</v>
@@ -6640,7 +6628,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -6652,7 +6640,7 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>3</v>
@@ -6666,7 +6654,7 @@
         <v>117</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -6903,34 +6891,34 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
+        <v>479</v>
+      </c>
+      <c r="F1" t="s">
+        <v>454</v>
+      </c>
+      <c r="G1" t="s">
+        <v>240</v>
+      </c>
+      <c r="H1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1" t="s">
+        <v>480</v>
+      </c>
+      <c r="J1" t="s">
+        <v>362</v>
+      </c>
+      <c r="K1" t="s">
         <v>481</v>
       </c>
-      <c r="F1" t="s">
-        <v>456</v>
-      </c>
-      <c r="G1" t="s">
-        <v>242</v>
-      </c>
-      <c r="H1" t="s">
-        <v>241</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>482</v>
-      </c>
-      <c r="J1" t="s">
-        <v>364</v>
-      </c>
-      <c r="K1" t="s">
-        <v>483</v>
-      </c>
-      <c r="L1" t="s">
-        <v>484</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -6947,16 +6935,16 @@
         <v>56</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>108</v>
@@ -6988,7 +6976,7 @@
         <v>140</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -7011,7 +6999,7 @@
         <v>138</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -7025,13 +7013,13 @@
         <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -7042,13 +7030,13 @@
         <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>139</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -7068,27 +7056,27 @@
         <v>138</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -7096,16 +7084,16 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -7113,16 +7101,16 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -7157,7 +7145,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -7169,10 +7157,10 @@
     <row r="2" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7181,7 +7169,7 @@
         <v>117</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -7190,7 +7178,7 @@
         <v>56</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -7198,10 +7186,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7441,7 +7429,7 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7455,13 +7443,13 @@
         <v>136</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7900,12 +7888,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7919,7 +7907,7 @@
         <v>135</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -7933,13 +7921,13 @@
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -7972,12 +7960,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -7991,7 +7979,7 @@
         <v>135</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -8008,10 +7996,10 @@
         <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -8045,13 +8033,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -8068,7 +8056,7 @@
         <v>135</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -8091,7 +8079,7 @@
         <v>136</v>
       </c>
       <c r="E3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -8099,16 +8087,16 @@
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="E4" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -8158,11 +8146,11 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D1" t="s">
         <v>39</v>
@@ -8171,7 +8159,7 @@
         <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G1" t="s">
         <v>41</v>
@@ -8180,7 +8168,7 @@
         <v>45</v>
       </c>
       <c r="I1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="J1" t="s">
         <v>43</v>
@@ -8189,19 +8177,19 @@
         <v>53</v>
       </c>
       <c r="L1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="M1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="N1" t="s">
         <v>37</v>
       </c>
       <c r="O1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="P1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="Q1" t="s">
         <v>47</v>
@@ -8210,16 +8198,16 @@
         <v>51</v>
       </c>
       <c r="S1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="T1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="U1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="V1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -8230,7 +8218,7 @@
         <v>55</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>38</v>
@@ -8239,7 +8227,7 @@
         <v>34</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>40</v>
@@ -8257,16 +8245,16 @@
         <v>52</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="N2" s="9" t="s">
         <v>36</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="P2" s="24" t="s">
         <v>11</v>
@@ -8278,16 +8266,16 @@
         <v>50</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -8307,7 +8295,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H4">
         <v>200</v>
@@ -8324,24 +8312,24 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="S6">
         <v>40</v>
@@ -8355,10 +8343,10 @@
         <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -8398,7 +8386,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -8415,7 +8403,7 @@
         <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I1" t="s">
         <v>46</v>
@@ -8424,16 +8412,16 @@
         <v>49</v>
       </c>
       <c r="K1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="L1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="M1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="N1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -8459,7 +8447,7 @@
         <v>36</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>9</v>
@@ -8468,16 +8456,16 @@
         <v>48</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -8516,7 +8504,7 @@
         <v>144</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -8549,10 +8537,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8561,42 +8549,42 @@
         <v>27</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>306</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>308</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>371</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>27</v>
@@ -8637,94 +8625,94 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>306</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>308</v>
-      </c>
       <c r="F4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H4" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="I4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="J4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="K4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="L4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="M4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J5" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="K5" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L5" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -8862,12 +8850,12 @@
         <v>144</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>138</v>
@@ -8875,7 +8863,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>138</v>
@@ -8883,7 +8871,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>139</v>
@@ -8971,7 +8959,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>141</v>
@@ -8982,10 +8970,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>139</v>
@@ -9025,17 +9013,17 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="H1" t="s">
         <v>132</v>
@@ -9070,7 +9058,7 @@
         <v>56</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>121</v>
@@ -9093,13 +9081,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>30</v>
@@ -9108,7 +9096,7 @@
         <v>138</v>
       </c>
       <c r="F3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -9151,22 +9139,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F1" t="s">
         <v>129</v>
       </c>
       <c r="G1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -9209,19 +9197,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3" t="s">
         <v>271</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="E3" t="s">
-        <v>273</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -9262,7 +9250,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -9291,7 +9279,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -9454,17 +9442,17 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="H1" t="s">
         <v>131</v>
@@ -9499,7 +9487,7 @@
         <v>56</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>121</v>
@@ -9522,13 +9510,13 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>141</v>
@@ -9537,7 +9525,7 @@
         <v>138</v>
       </c>
       <c r="F3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I3">
         <v>0.5</v>
@@ -9548,13 +9536,13 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>142</v>
@@ -9563,7 +9551,7 @@
         <v>138</v>
       </c>
       <c r="F4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -9574,13 +9562,13 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>141</v>
@@ -9589,7 +9577,7 @@
         <v>138</v>
       </c>
       <c r="F5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I5">
         <v>0.01</v>
@@ -9600,22 +9588,22 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>139</v>
       </c>
       <c r="F6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I6">
         <v>0.5</v>
@@ -9626,13 +9614,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>141</v>
@@ -9641,7 +9629,7 @@
         <v>138</v>
       </c>
       <c r="F7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I7">
         <v>0.01</v>
@@ -9679,12 +9667,12 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E1" t="s">
         <v>147</v>
@@ -9707,7 +9695,7 @@
         <v>145</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>146</v>
@@ -9724,13 +9712,13 @@
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -9738,16 +9726,16 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>385</v>
-      </c>
       <c r="C4" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -9755,16 +9743,16 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -9786,7 +9774,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9795,7 +9783,7 @@
     <col min="2" max="2" width="15.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.140625" style="4" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
     <col min="8" max="14" width="11.5703125" customWidth="1"/>
@@ -9803,15 +9791,15 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>155</v>
+        <v>503</v>
       </c>
       <c r="F1" t="s">
         <v>73</v>
@@ -9831,16 +9819,16 @@
         <v>31</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>148</v>
+        <v>502</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -9854,16 +9842,16 @@
         <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -9877,18 +9865,18 @@
         <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E4">
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
@@ -9897,18 +9885,18 @@
         <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>32</v>
@@ -9917,38 +9905,38 @@
         <v>76</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>33</v>
@@ -9957,53 +9945,53 @@
         <v>76</v>
       </c>
       <c r="D8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E9">
         <v>5</v>
       </c>
       <c r="G9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -10044,14 +10032,14 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" s="3"/>
       <c r="E1"/>
       <c r="F1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -10065,13 +10053,13 @@
         <v>56</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>134</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -10085,10 +10073,10 @@
         <v>140</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -10105,10 +10093,10 @@
         <v>138</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F4">
         <v>-0.1</v>
@@ -10116,19 +10104,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>383</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>325</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>385</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -10136,19 +10124,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -10185,13 +10173,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10208,7 +10196,7 @@
         <v>134</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -10242,15 +10230,15 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10264,21 +10252,21 @@
         <v>134</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -10314,12 +10302,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10333,7 +10321,7 @@
         <v>134</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -10366,12 +10354,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10385,18 +10373,18 @@
         <v>134</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D3">
         <v>-8</v>
@@ -10436,29 +10424,29 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D1" t="s">
+        <v>371</v>
+      </c>
+      <c r="E1" t="s">
+        <v>471</v>
+      </c>
+      <c r="F1" t="s">
+        <v>448</v>
+      </c>
+      <c r="G1" t="s">
+        <v>472</v>
+      </c>
+      <c r="H1" t="s">
         <v>491</v>
       </c>
-      <c r="D1" t="s">
-        <v>373</v>
-      </c>
-      <c r="E1" t="s">
-        <v>473</v>
-      </c>
-      <c r="F1" t="s">
-        <v>450</v>
-      </c>
-      <c r="G1" t="s">
-        <v>474</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>493</v>
-      </c>
-      <c r="I1" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10469,49 +10457,49 @@
         <v>74</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>492</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>494</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>496</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
+        <v>495</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>497</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>497</v>
-      </c>
-      <c r="M2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>499</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>500</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>501</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>502</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -10522,170 +10510,158 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E3" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="G3" t="s">
-        <v>451</v>
-      </c>
-      <c r="H3" t="s">
-        <v>505</v>
-      </c>
-      <c r="I3" t="s">
-        <v>504</v>
-      </c>
-      <c r="J3" t="s">
-        <v>506</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D4" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="G4" t="s">
-        <v>451</v>
-      </c>
-      <c r="I4" t="s">
-        <v>507</v>
+        <v>449</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="G5" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="G6" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C7" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="G7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D11" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -10720,7 +10696,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -10733,13 +10709,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10747,7 +10723,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>28</v>
@@ -10761,7 +10737,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>28</v>
@@ -10801,12 +10777,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10817,10 +10793,10 @@
         <v>101</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -11192,7 +11168,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
@@ -11249,7 +11225,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>101</v>
@@ -11257,7 +11233,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>102</v>
@@ -11265,7 +11241,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Lifetime_method introduced with options for reinvest_automatic and reinvest_choice.
Reinvest_choice means that at the end of the lifetime, the asset (unit, connection or storage in node) will cease to exist in the model unless the model decides to invest again. Automatic reinvestment means that whenever model invests in new capacity, it will be kept in the model forever through automatic reinvestments (the investment annuity is calculated until the end of model horizon for these investments).
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Toolbox_projects\FlexTool3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38742156-D32F-47E5-A5F4-B83F865A266F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E402EB-88A9-4269-8062-90BD563E90A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="1000" activeTab="18" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="508">
   <si>
     <t>commodity</t>
   </si>
@@ -1717,6 +1717,18 @@
   </si>
   <si>
     <t>How many years the period represents before the next period in the solve. Used for discounting. Can be below one (multiple periods in one year). Index: period, value: years.</t>
+  </si>
+  <si>
+    <t>21.0</t>
+  </si>
+  <si>
+    <t>Added lifetime_method to units, connections and nodes</t>
+  </si>
+  <si>
+    <t>lifetime_method</t>
+  </si>
+  <si>
+    <t>Choice how the investments behave after unit runs out of lifetime. Automatic reinvestment (reinvest_automatic - default) causes the model to keep the capacity until the end of model horizon and applies the annualized investment cost without further model choice. Choice of reinvestment (reinvest_choice) removes the capacity at the end of the lifetime and the model needs to decide how much new capacity is to be built.</t>
   </si>
 </sst>
 </file>
@@ -1901,7 +1913,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1998,6 +2010,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2709,7 +2724,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
+      <xdr:col>32</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -2919,7 +2934,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -3327,7 +3342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3693,13 +3708,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
-  <dimension ref="A1:AE9"/>
+  <dimension ref="A1:AF9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AE1" sqref="AE1"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3711,31 +3726,32 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" customWidth="1"/>
-    <col min="10" max="10" width="29.28515625" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" style="14" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" style="14" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" style="14" customWidth="1"/>
-    <col min="22" max="22" width="13.42578125" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" style="14" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" customWidth="1"/>
-    <col min="25" max="25" width="8.140625" customWidth="1"/>
-    <col min="26" max="27" width="18.140625" customWidth="1"/>
-    <col min="28" max="28" width="16.85546875" customWidth="1"/>
-    <col min="29" max="30" width="29.140625" customWidth="1"/>
-    <col min="31" max="31" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" customWidth="1"/>
+    <col min="11" max="11" width="29.28515625" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" style="14" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" style="14" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" style="14" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" style="14" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" customWidth="1"/>
+    <col min="26" max="26" width="8.140625" customWidth="1"/>
+    <col min="27" max="28" width="18.140625" customWidth="1"/>
+    <col min="29" max="29" width="16.85546875" customWidth="1"/>
+    <col min="30" max="31" width="29.140625" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>233</v>
       </c>
@@ -3756,79 +3772,82 @@
         <v>474</v>
       </c>
       <c r="H1" t="s">
+        <v>507</v>
+      </c>
+      <c r="I1" t="s">
         <v>437</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>428</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>157</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>457</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>458</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>347</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>348</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>68</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>283</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>69</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>284</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>349</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>350</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>351</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>70</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>414</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AC1" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>417</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>423</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -3851,79 +3870,82 @@
         <v>11</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="V2" s="24" t="s">
+      <c r="W2" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="W2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Z2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="AA2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AB2" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AC2" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AD2" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AE2" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="AE2" s="9" t="s">
+      <c r="AF2" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -3943,14 +3965,14 @@
       <c r="G3" t="s">
         <v>137</v>
       </c>
-      <c r="N3">
-        <v>10000</v>
-      </c>
       <c r="O3">
         <v>10000</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -3970,18 +3992,18 @@
       <c r="G4" t="s">
         <v>137</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f>100*8760</f>
         <v>876000</v>
       </c>
-      <c r="N4">
-        <v>10000</v>
-      </c>
       <c r="O4">
         <v>10000</v>
       </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -3994,14 +4016,14 @@
       <c r="G5" t="s">
         <v>137</v>
       </c>
-      <c r="N5">
-        <v>10000</v>
-      </c>
       <c r="O5">
         <v>10000</v>
       </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -4014,14 +4036,14 @@
       <c r="G6" t="s">
         <v>137</v>
       </c>
-      <c r="N6">
-        <v>10000</v>
-      </c>
       <c r="O6">
         <v>10000</v>
       </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>280</v>
       </c>
@@ -4040,35 +4062,35 @@
       <c r="G7" t="s">
         <v>137</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>427</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>424</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>425</v>
-      </c>
-      <c r="N7">
-        <v>12000</v>
       </c>
       <c r="O7">
         <v>12000</v>
       </c>
       <c r="P7">
+        <v>12000</v>
+      </c>
+      <c r="Q7">
         <v>20</v>
       </c>
-      <c r="Z7">
+      <c r="AA7">
         <v>0.01</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <v>0.1</v>
       </c>
-      <c r="AC7">
+      <c r="AD7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>381</v>
       </c>
@@ -4087,26 +4109,26 @@
       <c r="G8" t="s">
         <v>137</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>451</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>424</v>
-      </c>
-      <c r="N8">
-        <v>12000</v>
       </c>
       <c r="O8">
         <v>12000</v>
       </c>
       <c r="P8">
+        <v>12000</v>
+      </c>
+      <c r="Q8">
         <v>10000000</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>305</v>
       </c>
@@ -4116,19 +4138,19 @@
       <c r="G9" t="s">
         <v>438</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>800</v>
       </c>
-      <c r="U9" s="14">
+      <c r="V9" s="14">
         <v>200</v>
       </c>
-      <c r="W9" s="14">
+      <c r="X9" s="14">
         <v>0.05</v>
       </c>
-      <c r="Y9">
+      <c r="Z9">
         <v>10</v>
       </c>
-      <c r="AE9">
+      <c r="AF9">
         <v>1</v>
       </c>
     </row>
@@ -4881,13 +4903,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44D2B2-1DE7-400D-8C40-2CD59BEE6EC3}">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4900,22 +4922,23 @@
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
-    <col min="17" max="18" width="13" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" customWidth="1"/>
-    <col min="21" max="21" width="22" customWidth="1"/>
-    <col min="22" max="22" width="10" customWidth="1"/>
-    <col min="23" max="23" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
+    <col min="15" max="15" width="10.140625" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="19" width="13" customWidth="1"/>
+    <col min="20" max="20" width="9.85546875" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" customWidth="1"/>
+    <col min="22" max="22" width="22" customWidth="1"/>
+    <col min="23" max="23" width="10" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>233</v>
       </c>
@@ -4935,52 +4958,55 @@
         <v>439</v>
       </c>
       <c r="I1" t="s">
+        <v>507</v>
+      </c>
+      <c r="J1" t="s">
         <v>484</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>158</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>286</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>287</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>357</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>358</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>22</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>359</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>456</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>483</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -5006,52 +5032,55 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>453</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="W2" s="24" t="s">
+      <c r="X2" s="24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -5076,14 +5105,14 @@
       <c r="H3" t="s">
         <v>137</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>148</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>280</v>
       </c>
@@ -5108,14 +5137,14 @@
       <c r="H4" t="s">
         <v>137</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>10</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>305</v>
       </c>
@@ -5131,23 +5160,23 @@
       <c r="H5" t="s">
         <v>438</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>100</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>500</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>0.05</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>50</v>
       </c>
-      <c r="W5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>305</v>
       </c>
@@ -5163,19 +5192,19 @@
       <c r="H6" t="s">
         <v>438</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>100</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>0</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>0.05</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>20</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>1</v>
       </c>
     </row>
@@ -5599,13 +5628,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6619729E-584E-41E3-B72E-7B2979330C88}">
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5617,25 +5646,26 @@
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" customWidth="1"/>
-    <col min="15" max="15" width="8" customWidth="1"/>
-    <col min="16" max="16" width="8.5703125" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" customWidth="1"/>
-    <col min="20" max="20" width="12.140625" customWidth="1"/>
-    <col min="21" max="22" width="10.140625" customWidth="1"/>
-    <col min="23" max="24" width="8" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="7.7109375" customWidth="1"/>
+    <col min="16" max="16" width="8" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" customWidth="1"/>
+    <col min="19" max="19" width="11.7109375" customWidth="1"/>
+    <col min="20" max="20" width="9.85546875" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" customWidth="1"/>
+    <col min="22" max="23" width="10.140625" customWidth="1"/>
+    <col min="24" max="25" width="8" customWidth="1"/>
+    <col min="27" max="27" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>233</v>
       </c>
@@ -5656,58 +5686,61 @@
         <v>439</v>
       </c>
       <c r="H1" t="s">
+        <v>507</v>
+      </c>
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>286</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>287</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>360</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>361</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>359</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>158</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>106</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>297</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>478</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>182</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>183</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>1</v>
       </c>
@@ -5729,59 +5762,62 @@
       <c r="G2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="49" t="s">
+        <v>506</v>
+      </c>
+      <c r="I2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="J2" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="K2" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="24" t="s">
+      <c r="L2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="M2" s="24" t="s">
         <v>285</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="N2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="O2" s="24" t="s">
         <v>237</v>
       </c>
-      <c r="O2" s="24" t="s">
+      <c r="P2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="Q2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="24" t="s">
+      <c r="R2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="S2" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="24" t="s">
+      <c r="T2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="24" t="s">
+      <c r="U2" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="U2" s="24" t="s">
+      <c r="V2" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="V2" s="24" t="s">
+      <c r="W2" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="W2" s="24" t="s">
+      <c r="X2" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="X2" s="24" t="s">
+      <c r="Y2" s="24" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -5801,27 +5837,28 @@
       <c r="G3" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="47"/>
+      <c r="I3">
         <v>100</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>150</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>1000</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0.08</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>30</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>0.4</v>
       </c>
-      <c r="T3" s="5"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="U3" s="5"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -5841,14 +5878,15 @@
       <c r="G4" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="47"/>
+      <c r="I4">
         <v>100</v>
       </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -5868,17 +5906,18 @@
       <c r="G5" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="47"/>
+      <c r="I5">
         <v>200</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>0.45</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>305</v>
       </c>
@@ -5888,8 +5927,9 @@
       <c r="G6" s="47" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="H6" s="47"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>381</v>
       </c>
@@ -5908,10 +5948,11 @@
       <c r="G7" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="47"/>
+      <c r="I7">
         <v>10</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>1</v>
       </c>
     </row>
@@ -5925,9 +5966,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6443,6 +6486,20 @@
       </c>
       <c r="D38" t="s">
         <v>464</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="B39" s="25">
+        <v>45082</v>
+      </c>
+      <c r="C39" t="s">
+        <v>177</v>
+      </c>
+      <c r="D39" t="s">
+        <v>505</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
group output added flow_t result
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AETART\Documents\flextool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046A5A00-DB14-495D-8857-016014C1D7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744E1846-CB7E-487A-8218-0FE9E9D477C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28815" yWindow="-18120" windowWidth="29040" windowHeight="17640" tabRatio="1000" firstSheet="5" activeTab="16" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-15" yWindow="-18120" windowWidth="29040" windowHeight="17640" tabRatio="1000" firstSheet="8" activeTab="10" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -206,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="527">
   <si>
     <t>commodity</t>
   </si>
@@ -1582,9 +1582,6 @@
     <t>[MWh] Highest absolute flow in scaled inflow. Used only with inflow_method scale_to_annual_and_peak_flow. Constant or period.</t>
   </si>
   <si>
-    <t>scale_to_annual_and_peak_flow</t>
-  </si>
-  <si>
     <t>peak_inflow</t>
   </si>
   <si>
@@ -1753,9 +1750,6 @@
     <t>rolling_duration</t>
   </si>
   <si>
-    <t>(Optional) Timestamp from the timeline that is linked to the timeblockSet used. Start of the rolling, if not stated, assumed to be the first timestep</t>
-  </si>
-  <si>
     <t>(Required if rolling_window solve). The length of the jumps between rolls. Should be smaller than the horizon</t>
   </si>
   <si>
@@ -1765,9 +1759,6 @@
     <t>Hours (Optional). Duration of rolling, if not stated, assumed to be the whole time of the solve</t>
   </si>
   <si>
-    <t>rolling_start_time</t>
-  </si>
-  <si>
     <t>rolling_solve_jump</t>
   </si>
   <si>
@@ -1784,6 +1775,18 @@
   </si>
   <si>
     <t>availability</t>
+  </si>
+  <si>
+    <t>output_node_flows</t>
+  </si>
+  <si>
+    <t>output_aggregate_flows</t>
+  </si>
+  <si>
+    <t>Used with group_unit_node or group_connection_node to combine the flows when producing the output_node_flows of a node group.</t>
+  </si>
+  <si>
+    <t>Creates the timewise flow output for this node group (group_flow_t)</t>
   </si>
 </sst>
 </file>
@@ -2582,12 +2585,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5473550" cy="1023037"/>
+    <xdr:ext cx="5428794" cy="836896"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="TextBox 1">
@@ -2601,8 +2604,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10420350" y="1304925"/>
-          <a:ext cx="5473550" cy="1023037"/>
+          <a:off x="8924925" y="1304925"/>
+          <a:ext cx="5428794" cy="836896"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2636,14 +2639,6 @@
               <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
             <a:t>Define the rolling parameters. Required if the solve_mode is rolling_window:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="fi-FI" sz="1200" baseline="0">
-              <a:latin typeface="Arial Nova" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>- Rolling_start_time: Allows to set a different start time than the beginning</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3544,7 +3539,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3629,7 +3626,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="43"/>
@@ -3958,11 +3955,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AH3" sqref="AH3"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4013,19 +4010,19 @@
         <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F1" t="s">
         <v>169</v>
       </c>
       <c r="G1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="H1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="J1" t="s">
         <v>436</v>
@@ -4097,7 +4094,7 @@
         <v>422</v>
       </c>
       <c r="AG1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4123,10 +4120,10 @@
         <v>11</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>411</v>
@@ -4144,7 +4141,7 @@
         <v>57</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>60</v>
@@ -4201,7 +4198,7 @@
         <v>63</v>
       </c>
       <c r="AH2" s="9" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
@@ -4217,9 +4214,7 @@
       <c r="D3" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>458</v>
-      </c>
+      <c r="E3" s="14"/>
       <c r="F3" s="14"/>
       <c r="G3" t="s">
         <v>137</v>
@@ -4507,7 +4502,7 @@
         <v>57</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>8</v>
@@ -5164,7 +5159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D44D2B2-1DE7-400D-8C40-2CD59BEE6EC3}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="V3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -5218,10 +5213,10 @@
         <v>438</v>
       </c>
       <c r="I1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="K1" t="s">
         <v>158</v>
@@ -5260,7 +5255,7 @@
         <v>455</v>
       </c>
       <c r="W1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="X1" t="s">
         <v>432</v>
@@ -5292,7 +5287,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>274</v>
@@ -5340,7 +5335,7 @@
         <v>63</v>
       </c>
       <c r="Y2" s="24" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -6390,7 +6385,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B37" s="25">
         <v>44893</v>
@@ -6399,12 +6394,12 @@
         <v>177</v>
       </c>
       <c r="D37" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B38" s="25">
         <v>44903</v>
@@ -6413,12 +6408,12 @@
         <v>177</v>
       </c>
       <c r="D38" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B39" s="25">
         <v>45082</v>
@@ -6427,7 +6422,7 @@
         <v>177</v>
       </c>
       <c r="D39" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -6438,10 +6433,10 @@
         <v>45156</v>
       </c>
       <c r="C40" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D40" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
   </sheetData>
@@ -6502,16 +6497,16 @@
         <v>291</v>
       </c>
       <c r="E1" t="s">
+        <v>474</v>
+      </c>
+      <c r="F1" t="s">
         <v>475</v>
-      </c>
-      <c r="F1" t="s">
-        <v>476</v>
       </c>
       <c r="G1" t="s">
         <v>438</v>
       </c>
       <c r="H1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I1" t="s">
         <v>18</v>
@@ -6553,7 +6548,7 @@
         <v>296</v>
       </c>
       <c r="V1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="W1" t="s">
         <v>182</v>
@@ -6588,7 +6583,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="49" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I2" s="24" t="s">
         <v>4</v>
@@ -6642,7 +6637,7 @@
         <v>63</v>
       </c>
       <c r="Z2" s="24" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -7241,7 +7236,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F1" t="s">
         <v>453</v>
@@ -7253,16 +7248,16 @@
         <v>238</v>
       </c>
       <c r="I1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="J1" t="s">
         <v>361</v>
       </c>
       <c r="K1" t="s">
+        <v>479</v>
+      </c>
+      <c r="L1" t="s">
         <v>480</v>
-      </c>
-      <c r="L1" t="s">
-        <v>481</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -8453,13 +8448,13 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8468,27 +8463,29 @@
     <col min="2" max="2" width="17.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
-    <col min="15" max="15" width="14" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" customWidth="1"/>
-    <col min="19" max="20" width="20.85546875" customWidth="1"/>
-    <col min="21" max="22" width="16.7109375" customWidth="1"/>
-    <col min="23" max="23" width="16.42578125" customWidth="1"/>
-    <col min="24" max="28" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="22" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14" customWidth="1"/>
+    <col min="18" max="18" width="15.140625" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" customWidth="1"/>
+    <col min="21" max="22" width="20.85546875" customWidth="1"/>
+    <col min="23" max="24" width="16.7109375" customWidth="1"/>
+    <col min="25" max="25" width="16.42578125" customWidth="1"/>
+    <col min="26" max="30" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>232</v>
       </c>
@@ -8497,64 +8494,70 @@
         <v>333</v>
       </c>
       <c r="D1" t="s">
+        <v>526</v>
+      </c>
+      <c r="E1" t="s">
+        <v>525</v>
+      </c>
+      <c r="F1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>392</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>362</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>391</v>
       </c>
-      <c r="M1" t="s">
-        <v>469</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>468</v>
+      </c>
+      <c r="P1" t="s">
         <v>37</v>
       </c>
-      <c r="O1" t="s">
-        <v>464</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
+        <v>463</v>
+      </c>
+      <c r="R1" t="s">
         <v>438</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>47</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>51</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>326</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>327</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>336</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -8565,124 +8568,133 @@
         <v>334</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="O2" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>465</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>466</v>
-      </c>
-      <c r="P2" s="24" t="s">
+      <c r="R2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="X2" s="9" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E3">
+      <c r="D3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3">
         <v>10</v>
       </c>
-      <c r="P3" s="47"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="R3" s="47"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>200</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>5000</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>0.6</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>5500</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>303</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>148</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>329</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>40</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -8953,7 +8965,7 @@
         <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I1" t="s">
         <v>46</v>
@@ -8997,7 +9009,7 @@
         <v>36</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>9</v>
@@ -9367,7 +9379,7 @@
         <v>171</v>
       </c>
       <c r="G1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H1" t="s">
         <v>132</v>
@@ -9796,7 +9808,7 @@
         <v>170</v>
       </c>
       <c r="G1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="H1" t="s">
         <v>131</v>
@@ -10024,7 +10036,7 @@
         <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F1" t="s">
         <v>73</v>
@@ -10047,19 +10059,19 @@
         <v>192</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>189</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>507</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>508</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -10779,28 +10791,28 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E1" t="s">
         <v>370</v>
       </c>
       <c r="F1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G1" t="s">
         <v>447</v>
       </c>
       <c r="H1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10814,7 +10826,7 @@
         <v>156</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>369</v>
@@ -10829,34 +10841,34 @@
         <v>444</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K2" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>493</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>495</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>494</v>
-      </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>496</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>497</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>499</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -10867,7 +10879,7 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E3" t="s">
         <v>371</v>
@@ -10890,7 +10902,7 @@
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E4" t="s">
         <v>371</v>
@@ -10913,7 +10925,7 @@
         <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E5" t="s">
         <v>371</v>
@@ -10936,7 +10948,7 @@
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E6" t="s">
         <v>371</v>
@@ -10959,7 +10971,7 @@
         <v>185</v>
       </c>
       <c r="C7" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E7" t="s">
         <v>371</v>
@@ -11033,44 +11045,41 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84972591-1FC8-442A-8908-24ECB9BFD99C}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
-    <col min="10" max="18" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="17" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>232</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1" t="s">
         <v>515</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>516</v>
       </c>
-      <c r="E1" t="s">
-        <v>517</v>
-      </c>
-      <c r="F1" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -11078,17 +11087,15 @@
         <v>74</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>521</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>514</v>
-      </c>
+        <v>513</v>
+      </c>
+      <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
@@ -11100,125 +11107,121 @@
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C3" t="s">
-        <v>99</v>
+      <c r="C3">
+        <v>4800</v>
       </c>
       <c r="D3">
-        <v>4800</v>
+        <v>6780</v>
       </c>
       <c r="E3">
-        <v>6780</v>
-      </c>
-      <c r="F3">
         <v>15000</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="Q3" s="5"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>305</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="Q4" s="5"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>305</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="Q5" s="5"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>305</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="Q6" s="5"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="P6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>305</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="Q7" s="5"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>377</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>377</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>377</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>377</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -11274,7 +11277,7 @@
         <v>193</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
group_output docs and examples
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AETART\Documents\flextool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744E1846-CB7E-487A-8218-0FE9E9D477C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101B3C87-F035-4351-9E32-0B89C628E0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-18120" windowWidth="29040" windowHeight="17640" tabRatio="1000" firstSheet="8" activeTab="10" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="15" yWindow="-18120" windowWidth="29040" windowHeight="17640" tabRatio="1000" firstSheet="35" activeTab="45" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -58,6 +58,7 @@
     <sheet name="node_constraint_c" sheetId="60" r:id="rId43"/>
     <sheet name="unit_constraint_c" sheetId="61" r:id="rId44"/>
     <sheet name="connection_constraint_c" sheetId="62" r:id="rId45"/>
+    <sheet name="optional_outputs" sheetId="64" r:id="rId46"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -206,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="543">
   <si>
     <t>commodity</t>
   </si>
@@ -1787,6 +1788,54 @@
   </si>
   <si>
     <t>Creates the timewise flow output for this node group (group_flow_t)</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>output_connection__node__node_flow_t</t>
+  </si>
+  <si>
+    <t>output_connection_flow_separate</t>
+  </si>
+  <si>
+    <t>output_node_balance_t</t>
+  </si>
+  <si>
+    <t>output_ramp_envelope</t>
+  </si>
+  <si>
+    <t>output_unit__node_flow_t</t>
+  </si>
+  <si>
+    <t>output_unit__node_ramp_t</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The flows between the nodes for each timestep.</t>
+  </si>
+  <si>
+    <t>Produces the connection flows separately for both directions.</t>
+  </si>
+  <si>
+    <t>Produces detailed inflows and outflows for all the nodes for all timesteps. Mainly useful to diagnose what is wrong with the model.</t>
+  </si>
+  <si>
+    <t>Includes seven parameters that form the ramp room envelope (how much there is additional ramping capability in a given node).</t>
+  </si>
+  <si>
+    <t>The flows from units to the nodes for each timestep.</t>
+  </si>
+  <si>
+    <t>Produces the ramps of individual units for all timesteps.</t>
+  </si>
+  <si>
+    <t>optional_outputs</t>
+  </si>
+  <si>
+    <t>Added optional_outputs sheet and the output_aggregate_flows and output_node_flows to the group_c</t>
   </si>
 </sst>
 </file>
@@ -1971,7 +2020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2072,6 +2121,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3537,10 +3589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F991596-B8AE-4F8F-B051-2E61303D5CC8}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3632,273 +3684,281 @@
       <c r="C9" s="43"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="E10" t="s">
+      <c r="A10" s="43" t="s">
+        <v>541</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
+      <c r="E11" t="s">
         <v>235</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B13" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="C12" s="32"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="C13" s="32"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="C14" s="31" t="s">
-        <v>208</v>
-      </c>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
+        <v>225</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="B16" s="32"/>
-      <c r="C16" s="31" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="31" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-    </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="39"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="40" t="s">
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="39"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="40" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="33"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
+      <c r="A22" s="45" t="s">
+        <v>255</v>
+      </c>
+      <c r="B22" s="45"/>
+      <c r="C22" s="45"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="33"/>
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B24" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="28"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
-        <v>212</v>
-      </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
+      <c r="A29" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
         <v>218</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="35" t="s">
+      <c r="B32" s="36"/>
+      <c r="C32" s="35" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="42" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
         <v>220</v>
       </c>
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="48" t="s">
-        <v>210</v>
-      </c>
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
+      <c r="B33" s="42"/>
+      <c r="C33" s="42"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>410</v>
+        <v>211</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B39" s="48"/>
       <c r="C39" s="48"/>
     </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="48" t="s">
+        <v>408</v>
+      </c>
+      <c r="B40" s="48"/>
+      <c r="C40" s="48"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A30" location="reserve_unit_node_c!A1" display="reserve_connection_node_c" xr:uid="{3F855114-4A57-4E0A-A766-0317F980F4BF}"/>
-    <hyperlink ref="A28" location="group_unit_node!A1" display="group_unit_node" xr:uid="{B7C2FCA3-F9B2-4C44-95E7-EE78C953ADDA}"/>
-    <hyperlink ref="A27" location="group_unit!A1" display="group_unit" xr:uid="{B05CA82D-DD0B-41C5-A4A2-737EB6D8AF37}"/>
-    <hyperlink ref="A26" location="group_node!A1" display="group_node" xr:uid="{920BB948-3B7C-488B-B8B1-7504F3D3AD1A}"/>
-    <hyperlink ref="A25" location="group_connection_node!A1" display="group_connection_node" xr:uid="{811FD465-B06B-4481-9ED6-DE1222C0D3DE}"/>
-    <hyperlink ref="A31" location="reserve_group_c!A1" display="reserve_group_c" xr:uid="{2CFA818C-9B6A-474B-8E40-2E804C4A9677}"/>
-    <hyperlink ref="C31" location="reserve_group_t!A1" display="reserve_group_t" xr:uid="{401EE982-2E1A-4DC0-A8C5-8E9B177FDA74}"/>
-    <hyperlink ref="A32" location="reserve_unit_node_c!A1" display="reserve_unit_node_c" xr:uid="{78371C66-B81A-4E9B-96E1-6659A71B0BF4}"/>
-    <hyperlink ref="A24" location="group_connection!A1" display="group_connection" xr:uid="{A00C70C1-5203-41C9-BCBD-CC42FCD43017}"/>
-    <hyperlink ref="A23" location="group_c!A1" display="group_c" xr:uid="{8516B270-11A5-45FE-B8AE-F8BD21CE42EE}"/>
-    <hyperlink ref="B23" location="group_p!A1" display="group_p" xr:uid="{24A5AB85-580D-4C07-9C0C-EF096DF9B6A4}"/>
-    <hyperlink ref="A35" location="unit_node_constraint_c!A1" display="unit_node_constraint_c" xr:uid="{E752EE81-721A-467B-A89A-558EAD27CD18}"/>
-    <hyperlink ref="A34" location="constraint_sense_c!A1" display="constraint_sense_c" xr:uid="{E3638194-ABA1-4B52-B562-9CB1B5A7326A}"/>
-    <hyperlink ref="A16" location="unit_node_c!A1" display="unit_node_c" xr:uid="{588C2786-F4D1-490C-8299-996C761D1B0B}"/>
-    <hyperlink ref="C16" location="unit_node_t!A1" display="unit_node_t" xr:uid="{848C3082-4242-4C02-A2C8-1DDCCECDDCE4}"/>
-    <hyperlink ref="A15" location="unit_c!A1" display="unit_c" xr:uid="{0B24F06D-DF0D-43E9-A754-3D573B0328ED}"/>
-    <hyperlink ref="B15" location="unit_p!A1" display="unit_p" xr:uid="{6B0EC5F5-0D3E-41BB-B4D8-64F5821432A7}"/>
-    <hyperlink ref="C15" location="unit_t!A1" display="unit_t" xr:uid="{563A1A91-8913-4B2F-8BA5-4D350923C03F}"/>
-    <hyperlink ref="C18" location="profile_t!A1" display="profile_t" xr:uid="{78412094-AA9A-4901-935D-64F3C1AC7206}"/>
-    <hyperlink ref="A14" location="connection_c!A1" display="connection_c" xr:uid="{03E6664B-5F07-4921-A88F-1CC8DA8E9FAE}"/>
-    <hyperlink ref="B14" location="connection_p!A1" display="connection_p" xr:uid="{46902093-FDC0-4939-BBFD-2D41FFBE0F05}"/>
-    <hyperlink ref="C14" location="connection_t!A1" display="connection_t" xr:uid="{5D63301C-ED60-425E-8FC0-334B75B4F98C}"/>
-    <hyperlink ref="A13" location="commodity_node!A1" display="commodity_node" xr:uid="{1A8DF925-BFFA-47C2-B595-2F06AACA43EF}"/>
-    <hyperlink ref="A12" location="commodity_c!A1" display="commodity_c" xr:uid="{37D28BB2-4F57-4EDF-A58D-D5D0B0DFCD29}"/>
-    <hyperlink ref="B12" location="commodity_p!A1" display="commodity_p" xr:uid="{B8974311-BDD6-456A-9C22-7DD64599915A}"/>
-    <hyperlink ref="A11" location="node_c!A1" display="node_c" xr:uid="{96541F46-A5D0-46A0-A7C5-61D6136DE6D8}"/>
-    <hyperlink ref="B11" location="node_p!A1" display="node_p" xr:uid="{AA8FF5EE-A7C6-4A42-B219-867295F74C98}"/>
-    <hyperlink ref="C11" location="node_t!A1" display="node_t" xr:uid="{10D2F31E-4A77-4C8D-A909-F30F7DA9A1B0}"/>
+    <hyperlink ref="A31" location="reserve_unit_node_c!A1" display="reserve_connection_node_c" xr:uid="{3F855114-4A57-4E0A-A766-0317F980F4BF}"/>
+    <hyperlink ref="A29" location="group_unit_node!A1" display="group_unit_node" xr:uid="{B7C2FCA3-F9B2-4C44-95E7-EE78C953ADDA}"/>
+    <hyperlink ref="A28" location="group_unit!A1" display="group_unit" xr:uid="{B05CA82D-DD0B-41C5-A4A2-737EB6D8AF37}"/>
+    <hyperlink ref="A27" location="group_node!A1" display="group_node" xr:uid="{920BB948-3B7C-488B-B8B1-7504F3D3AD1A}"/>
+    <hyperlink ref="A26" location="group_connection_node!A1" display="group_connection_node" xr:uid="{811FD465-B06B-4481-9ED6-DE1222C0D3DE}"/>
+    <hyperlink ref="A32" location="reserve_group_c!A1" display="reserve_group_c" xr:uid="{2CFA818C-9B6A-474B-8E40-2E804C4A9677}"/>
+    <hyperlink ref="C32" location="reserve_group_t!A1" display="reserve_group_t" xr:uid="{401EE982-2E1A-4DC0-A8C5-8E9B177FDA74}"/>
+    <hyperlink ref="A33" location="reserve_unit_node_c!A1" display="reserve_unit_node_c" xr:uid="{78371C66-B81A-4E9B-96E1-6659A71B0BF4}"/>
+    <hyperlink ref="A25" location="group_connection!A1" display="group_connection" xr:uid="{A00C70C1-5203-41C9-BCBD-CC42FCD43017}"/>
+    <hyperlink ref="A24" location="group_c!A1" display="group_c" xr:uid="{8516B270-11A5-45FE-B8AE-F8BD21CE42EE}"/>
+    <hyperlink ref="B24" location="group_p!A1" display="group_p" xr:uid="{24A5AB85-580D-4C07-9C0C-EF096DF9B6A4}"/>
+    <hyperlink ref="A36" location="unit_node_constraint_c!A1" display="unit_node_constraint_c" xr:uid="{E752EE81-721A-467B-A89A-558EAD27CD18}"/>
+    <hyperlink ref="A35" location="constraint_sense_c!A1" display="constraint_sense_c" xr:uid="{E3638194-ABA1-4B52-B562-9CB1B5A7326A}"/>
+    <hyperlink ref="A17" location="unit_node_c!A1" display="unit_node_c" xr:uid="{588C2786-F4D1-490C-8299-996C761D1B0B}"/>
+    <hyperlink ref="C17" location="unit_node_t!A1" display="unit_node_t" xr:uid="{848C3082-4242-4C02-A2C8-1DDCCECDDCE4}"/>
+    <hyperlink ref="A16" location="unit_c!A1" display="unit_c" xr:uid="{0B24F06D-DF0D-43E9-A754-3D573B0328ED}"/>
+    <hyperlink ref="B16" location="unit_p!A1" display="unit_p" xr:uid="{6B0EC5F5-0D3E-41BB-B4D8-64F5821432A7}"/>
+    <hyperlink ref="C16" location="unit_t!A1" display="unit_t" xr:uid="{563A1A91-8913-4B2F-8BA5-4D350923C03F}"/>
+    <hyperlink ref="C19" location="profile_t!A1" display="profile_t" xr:uid="{78412094-AA9A-4901-935D-64F3C1AC7206}"/>
+    <hyperlink ref="A15" location="connection_c!A1" display="connection_c" xr:uid="{03E6664B-5F07-4921-A88F-1CC8DA8E9FAE}"/>
+    <hyperlink ref="B15" location="connection_p!A1" display="connection_p" xr:uid="{46902093-FDC0-4939-BBFD-2D41FFBE0F05}"/>
+    <hyperlink ref="C15" location="connection_t!A1" display="connection_t" xr:uid="{5D63301C-ED60-425E-8FC0-334B75B4F98C}"/>
+    <hyperlink ref="A14" location="commodity_node!A1" display="commodity_node" xr:uid="{1A8DF925-BFFA-47C2-B595-2F06AACA43EF}"/>
+    <hyperlink ref="A13" location="commodity_c!A1" display="commodity_c" xr:uid="{37D28BB2-4F57-4EDF-A58D-D5D0B0DFCD29}"/>
+    <hyperlink ref="B13" location="commodity_p!A1" display="commodity_p" xr:uid="{B8974311-BDD6-456A-9C22-7DD64599915A}"/>
+    <hyperlink ref="A12" location="node_c!A1" display="node_c" xr:uid="{96541F46-A5D0-46A0-A7C5-61D6136DE6D8}"/>
+    <hyperlink ref="B12" location="node_p!A1" display="node_p" xr:uid="{AA8FF5EE-A7C6-4A42-B219-867295F74C98}"/>
+    <hyperlink ref="C12" location="node_t!A1" display="node_t" xr:uid="{10D2F31E-4A77-4C8D-A909-F30F7DA9A1B0}"/>
     <hyperlink ref="A8" location="timeblockSet_timeline!A1" display="timeblockSet_timeline" xr:uid="{7E649E3B-8603-412B-85C7-55801419EDEB}"/>
     <hyperlink ref="C7" location="timeline_t!A1" display="timeline_t" xr:uid="{0049663E-A2F9-49A0-A576-07D0A457655D}"/>
     <hyperlink ref="A7" location="timeline_s!A1" display="timeline_s" xr:uid="{252B2493-68D2-4C5E-A6EA-89A71C7FBE09}"/>
     <hyperlink ref="A2" location="version!A1" display="version" xr:uid="{5528FB5D-B49F-4A94-B79B-BD7CACBF6421}"/>
-    <hyperlink ref="A20" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{BFEE1E54-8BED-43DB-81D7-EF22B030644E}"/>
-    <hyperlink ref="A21" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{F130C8C0-C1F9-49C3-9475-FD4618C13C76}"/>
-    <hyperlink ref="A19" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{844403FD-DCCB-46C7-BE3C-C68DCAAB6B04}"/>
-    <hyperlink ref="A19:C19" location="node_profile_c!A1" display="node_profile_c" xr:uid="{826B47E5-87EB-412A-A0AE-C49CDB5CEB93}"/>
-    <hyperlink ref="A20:C20" location="connection_profile_c!A1" display="connection_profile_c" xr:uid="{DB781E38-3ACC-4F21-8D1E-B47D2A016C51}"/>
-    <hyperlink ref="A21:C21" location="unit_node_profile_c!A1" display="unit_profile_c" xr:uid="{B2BA97AF-8BE5-4D5F-8341-41044F5963AA}"/>
+    <hyperlink ref="A21" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{BFEE1E54-8BED-43DB-81D7-EF22B030644E}"/>
+    <hyperlink ref="A22" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{F130C8C0-C1F9-49C3-9475-FD4618C13C76}"/>
+    <hyperlink ref="A20" location="unit_profile_c!A1" display="unit_profile_c" xr:uid="{844403FD-DCCB-46C7-BE3C-C68DCAAB6B04}"/>
+    <hyperlink ref="A20:C20" location="node_profile_c!A1" display="node_profile_c" xr:uid="{826B47E5-87EB-412A-A0AE-C49CDB5CEB93}"/>
+    <hyperlink ref="A21:C21" location="connection_profile_c!A1" display="connection_profile_c" xr:uid="{DB781E38-3ACC-4F21-8D1E-B47D2A016C51}"/>
+    <hyperlink ref="A22:C22" location="unit_node_profile_c!A1" display="unit_profile_c" xr:uid="{B2BA97AF-8BE5-4D5F-8341-41044F5963AA}"/>
     <hyperlink ref="A4" location="solve_period!A1" display="solve_period" xr:uid="{1A642A0E-886B-4C5F-9459-AF06B635D1C8}"/>
     <hyperlink ref="A5" location="solve_sequence!A1" display="solve_sequence" xr:uid="{3B08721C-A5BF-4AD9-9840-41F099D6F77C}"/>
     <hyperlink ref="A6" location="timeblockSet!A1" display="timeblockSet" xr:uid="{4C69C415-5F99-4696-8AE3-CE2F554DC3A9}"/>
     <hyperlink ref="A3" location="scenario!B3" display="scenario" xr:uid="{6595CB33-4050-4638-93A2-B2C50D1ED6D3}"/>
-    <hyperlink ref="A37" location="node_constraint_c!A1" display="node_constraint_c" xr:uid="{AC3AB525-A059-400D-8A88-BB691B8190B0}"/>
-    <hyperlink ref="A38" location="unit_constraint_c!A1" display="unit_constraint_c" xr:uid="{52E2C769-7950-491B-8D4F-A3098C5C0800}"/>
-    <hyperlink ref="A39" location="connection_constraint_c!A1" display="connection_constraint_c" xr:uid="{4F42D9DB-BE6E-4724-A8BC-46902175E215}"/>
-    <hyperlink ref="A36" location="connection_node_constraint_c!A1" display="connection_node_constraint_c" xr:uid="{8884D5A7-21E8-46CA-9DDB-FA2BA31F034A}"/>
+    <hyperlink ref="A38" location="node_constraint_c!A1" display="node_constraint_c" xr:uid="{AC3AB525-A059-400D-8A88-BB691B8190B0}"/>
+    <hyperlink ref="A39" location="unit_constraint_c!A1" display="unit_constraint_c" xr:uid="{52E2C769-7950-491B-8D4F-A3098C5C0800}"/>
+    <hyperlink ref="A40" location="connection_constraint_c!A1" display="connection_constraint_c" xr:uid="{4F42D9DB-BE6E-4724-A8BC-46902175E215}"/>
+    <hyperlink ref="A37" location="connection_node_constraint_c!A1" display="connection_node_constraint_c" xr:uid="{8884D5A7-21E8-46CA-9DDB-FA2BA31F034A}"/>
     <hyperlink ref="A9" location="solve_commands!A1" display="solve_commands" xr:uid="{8D72B1F0-8235-4F44-A670-254B53148E29}"/>
+    <hyperlink ref="A10" location="optional_outputs!A1" display="optional_outputs" xr:uid="{CEBE0D39-4AF1-4C73-8380-3A7E975CFB9C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -3955,7 +4015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -5889,16 +5949,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4446509C-CB62-4FDB-A8D2-BE0D15E8AAF2}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6437,6 +6497,20 @@
       </c>
       <c r="D40" t="s">
         <v>520</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>23</v>
+      </c>
+      <c r="B41" s="25">
+        <v>45282</v>
+      </c>
+      <c r="C41" t="s">
+        <v>519</v>
+      </c>
+      <c r="D41" t="s">
+        <v>542</v>
       </c>
     </row>
   </sheetData>
@@ -10761,6 +10835,121 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9360ADFF-4DA4-424D-81E2-83D3CB4EF97B}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14" style="52" customWidth="1"/>
+    <col min="4" max="4" width="117.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="50"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>527</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="D3" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="D4" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D5" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="D6" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="D7" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" t="s">
+        <v>540</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="navigate!A1" display="navigate" xr:uid="{714DE2DC-5C1E-48BB-85FF-E3051838D903}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9640D032-37A5-47CC-8407-C4F7168BB93B}">
   <dimension ref="A1:R11"/>
@@ -11240,7 +11429,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
load_sharing and db changes
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AETART\Documents\flextool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101B3C87-F035-4351-9E32-0B89C628E0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B70396-CE37-49F7-B85E-98CA1D809995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-18120" windowWidth="29040" windowHeight="17640" tabRatio="1000" firstSheet="35" activeTab="45" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="15" yWindow="-18120" windowWidth="29040" windowHeight="17640" tabRatio="1000" activeTab="28" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="546">
   <si>
     <t>commodity</t>
   </si>
@@ -1836,6 +1836,15 @@
   </si>
   <si>
     <t>Added optional_outputs sheet and the output_aggregate_flows and output_node_flows to the group_c</t>
+  </si>
+  <si>
+    <t>Force the upward slack of the nodes in this group to be equal or inflow (demand) weighted</t>
+  </si>
+  <si>
+    <t>share_loss_of_load</t>
+  </si>
+  <si>
+    <t>inflow_weighted</t>
   </si>
 </sst>
 </file>
@@ -8522,13 +8531,13 @@
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
-  <dimension ref="A1:X7"/>
+  <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8559,7 +8568,7 @@
     <col min="26" max="30" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>232</v>
       </c>
@@ -8630,8 +8639,11 @@
       <c r="X1" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -8704,8 +8716,11 @@
       <c r="X2" s="9" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y2" s="9" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -8720,7 +8735,7 @@
       </c>
       <c r="R3" s="47"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -8740,7 +8755,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>303</v>
       </c>
@@ -8754,7 +8769,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>329</v>
       </c>
@@ -8768,7 +8783,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>27</v>
       </c>
@@ -8777,6 +8792,9 @@
       </c>
       <c r="C7" t="s">
         <v>148</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>545</v>
       </c>
     </row>
   </sheetData>
@@ -10839,7 +10857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9360ADFF-4DA4-424D-81E2-83D3CB4EF97B}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
entity alternative for new db
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AETART\Documents\flextool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B70396-CE37-49F7-B85E-98CA1D809995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB93A695-3C01-497C-8355-492643BFADA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-18120" windowWidth="29040" windowHeight="17640" tabRatio="1000" activeTab="28" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="28815" yWindow="-18120" windowWidth="29040" windowHeight="17640" tabRatio="1000" firstSheet="2" activeTab="2" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1482" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="542">
   <si>
     <t>commodity</t>
   </si>
@@ -719,12 +719,6 @@
     <t>A flag whether has a state variable (storage). If empty, then not true. Use 'yes' to indicate true.</t>
   </si>
   <si>
-    <t>Can the unit provide this reserve. Empty indicates not allowed. Use 'yes' to indicate true.</t>
-  </si>
-  <si>
-    <t>Can the connection provide this reserve. Empty indicates not allowed. Use 'yes' to indicate true.</t>
-  </si>
-  <si>
     <t>Map of timestep durations. Index: timestep name, value: duration of time step [in hours].</t>
   </si>
   <si>
@@ -1043,9 +1037,6 @@
     <t>Whether the unit is present in the alternative.</t>
   </si>
   <si>
-    <t>Whether the node is present in the alternative.</t>
-  </si>
-  <si>
     <t>Battery</t>
   </si>
   <si>
@@ -1104,9 +1095,6 @@
   </si>
   <si>
     <t>Added 'efficiency_at_min_load' and 'min_load' to unit_t sheet.</t>
-  </si>
-  <si>
-    <t>Whether the constraint is active.</t>
   </si>
   <si>
     <t>9.2</t>
@@ -3095,7 +3083,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>34</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -3613,88 +3601,88 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>265</v>
       </c>
-      <c r="B1" s="46" t="s">
-        <v>267</v>
-      </c>
       <c r="C1" s="46" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="43" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="43" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B4" s="43"/>
       <c r="C4" s="43"/>
       <c r="E4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="43" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="E5" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B6" s="43"/>
       <c r="C6" s="43"/>
       <c r="E6" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="43" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B8" s="43"/>
       <c r="C8" s="43"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="43"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="43" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B10" s="43"/>
       <c r="C10" s="43"/>
@@ -3704,65 +3692,65 @@
       <c r="B11" s="27"/>
       <c r="C11" s="27"/>
       <c r="E11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="31" t="s">
         <v>200</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C13" s="32"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B14" s="44"/>
       <c r="C14" s="44"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" s="31" t="s">
         <v>206</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
+        <v>223</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>224</v>
+      </c>
+      <c r="C16" s="31" t="s">
         <v>225</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>226</v>
-      </c>
-      <c r="C16" s="31" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B17" s="32"/>
       <c r="C17" s="31" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3774,26 +3762,26 @@
       <c r="A19" s="39"/>
       <c r="B19" s="39"/>
       <c r="C19" s="40" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
@@ -3805,45 +3793,45 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="28"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B25" s="41"/>
       <c r="C25" s="41"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B26" s="41"/>
       <c r="C26" s="41"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="41"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B28" s="41"/>
       <c r="C28" s="41"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B29" s="41"/>
       <c r="C29" s="41"/>
@@ -3855,65 +3843,65 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B32" s="36"/>
       <c r="C32" s="35" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="42"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B39" s="48"/>
       <c r="C39" s="48"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B40" s="48"/>
       <c r="C40" s="48"/>
@@ -3992,7 +3980,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>101</v>
@@ -4022,255 +4010,248 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
-  <dimension ref="A1:AH9"/>
+  <dimension ref="A1:AG9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" customWidth="1"/>
-    <col min="12" max="12" width="29.28515625" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" customWidth="1"/>
-    <col min="14" max="14" width="12" customWidth="1"/>
-    <col min="15" max="15" width="10.42578125" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" customWidth="1"/>
-    <col min="21" max="21" width="10.140625" style="14" customWidth="1"/>
-    <col min="22" max="22" width="9.85546875" style="14" customWidth="1"/>
-    <col min="23" max="23" width="10.85546875" style="14" customWidth="1"/>
-    <col min="24" max="24" width="13.42578125" customWidth="1"/>
-    <col min="25" max="25" width="12.7109375" style="14" customWidth="1"/>
-    <col min="26" max="26" width="10.5703125" customWidth="1"/>
-    <col min="27" max="27" width="8.140625" customWidth="1"/>
-    <col min="28" max="29" width="18.140625" customWidth="1"/>
-    <col min="30" max="30" width="16.85546875" customWidth="1"/>
-    <col min="31" max="32" width="29.140625" customWidth="1"/>
-    <col min="33" max="33" width="14.7109375" customWidth="1"/>
-    <col min="34" max="34" width="10" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="10" max="10" width="25.140625" customWidth="1"/>
+    <col min="11" max="11" width="29.28515625" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" customWidth="1"/>
+    <col min="18" max="18" width="10.5703125" customWidth="1"/>
+    <col min="19" max="19" width="10.28515625" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" style="14" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" style="14" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" style="14" customWidth="1"/>
+    <col min="23" max="23" width="13.42578125" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" style="14" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" customWidth="1"/>
+    <col min="26" max="26" width="8.140625" customWidth="1"/>
+    <col min="27" max="28" width="18.140625" customWidth="1"/>
+    <col min="29" max="29" width="16.85546875" customWidth="1"/>
+    <col min="30" max="31" width="29.140625" customWidth="1"/>
+    <col min="32" max="32" width="14.7109375" customWidth="1"/>
+    <col min="33" max="33" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>278</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
-        <v>168</v>
+        <v>467</v>
       </c>
       <c r="E1" t="s">
-        <v>471</v>
+        <v>169</v>
       </c>
       <c r="F1" t="s">
-        <v>169</v>
+        <v>468</v>
       </c>
       <c r="G1" t="s">
-        <v>472</v>
+        <v>501</v>
       </c>
       <c r="H1" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="I1" t="s">
-        <v>512</v>
+        <v>432</v>
       </c>
       <c r="J1" t="s">
-        <v>436</v>
-      </c>
-      <c r="K1" t="s">
-        <v>427</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>419</v>
+        <v>423</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="L1" t="s">
+        <v>157</v>
       </c>
       <c r="M1" t="s">
-        <v>157</v>
+        <v>452</v>
       </c>
       <c r="N1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="O1" t="s">
-        <v>457</v>
+        <v>342</v>
       </c>
       <c r="P1" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" t="s">
+        <v>279</v>
+      </c>
+      <c r="T1" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" t="s">
+        <v>280</v>
+      </c>
+      <c r="V1" t="s">
+        <v>344</v>
+      </c>
+      <c r="W1" t="s">
+        <v>345</v>
+      </c>
+      <c r="X1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" t="s">
         <v>346</v>
       </c>
-      <c r="Q1" t="s">
-        <v>347</v>
-      </c>
-      <c r="R1" t="s">
-        <v>65</v>
-      </c>
-      <c r="S1" t="s">
-        <v>68</v>
-      </c>
-      <c r="T1" t="s">
-        <v>282</v>
-      </c>
-      <c r="U1" t="s">
-        <v>69</v>
-      </c>
-      <c r="V1" t="s">
-        <v>283</v>
-      </c>
-      <c r="W1" t="s">
-        <v>348</v>
-      </c>
-      <c r="X1" t="s">
-        <v>349</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>19</v>
-      </c>
       <c r="Z1" t="s">
-        <v>350</v>
+        <v>22</v>
       </c>
       <c r="AA1" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="AB1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>413</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>415</v>
+        <v>409</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>412</v>
       </c>
       <c r="AE1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="AF1" t="s">
-        <v>422</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>280</v>
+      <c r="C2" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>58</v>
+        <v>246</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>248</v>
+        <v>424</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>428</v>
+        <v>11</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>11</v>
+        <v>500</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>504</v>
+        <v>517</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>521</v>
+        <v>407</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="K2" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="W2" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>416</v>
+      </c>
+      <c r="AE2" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>418</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>458</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="V2" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="W2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="X2" s="24" t="s">
-        <v>236</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z2" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AB2" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>412</v>
-      </c>
-      <c r="AD2" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="AE2" s="9" t="s">
-        <v>420</v>
-      </c>
       <c r="AF2" s="9" t="s">
-        <v>421</v>
+        <v>63</v>
       </c>
       <c r="AG2" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -4280,22 +4261,19 @@
       <c r="C3" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>148</v>
-      </c>
+      <c r="D3" s="14"/>
       <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" t="s">
+      <c r="F3" t="s">
         <v>137</v>
+      </c>
+      <c r="O3">
+        <v>10000</v>
       </c>
       <c r="P3">
         <v>10000</v>
       </c>
-      <c r="Q3">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -4306,174 +4284,159 @@
         <v>148</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>379</v>
-      </c>
-      <c r="F4" s="14"/>
-      <c r="G4" t="s">
+        <v>375</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" t="s">
         <v>137</v>
       </c>
-      <c r="N4">
+      <c r="M4">
         <f>100*8760</f>
         <v>876000</v>
       </c>
+      <c r="O4">
+        <v>10000</v>
+      </c>
       <c r="P4">
         <v>10000</v>
       </c>
-      <c r="Q4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F5" t="s">
         <v>137</v>
+      </c>
+      <c r="O5">
+        <v>10000</v>
       </c>
       <c r="P5">
         <v>10000</v>
       </c>
-      <c r="Q5">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F6" t="s">
         <v>137</v>
+      </c>
+      <c r="O6">
+        <v>10000</v>
       </c>
       <c r="P6">
         <v>10000</v>
       </c>
-      <c r="Q6">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C7" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="C7" t="s">
         <v>148</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>148</v>
       </c>
       <c r="F7" t="s">
-        <v>148</v>
-      </c>
-      <c r="G7" t="s">
         <v>137</v>
       </c>
+      <c r="I7" t="s">
+        <v>422</v>
+      </c>
       <c r="J7" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="K7" t="s">
-        <v>423</v>
-      </c>
-      <c r="L7" t="s">
-        <v>424</v>
+        <v>420</v>
+      </c>
+      <c r="O7">
+        <v>12000</v>
       </c>
       <c r="P7">
         <v>12000</v>
       </c>
       <c r="Q7">
+        <v>20</v>
+      </c>
+      <c r="AA7">
+        <v>0.01</v>
+      </c>
+      <c r="AB7">
+        <v>0.1</v>
+      </c>
+      <c r="AD7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F8" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" t="s">
+        <v>446</v>
+      </c>
+      <c r="J8" t="s">
+        <v>419</v>
+      </c>
+      <c r="O8">
         <v>12000</v>
-      </c>
-      <c r="R7">
-        <v>20</v>
-      </c>
-      <c r="AB7">
-        <v>0.01</v>
-      </c>
-      <c r="AC7">
-        <v>0.1</v>
-      </c>
-      <c r="AE7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D8" t="s">
-        <v>148</v>
-      </c>
-      <c r="F8" t="s">
-        <v>148</v>
-      </c>
-      <c r="G8" t="s">
-        <v>137</v>
-      </c>
-      <c r="J8" t="s">
-        <v>450</v>
-      </c>
-      <c r="K8" t="s">
-        <v>423</v>
       </c>
       <c r="P8">
         <v>12000</v>
       </c>
       <c r="Q8">
-        <v>12000</v>
-      </c>
-      <c r="R8">
         <v>10000000</v>
       </c>
-      <c r="AC8">
+      <c r="AB8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="G9" t="s">
-        <v>437</v>
-      </c>
-      <c r="S9">
+        <v>255</v>
+      </c>
+      <c r="F9" t="s">
+        <v>433</v>
+      </c>
+      <c r="R9">
         <v>800</v>
       </c>
-      <c r="W9" s="14">
+      <c r="V9" s="14">
         <v>200</v>
       </c>
-      <c r="Y9" s="14">
+      <c r="X9" s="14">
         <v>0.05</v>
       </c>
-      <c r="AA9">
+      <c r="Z9">
         <v>10</v>
       </c>
-      <c r="AG9">
+      <c r="AF9">
         <v>1</v>
       </c>
     </row>
@@ -4516,7 +4479,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -4524,7 +4487,7 @@
         <v>64</v>
       </c>
       <c r="E1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="F1" t="s">
         <v>66</v>
@@ -4533,19 +4496,19 @@
         <v>67</v>
       </c>
       <c r="H1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="I1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="J1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="K1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="L1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
@@ -4554,7 +4517,7 @@
         <v>22</v>
       </c>
       <c r="O1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4571,7 +4534,7 @@
         <v>57</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>8</v>
@@ -4586,13 +4549,13 @@
         <v>13</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>6</v>
@@ -4648,7 +4611,7 @@
         <v>138</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <f>250*8760*1.1</f>
@@ -4674,7 +4637,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4687,7 +4650,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5020,14 +4983,14 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1"/>
       <c r="C1" t="s">
         <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5098,12 +5061,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5156,7 +5119,7 @@
         <v>150</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <v>22</v>
@@ -5232,7 +5195,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="V3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y5" sqref="Y5"/>
+      <selection pane="bottomRight" activeCell="AJ19" sqref="AJ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5264,13 +5227,13 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F1" t="s">
         <v>166</v>
@@ -5279,13 +5242,13 @@
         <v>167</v>
       </c>
       <c r="H1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="I1" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="J1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="K1" t="s">
         <v>158</v>
@@ -5297,19 +5260,19 @@
         <v>21</v>
       </c>
       <c r="N1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="O1" t="s">
         <v>24</v>
       </c>
       <c r="P1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="Q1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="R1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="S1" t="s">
         <v>19</v>
@@ -5318,16 +5281,16 @@
         <v>22</v>
       </c>
       <c r="U1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="V1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="W1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="X1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -5338,13 +5301,13 @@
         <v>25</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -5356,10 +5319,10 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>15</v>
@@ -5377,13 +5340,13 @@
         <v>14</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="S2" s="9" t="s">
         <v>6</v>
@@ -5395,7 +5358,7 @@
         <v>5</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>3</v>
@@ -5404,7 +5367,7 @@
         <v>63</v>
       </c>
       <c r="Y2" s="24" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -5441,16 +5404,16 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E4" t="s">
         <v>148</v>
@@ -5476,7 +5439,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>30</v>
@@ -5488,7 +5451,7 @@
         <v>139</v>
       </c>
       <c r="H5" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="M5">
         <v>100</v>
@@ -5508,19 +5471,19 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H6" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="M6">
         <v>100</v>
@@ -5577,7 +5540,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -5585,19 +5548,19 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F1" t="s">
         <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="I1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="J1" t="s">
         <v>19</v>
@@ -5606,10 +5569,10 @@
         <v>22</v>
       </c>
       <c r="L1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="M1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -5632,13 +5595,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -5650,7 +5613,7 @@
         <v>5</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -5689,7 +5652,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <v>150</v>
@@ -5724,7 +5687,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -5973,525 +5936,525 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" t="s">
         <v>173</v>
       </c>
-      <c r="B3" t="s">
-        <v>175</v>
-      </c>
       <c r="C3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" t="s">
         <v>176</v>
-      </c>
-      <c r="D3" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B4" s="25">
         <v>44594</v>
       </c>
       <c r="C4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" t="s">
         <v>177</v>
-      </c>
-      <c r="D4" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B5" s="25">
         <v>44595</v>
       </c>
       <c r="C5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B6" s="25">
         <v>44600</v>
       </c>
       <c r="C6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B7" s="25">
         <v>44602</v>
       </c>
       <c r="C7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B8" s="25">
         <v>44602</v>
       </c>
       <c r="C8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B9" s="25">
         <v>44602</v>
       </c>
       <c r="C9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B10" s="25">
         <v>44602</v>
       </c>
       <c r="C10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B11" s="25">
         <v>44603</v>
       </c>
       <c r="C11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B12" s="25">
         <v>44605</v>
       </c>
       <c r="C12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D12" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B13" s="25">
         <v>44605</v>
       </c>
       <c r="C13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D13" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B14" s="25">
         <v>44605</v>
       </c>
       <c r="C14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B15" s="25">
         <v>44635</v>
       </c>
       <c r="C15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
       </c>
       <c r="C16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D16" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
       </c>
       <c r="C17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D17" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
       </c>
       <c r="C18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D18" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
       </c>
       <c r="C19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D19" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
       </c>
       <c r="C20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D20" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
       </c>
       <c r="C21" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D21" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
       </c>
       <c r="C22" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D22" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
       </c>
       <c r="C23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D23" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
       </c>
       <c r="C24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D24" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
       </c>
       <c r="C25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D25" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
       </c>
       <c r="C26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D26" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B27" s="25">
         <v>44701</v>
       </c>
       <c r="C27" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D27" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B28" s="25">
         <v>44712</v>
       </c>
       <c r="C28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D28" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B29" s="25">
         <v>44727</v>
       </c>
       <c r="C29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D29" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B30" s="25">
         <v>44734</v>
       </c>
       <c r="C30" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D30" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B31" s="25">
         <v>44741</v>
       </c>
       <c r="C31" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D31" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B32" s="25">
         <v>44840</v>
       </c>
       <c r="C32" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D32" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B33" s="25">
         <v>44850</v>
       </c>
       <c r="C33" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D33" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B34" s="25">
         <v>44875</v>
       </c>
       <c r="C34" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D34" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B35" s="25">
         <v>44876</v>
       </c>
       <c r="C35" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D35" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B36" s="25">
         <v>44889</v>
       </c>
       <c r="C36" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D36" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B37" s="25">
         <v>44893</v>
       </c>
       <c r="C37" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D37" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B38" s="25">
         <v>44903</v>
       </c>
       <c r="C38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D38" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B39" s="25">
         <v>45082</v>
       </c>
       <c r="C39" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D39" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -6502,10 +6465,10 @@
         <v>45156</v>
       </c>
       <c r="C40" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D40" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -6516,10 +6479,10 @@
         <v>45282</v>
       </c>
       <c r="C41" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D41" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
   </sheetData>
@@ -6570,26 +6533,26 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="F1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="G1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="H1" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="I1" t="s">
         <v>18</v>
@@ -6598,19 +6561,19 @@
         <v>21</v>
       </c>
       <c r="K1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="L1" t="s">
         <v>24</v>
       </c>
       <c r="M1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="N1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="O1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="P1" t="s">
         <v>19</v>
@@ -6619,7 +6582,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="S1" t="s">
         <v>158</v>
@@ -6628,19 +6591,19 @@
         <v>106</v>
       </c>
       <c r="U1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="V1" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="W1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="X1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Y1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6651,7 +6614,7 @@
         <v>117</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>105</v>
@@ -6666,7 +6629,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="49" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="I2" s="24" t="s">
         <v>4</v>
@@ -6681,13 +6644,13 @@
         <v>14</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="N2" s="24" t="s">
         <v>7</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="P2" s="24" t="s">
         <v>6</v>
@@ -6720,7 +6683,7 @@
         <v>63</v>
       </c>
       <c r="Z2" s="24" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -6734,7 +6697,7 @@
         <v>148</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E3" s="47" t="s">
         <v>160</v>
@@ -6775,7 +6738,7 @@
         <v>148</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E4" s="47" t="s">
         <v>160</v>
@@ -6806,10 +6769,10 @@
         <v>148</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
@@ -6828,28 +6791,28 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>141</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="H6" s="47"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C7" s="47" t="s">
         <v>148</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E7" s="47" t="s">
         <v>160</v>
@@ -6903,7 +6866,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -6911,19 +6874,19 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F1" t="s">
         <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="I1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="J1" t="s">
         <v>19</v>
@@ -6932,7 +6895,7 @@
         <v>22</v>
       </c>
       <c r="L1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="M1" t="s">
         <v>158</v>
@@ -6958,13 +6921,13 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>6</v>
@@ -7015,7 +6978,7 @@
         <v>141</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D5">
         <v>75</v>
@@ -7050,7 +7013,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -7313,34 +7276,34 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="G1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="H1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="J1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="K1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="L1" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -7357,16 +7320,16 @@
         <v>56</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>108</v>
@@ -7398,7 +7361,7 @@
         <v>140</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -7421,7 +7384,7 @@
         <v>138</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -7441,7 +7404,7 @@
         <v>149</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -7458,7 +7421,7 @@
         <v>139</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -7478,7 +7441,7 @@
         <v>138</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -7489,16 +7452,16 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>149</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -7506,16 +7469,16 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -7523,16 +7486,16 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -7567,7 +7530,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -7582,7 +7545,7 @@
         <v>161</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7608,10 +7571,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7851,7 +7814,7 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7865,13 +7828,13 @@
         <v>136</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -8310,12 +8273,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -8343,10 +8306,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D3" t="s">
         <v>163</v>
@@ -8382,12 +8345,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -8418,7 +8381,7 @@
         <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D3" t="s">
         <v>163</v>
@@ -8455,13 +8418,13 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -8509,16 +8472,16 @@
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E4" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>
@@ -8533,7 +8496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17A58EF0-B113-4E3B-A099-AB516EC20AF0}">
   <dimension ref="A1:Y7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -8570,17 +8533,17 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="D1" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E1" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="F1" t="s">
         <v>39</v>
@@ -8589,7 +8552,7 @@
         <v>35</v>
       </c>
       <c r="H1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="I1" t="s">
         <v>41</v>
@@ -8598,7 +8561,7 @@
         <v>45</v>
       </c>
       <c r="K1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="L1" t="s">
         <v>43</v>
@@ -8607,19 +8570,19 @@
         <v>53</v>
       </c>
       <c r="N1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="O1" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="P1" t="s">
         <v>37</v>
       </c>
       <c r="Q1" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="R1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="S1" t="s">
         <v>47</v>
@@ -8628,19 +8591,19 @@
         <v>51</v>
       </c>
       <c r="U1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="V1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="W1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="X1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="Y1" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -8651,13 +8614,13 @@
         <v>55</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>38</v>
@@ -8666,7 +8629,7 @@
         <v>34</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>40</v>
@@ -8684,16 +8647,16 @@
         <v>52</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>36</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="R2" s="24" t="s">
         <v>11</v>
@@ -8705,19 +8668,19 @@
         <v>50</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="W2" s="9" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="X2" s="9" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="Y2" s="9" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -8740,7 +8703,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J4">
         <v>200</v>
@@ -8757,10 +8720,10 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I5" t="s">
         <v>148</v>
@@ -8771,10 +8734,10 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="U6">
         <v>40</v>
@@ -8788,13 +8751,13 @@
         <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C7" t="s">
         <v>148</v>
       </c>
       <c r="Y7" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -8809,11 +8772,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6AC2C8-7B82-4BFA-94A3-ECFAF63F0D5D}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8824,10 +8787,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8836,42 +8799,42 @@
         <v>27</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="L2" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>376</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>27</v>
@@ -8912,94 +8875,94 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="G4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H4" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="I4" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="J4" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K4" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="L4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="M4" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="J5" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="K5" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="L5" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -9040,7 +9003,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -9057,7 +9020,7 @@
         <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="I1" t="s">
         <v>46</v>
@@ -9066,16 +9029,16 @@
         <v>49</v>
       </c>
       <c r="K1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="L1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="M1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="N1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -9101,7 +9064,7 @@
         <v>36</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>9</v>
@@ -9110,16 +9073,16 @@
         <v>48</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -9158,7 +9121,7 @@
         <v>144</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G5">
         <v>20</v>
@@ -9303,7 +9266,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>138</v>
@@ -9311,7 +9274,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>138</v>
@@ -9319,7 +9282,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>139</v>
@@ -9407,7 +9370,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>141</v>
@@ -9418,7 +9381,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>151</v>
@@ -9437,13 +9400,13 @@
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB87FF22-BB83-4D5E-B38D-455D581CF757}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9453,43 +9416,39 @@
     <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="11" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="13" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="13" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="12" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>171</v>
+        <v>479</v>
       </c>
       <c r="G1" t="s">
-        <v>483</v>
+        <v>132</v>
       </c>
       <c r="H1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J1" t="s">
         <v>126</v>
       </c>
+      <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -9506,36 +9465,33 @@
         <v>56</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>280</v>
+        <v>121</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="J2" s="9" t="s">
         <v>125</v>
       </c>
+      <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>30</v>
@@ -9543,13 +9499,10 @@
       <c r="E3" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="F3" t="s">
-        <v>148</v>
+      <c r="H3">
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
         <v>1</v>
       </c>
     </row>
@@ -9587,22 +9540,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F1" t="s">
         <v>129</v>
       </c>
       <c r="G1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -9645,19 +9598,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" t="s">
         <v>268</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="E3" t="s">
-        <v>270</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -9698,7 +9651,7 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -9865,13 +9818,13 @@
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C0D5E-7DB2-4BCF-8A8C-24C978AAECC4}">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9881,44 +9834,40 @@
     <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="11" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="13" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1"/>
-    <col min="10" max="13" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="12" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>170</v>
+        <v>480</v>
       </c>
       <c r="G1" t="s">
-        <v>484</v>
+        <v>131</v>
       </c>
       <c r="H1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="I1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J1" t="s">
         <v>126</v>
       </c>
+      <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -9935,36 +9884,33 @@
         <v>56</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>280</v>
+        <v>121</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="J2" s="9" t="s">
         <v>125</v>
       </c>
+      <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>141</v>
@@ -9972,25 +9918,22 @@
       <c r="E3" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="F3" t="s">
-        <v>148</v>
+      <c r="H3">
+        <v>0.5</v>
       </c>
       <c r="I3">
-        <v>0.5</v>
-      </c>
-      <c r="J3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>142</v>
@@ -9998,25 +9941,22 @@
       <c r="E4" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="F4" t="s">
-        <v>148</v>
+      <c r="H4">
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>141</v>
@@ -10024,25 +9964,22 @@
       <c r="E5" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="F5" t="s">
-        <v>148</v>
+      <c r="H5">
+        <v>0.01</v>
       </c>
       <c r="I5">
-        <v>0.01</v>
-      </c>
-      <c r="J5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>151</v>
@@ -10050,25 +9987,22 @@
       <c r="E6" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="F6" t="s">
-        <v>148</v>
+      <c r="H6">
+        <v>0.5</v>
       </c>
       <c r="I6">
-        <v>0.5</v>
-      </c>
-      <c r="J6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>141</v>
@@ -10076,13 +10010,10 @@
       <c r="E7" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="F7" t="s">
-        <v>148</v>
+      <c r="H7">
+        <v>0.01</v>
       </c>
       <c r="I7">
-        <v>0.01</v>
-      </c>
-      <c r="J7">
         <v>1</v>
       </c>
     </row>
@@ -10120,7 +10051,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -10128,7 +10059,7 @@
         <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="F1" t="s">
         <v>73</v>
@@ -10148,22 +10079,22 @@
         <v>31</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -10211,7 +10142,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
@@ -10231,7 +10162,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>32</v>
@@ -10251,7 +10182,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>152</v>
@@ -10271,7 +10202,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>33</v>
@@ -10291,13 +10222,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D9" t="s">
         <v>155</v>
@@ -10311,10 +10242,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>76</v>
@@ -10345,13 +10276,13 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C017E3-B844-46CF-8B82-D76F5D9D7ACD}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10359,29 +10290,26 @@
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
-    <col min="4" max="9" width="11.5703125" customWidth="1"/>
+    <col min="4" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E1" t="s">
         <v>147</v>
       </c>
+      <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -10392,19 +10320,16 @@
         <v>145</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="E2" s="9" t="s">
         <v>146</v>
       </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -10414,44 +10339,35 @@
       <c r="C3" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="D3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E3">
+      <c r="D3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="D4" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4">
+        <v>379</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="D5" t="s">
-        <v>148</v>
-      </c>
-      <c r="E5">
+        <v>379</v>
+      </c>
+      <c r="D5">
         <v>0</v>
       </c>
     </row>
@@ -10487,14 +10403,14 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" s="3"/>
       <c r="E1"/>
       <c r="F1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -10508,13 +10424,13 @@
         <v>56</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>134</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -10528,7 +10444,7 @@
         <v>140</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>164</v>
@@ -10548,7 +10464,7 @@
         <v>138</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>164</v>
@@ -10559,19 +10475,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>149</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -10579,19 +10495,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -10628,13 +10544,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10651,7 +10567,7 @@
         <v>134</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -10685,15 +10601,15 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="E1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10707,21 +10623,21 @@
         <v>134</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -10757,12 +10673,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10776,7 +10692,7 @@
         <v>134</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -10809,12 +10725,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10828,18 +10744,18 @@
         <v>134</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D3">
         <v>-8</v>
@@ -10871,7 +10787,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="50"/>
@@ -10881,13 +10797,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10895,10 +10811,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="D3" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -10906,10 +10822,10 @@
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="D4" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -10917,10 +10833,10 @@
         <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="D5" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -10928,10 +10844,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D6" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -10939,10 +10855,10 @@
         <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="D7" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -10950,13 +10866,13 @@
         <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>148</v>
       </c>
       <c r="D8" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -10994,32 +10910,32 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D1" t="s">
+        <v>505</v>
+      </c>
+      <c r="E1" t="s">
+        <v>366</v>
+      </c>
+      <c r="F1" t="s">
+        <v>465</v>
+      </c>
+      <c r="G1" t="s">
+        <v>443</v>
+      </c>
+      <c r="H1" t="s">
+        <v>466</v>
+      </c>
+      <c r="I1" t="s">
+        <v>485</v>
+      </c>
+      <c r="J1" t="s">
         <v>487</v>
-      </c>
-      <c r="D1" t="s">
-        <v>509</v>
-      </c>
-      <c r="E1" t="s">
-        <v>370</v>
-      </c>
-      <c r="F1" t="s">
-        <v>469</v>
-      </c>
-      <c r="G1" t="s">
-        <v>447</v>
-      </c>
-      <c r="H1" t="s">
-        <v>470</v>
-      </c>
-      <c r="I1" t="s">
-        <v>489</v>
-      </c>
-      <c r="J1" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -11033,49 +10949,49 @@
         <v>156</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="I2" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="K2" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="M2" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="O2" s="9" t="s">
         <v>492</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="P2" s="9" t="s">
+        <v>493</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>494</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>493</v>
-      </c>
-      <c r="N2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>495</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>496</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>497</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>498</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -11086,158 +11002,158 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="E3" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F3" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="H3" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="E4" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F4" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="H4" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="E5" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F5" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="H5" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="E6" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F6" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="H6" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="E7" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F7" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="H7" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E9" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E11" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="G11" s="5"/>
     </row>
@@ -11273,17 +11189,17 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D1" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="E1" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -11294,13 +11210,13 @@
         <v>74</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -11340,7 +11256,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>32</v>
@@ -11354,7 +11270,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>152</v>
@@ -11368,7 +11284,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>33</v>
@@ -11382,10 +11298,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F7" s="5"/>
       <c r="H7" s="5"/>
@@ -11396,7 +11312,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>32</v>
@@ -11405,7 +11321,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>152</v>
@@ -11414,7 +11330,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>33</v>
@@ -11423,10 +11339,10 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -11462,7 +11378,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -11475,16 +11391,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>78</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -11546,12 +11462,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -11562,10 +11478,10 @@
         <v>101</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -11937,7 +11853,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">

</xml_diff>

<commit_message>
0.8 change related fixes
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AETART\Documents\flextool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB93A695-3C01-497C-8355-492643BFADA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3666B95-CED2-4B47-8BC1-83CA851AFFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28815" yWindow="-18120" windowWidth="29040" windowHeight="17640" tabRatio="1000" firstSheet="2" activeTab="2" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" activeTab="10" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="542">
   <si>
     <t>commodity</t>
   </si>
@@ -3083,7 +3083,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>33</xdr:col>
+      <xdr:col>34</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -4010,51 +4010,51 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" customWidth="1"/>
-    <col min="11" max="11" width="29.28515625" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" customWidth="1"/>
-    <col min="13" max="13" width="12" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" customWidth="1"/>
-    <col min="20" max="20" width="10.140625" style="14" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" style="14" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" style="14" customWidth="1"/>
-    <col min="23" max="23" width="13.42578125" customWidth="1"/>
-    <col min="24" max="24" width="12.7109375" style="14" customWidth="1"/>
-    <col min="25" max="25" width="10.5703125" customWidth="1"/>
-    <col min="26" max="26" width="8.140625" customWidth="1"/>
-    <col min="27" max="28" width="18.140625" customWidth="1"/>
-    <col min="29" max="29" width="16.85546875" customWidth="1"/>
-    <col min="30" max="31" width="29.140625" customWidth="1"/>
-    <col min="32" max="32" width="14.7109375" customWidth="1"/>
-    <col min="33" max="33" width="10" customWidth="1"/>
+    <col min="3" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1"/>
+    <col min="11" max="11" width="25.140625" customWidth="1"/>
+    <col min="12" max="12" width="29.28515625" customWidth="1"/>
+    <col min="13" max="13" width="7.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" style="14" customWidth="1"/>
+    <col min="22" max="22" width="9.85546875" style="14" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" style="14" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="14" customWidth="1"/>
+    <col min="26" max="26" width="10.5703125" customWidth="1"/>
+    <col min="27" max="27" width="8.140625" customWidth="1"/>
+    <col min="28" max="29" width="18.140625" customWidth="1"/>
+    <col min="30" max="30" width="16.85546875" customWidth="1"/>
+    <col min="31" max="32" width="29.140625" customWidth="1"/>
+    <col min="33" max="33" width="14.7109375" customWidth="1"/>
+    <col min="34" max="34" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>230</v>
       </c>
@@ -4062,95 +4062,95 @@
       <c r="C1" t="s">
         <v>168</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>467</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>169</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>468</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>501</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>508</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>432</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>423</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>157</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>452</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>453</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>342</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>343</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>65</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>68</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>279</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>69</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>280</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>344</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>345</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>346</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>70</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>409</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>411</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>412</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>418</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -4161,97 +4161,100 @@
         <v>58</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>500</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>517</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="W2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="24" t="s">
+      <c r="X2" s="24" t="s">
         <v>234</v>
       </c>
-      <c r="X2" s="9" t="s">
+      <c r="Y2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Z2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="AA2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="9" t="s">
+      <c r="AB2" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AB2" s="9" t="s">
+      <c r="AC2" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AD2" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AE2" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="AE2" s="9" t="s">
+      <c r="AF2" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AG2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="AG2" s="9" t="s">
+      <c r="AH2" s="9" t="s">
         <v>518</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -4261,19 +4264,22 @@
       <c r="C3" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="14" t="s">
+        <v>148</v>
+      </c>
       <c r="E3" s="14"/>
-      <c r="F3" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" t="s">
         <v>137</v>
-      </c>
-      <c r="O3">
-        <v>10000</v>
       </c>
       <c r="P3">
         <v>10000</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -4284,58 +4290,61 @@
         <v>148</v>
       </c>
       <c r="D4" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" t="s">
         <v>137</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <f>100*8760</f>
         <v>876000</v>
       </c>
-      <c r="O4">
-        <v>10000</v>
-      </c>
       <c r="P4">
         <v>10000</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>137</v>
-      </c>
-      <c r="O5">
-        <v>10000</v>
       </c>
       <c r="P5">
         <v>10000</v>
       </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>137</v>
-      </c>
-      <c r="O6">
-        <v>10000</v>
       </c>
       <c r="P6">
         <v>10000</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>276</v>
       </c>
@@ -4345,41 +4354,41 @@
       <c r="C7" t="s">
         <v>148</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>148</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>137</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>422</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>419</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>420</v>
-      </c>
-      <c r="O7">
-        <v>12000</v>
       </c>
       <c r="P7">
         <v>12000</v>
       </c>
       <c r="Q7">
+        <v>12000</v>
+      </c>
+      <c r="R7">
         <v>20</v>
       </c>
-      <c r="AA7">
+      <c r="AB7">
         <v>0.01</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <v>0.1</v>
       </c>
-      <c r="AD7">
+      <c r="AE7">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>376</v>
       </c>
@@ -4389,54 +4398,57 @@
       <c r="C8" t="s">
         <v>148</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>148</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>137</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>446</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>419</v>
-      </c>
-      <c r="O8">
-        <v>12000</v>
       </c>
       <c r="P8">
         <v>12000</v>
       </c>
       <c r="Q8">
+        <v>12000</v>
+      </c>
+      <c r="R8">
         <v>10000000</v>
       </c>
-      <c r="AB8">
+      <c r="AC8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>300</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="F9" t="s">
+      <c r="D9" t="s">
+        <v>148</v>
+      </c>
+      <c r="G9" t="s">
         <v>433</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>800</v>
       </c>
-      <c r="V9" s="14">
+      <c r="W9" s="14">
         <v>200</v>
       </c>
-      <c r="X9" s="14">
+      <c r="Y9" s="14">
         <v>0.05</v>
       </c>
-      <c r="Z9">
+      <c r="AA9">
         <v>10</v>
       </c>
-      <c r="AF9">
+      <c r="AG9">
         <v>1</v>
       </c>
     </row>
@@ -8772,7 +8784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6AC2C8-7B82-4BFA-94A3-ECFAF63F0D5D}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>

</xml_diff>

<commit_message>
Changed excel to use import entity alternative
</commit_message>
<xml_diff>
--- a/FlexTool_import_template.xlsx
+++ b/FlexTool_import_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AETART\Documents\flextool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3666B95-CED2-4B47-8BC1-83CA851AFFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F467DBA0-B6A4-4F3E-BAF7-48BB6370D16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" activeTab="10" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" firstSheet="28" activeTab="39" xr2:uid="{D5BEC09F-8FA9-46E6-8F36-396DCDACE376}"/>
   </bookViews>
   <sheets>
     <sheet name="navigate" sheetId="54" r:id="rId1"/>
@@ -207,7 +207,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1463" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1455" uniqueCount="542">
   <si>
     <t>commodity</t>
   </si>
@@ -1040,9 +1040,6 @@
     <t>Battery</t>
   </si>
   <si>
-    <t>is_active</t>
-  </si>
-  <si>
     <t>timestep_duration</t>
   </si>
   <si>
@@ -1833,6 +1830,9 @@
   </si>
   <si>
     <t>inflow_weighted</t>
+  </si>
+  <si>
+    <t>Entity Alternative</t>
   </si>
 </sst>
 </file>
@@ -3619,7 +3619,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
@@ -3675,14 +3675,14 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="43" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B9" s="43"/>
       <c r="C9" s="43"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="43" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B10" s="43"/>
       <c r="C10" s="43"/>
@@ -3880,28 +3880,28 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="48" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="48" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="48" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B39" s="48"/>
       <c r="C39" s="48"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="48" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B40" s="48"/>
       <c r="C40" s="48"/>
@@ -4012,18 +4012,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4889F5-3956-475B-A853-BA105023BA1D}">
   <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -4063,43 +4064,43 @@
         <v>168</v>
       </c>
       <c r="E1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F1" t="s">
         <v>169</v>
       </c>
       <c r="G1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="H1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="J1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="K1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="M1" t="s">
         <v>157</v>
       </c>
       <c r="N1" t="s">
+        <v>451</v>
+      </c>
+      <c r="O1" t="s">
         <v>452</v>
       </c>
-      <c r="O1" t="s">
-        <v>453</v>
-      </c>
       <c r="P1" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q1" t="s">
         <v>342</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>343</v>
       </c>
       <c r="R1" t="s">
         <v>65</v>
@@ -4108,25 +4109,25 @@
         <v>68</v>
       </c>
       <c r="T1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="U1" t="s">
         <v>69</v>
       </c>
       <c r="V1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="W1" t="s">
+        <v>343</v>
+      </c>
+      <c r="X1" t="s">
         <v>344</v>
-      </c>
-      <c r="X1" t="s">
-        <v>345</v>
       </c>
       <c r="Y1" t="s">
         <v>19</v>
       </c>
       <c r="Z1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AA1" t="s">
         <v>22</v>
@@ -4135,19 +4136,19 @@
         <v>70</v>
       </c>
       <c r="AC1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AD1" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="AE1" t="s">
         <v>411</v>
       </c>
-      <c r="AE1" t="s">
-        <v>412</v>
-      </c>
       <c r="AF1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="AG1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4161,31 +4162,31 @@
         <v>58</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>277</v>
+        <v>541</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>246</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K2" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>413</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>414</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>59</v>
@@ -4194,7 +4195,7 @@
         <v>57</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>60</v>
@@ -4215,7 +4216,7 @@
         <v>14</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>7</v>
@@ -4236,22 +4237,22 @@
         <v>62</v>
       </c>
       <c r="AC2" s="9" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AD2" s="9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AE2" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="AF2" s="9" t="s">
         <v>416</v>
-      </c>
-      <c r="AF2" s="9" t="s">
-        <v>417</v>
       </c>
       <c r="AG2" s="9" t="s">
         <v>63</v>
       </c>
       <c r="AH2" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
@@ -4264,8 +4265,8 @@
       <c r="C3" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>148</v>
+      <c r="D3" t="b">
+        <v>1</v>
       </c>
       <c r="E3" s="14"/>
       <c r="F3" s="14"/>
@@ -4289,11 +4290,11 @@
       <c r="C4" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>148</v>
+      <c r="D4" t="b">
+        <v>1</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" t="s">
@@ -4361,13 +4362,13 @@
         <v>137</v>
       </c>
       <c r="J7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K7" t="s">
+        <v>418</v>
+      </c>
+      <c r="L7" t="s">
         <v>419</v>
-      </c>
-      <c r="L7" t="s">
-        <v>420</v>
       </c>
       <c r="P7">
         <v>12000</v>
@@ -4390,10 +4391,10 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C8" t="s">
         <v>148</v>
@@ -4405,10 +4406,10 @@
         <v>137</v>
       </c>
       <c r="J8" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="K8" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="P8">
         <v>12000</v>
@@ -4425,16 +4426,16 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="D9" t="s">
-        <v>148</v>
+      <c r="D9" t="b">
+        <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="S9">
         <v>800</v>
@@ -4457,7 +4458,8 @@
     <hyperlink ref="A1" location="navigate!A1" display="navigate" xr:uid="{8750FC4E-23A9-46B0-9138-4EFB651E5F58}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4499,7 +4501,7 @@
         <v>64</v>
       </c>
       <c r="E1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F1" t="s">
         <v>66</v>
@@ -4508,19 +4510,19 @@
         <v>67</v>
       </c>
       <c r="H1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I1" t="s">
+        <v>346</v>
+      </c>
+      <c r="J1" t="s">
         <v>347</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>343</v>
+      </c>
+      <c r="L1" t="s">
         <v>348</v>
-      </c>
-      <c r="K1" t="s">
-        <v>344</v>
-      </c>
-      <c r="L1" t="s">
-        <v>349</v>
       </c>
       <c r="M1" t="s">
         <v>19</v>
@@ -4529,7 +4531,7 @@
         <v>22</v>
       </c>
       <c r="O1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4546,7 +4548,7 @@
         <v>57</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>8</v>
@@ -4561,7 +4563,7 @@
         <v>13</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>7</v>
@@ -5002,7 +5004,7 @@
         <v>71</v>
       </c>
       <c r="D1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5078,7 +5080,7 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -5204,10 +5206,10 @@
   <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="V3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AJ19" sqref="AJ19"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5254,13 +5256,13 @@
         <v>167</v>
       </c>
       <c r="H1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="J1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="K1" t="s">
         <v>158</v>
@@ -5272,19 +5274,19 @@
         <v>21</v>
       </c>
       <c r="N1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="O1" t="s">
         <v>24</v>
       </c>
       <c r="P1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Q1" t="s">
+        <v>351</v>
+      </c>
+      <c r="R1" t="s">
         <v>352</v>
-      </c>
-      <c r="R1" t="s">
-        <v>353</v>
       </c>
       <c r="S1" t="s">
         <v>19</v>
@@ -5293,16 +5295,16 @@
         <v>22</v>
       </c>
       <c r="U1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="V1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="W1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="X1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -5318,8 +5320,8 @@
       <c r="D2" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="E2" s="24" t="s">
-        <v>277</v>
+      <c r="E2" s="9" t="s">
+        <v>541</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>17</v>
@@ -5331,7 +5333,7 @@
         <v>11</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>272</v>
@@ -5352,7 +5354,7 @@
         <v>14</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>7</v>
@@ -5370,7 +5372,7 @@
         <v>5</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="W2" s="9" t="s">
         <v>3</v>
@@ -5379,7 +5381,7 @@
         <v>63</v>
       </c>
       <c r="Y2" s="24" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -5395,8 +5397,8 @@
       <c r="D3" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="E3" t="s">
-        <v>148</v>
+      <c r="E3" t="b">
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>159</v>
@@ -5427,8 +5429,8 @@
       <c r="D4" s="11" t="s">
         <v>255</v>
       </c>
-      <c r="E4" t="s">
-        <v>148</v>
+      <c r="E4" t="b">
+        <v>1</v>
       </c>
       <c r="F4" t="s">
         <v>159</v>
@@ -5451,7 +5453,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>30</v>
@@ -5463,7 +5465,7 @@
         <v>139</v>
       </c>
       <c r="H5" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M5">
         <v>100</v>
@@ -5483,7 +5485,7 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>254</v>
@@ -5495,7 +5497,7 @@
         <v>255</v>
       </c>
       <c r="H6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M6">
         <v>100</v>
@@ -5560,19 +5562,19 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F1" t="s">
         <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H1" t="s">
+        <v>351</v>
+      </c>
+      <c r="I1" t="s">
         <v>352</v>
-      </c>
-      <c r="I1" t="s">
-        <v>353</v>
       </c>
       <c r="J1" t="s">
         <v>19</v>
@@ -5581,10 +5583,10 @@
         <v>22</v>
       </c>
       <c r="L1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -5607,7 +5609,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
@@ -5625,7 +5627,7 @@
         <v>5</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -6135,7 +6137,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B16" s="25">
         <v>44643</v>
@@ -6144,12 +6146,12 @@
         <v>175</v>
       </c>
       <c r="D16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B17" s="25">
         <v>44643</v>
@@ -6158,12 +6160,12 @@
         <v>175</v>
       </c>
       <c r="D17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B18" s="25">
         <v>44643</v>
@@ -6172,12 +6174,12 @@
         <v>175</v>
       </c>
       <c r="D18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B19" s="25">
         <v>44656</v>
@@ -6186,12 +6188,12 @@
         <v>175</v>
       </c>
       <c r="D19" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B20" s="25">
         <v>44657</v>
@@ -6200,12 +6202,12 @@
         <v>175</v>
       </c>
       <c r="D20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B21" s="25">
         <v>44657</v>
@@ -6214,12 +6216,12 @@
         <v>175</v>
       </c>
       <c r="D21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B22" s="25">
         <v>44680</v>
@@ -6228,12 +6230,12 @@
         <v>175</v>
       </c>
       <c r="D22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B23" s="25">
         <v>44680</v>
@@ -6242,12 +6244,12 @@
         <v>175</v>
       </c>
       <c r="D23" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B24" s="25">
         <v>44690</v>
@@ -6256,12 +6258,12 @@
         <v>175</v>
       </c>
       <c r="D24" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B25" s="25">
         <v>44695</v>
@@ -6270,12 +6272,12 @@
         <v>175</v>
       </c>
       <c r="D25" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B26" s="25">
         <v>44701</v>
@@ -6284,12 +6286,12 @@
         <v>175</v>
       </c>
       <c r="D26" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B27" s="25">
         <v>44701</v>
@@ -6298,12 +6300,12 @@
         <v>175</v>
       </c>
       <c r="D27" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B28" s="25">
         <v>44712</v>
@@ -6312,12 +6314,12 @@
         <v>175</v>
       </c>
       <c r="D28" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B29" s="25">
         <v>44727</v>
@@ -6326,12 +6328,12 @@
         <v>175</v>
       </c>
       <c r="D29" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B30" s="25">
         <v>44734</v>
@@ -6340,12 +6342,12 @@
         <v>175</v>
       </c>
       <c r="D30" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B31" s="25">
         <v>44741</v>
@@ -6354,12 +6356,12 @@
         <v>175</v>
       </c>
       <c r="D31" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B32" s="25">
         <v>44840</v>
@@ -6368,12 +6370,12 @@
         <v>175</v>
       </c>
       <c r="D32" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B33" s="25">
         <v>44850</v>
@@ -6382,12 +6384,12 @@
         <v>175</v>
       </c>
       <c r="D33" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B34" s="25">
         <v>44875</v>
@@ -6396,12 +6398,12 @@
         <v>175</v>
       </c>
       <c r="D34" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B35" s="25">
         <v>44876</v>
@@ -6410,12 +6412,12 @@
         <v>175</v>
       </c>
       <c r="D35" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B36" s="25">
         <v>44889</v>
@@ -6424,12 +6426,12 @@
         <v>175</v>
       </c>
       <c r="D36" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B37" s="25">
         <v>44893</v>
@@ -6438,12 +6440,12 @@
         <v>175</v>
       </c>
       <c r="D37" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B38" s="25">
         <v>44903</v>
@@ -6452,12 +6454,12 @@
         <v>175</v>
       </c>
       <c r="D38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B39" s="25">
         <v>45082</v>
@@ -6466,7 +6468,7 @@
         <v>175</v>
       </c>
       <c r="D39" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -6477,10 +6479,10 @@
         <v>45156</v>
       </c>
       <c r="C40" t="s">
+        <v>514</v>
+      </c>
+      <c r="D40" t="s">
         <v>515</v>
-      </c>
-      <c r="D40" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -6491,10 +6493,10 @@
         <v>45282</v>
       </c>
       <c r="C41" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D41" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
   </sheetData>
@@ -6508,10 +6510,10 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA7" sqref="AA7"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6552,19 +6554,19 @@
         <v>275</v>
       </c>
       <c r="D1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E1" t="s">
+        <v>469</v>
+      </c>
+      <c r="F1" t="s">
         <v>470</v>
       </c>
-      <c r="F1" t="s">
-        <v>471</v>
-      </c>
       <c r="G1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I1" t="s">
         <v>18</v>
@@ -6573,19 +6575,19 @@
         <v>21</v>
       </c>
       <c r="K1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L1" t="s">
         <v>24</v>
       </c>
       <c r="M1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="N1" t="s">
+        <v>354</v>
+      </c>
+      <c r="O1" t="s">
         <v>355</v>
-      </c>
-      <c r="O1" t="s">
-        <v>356</v>
       </c>
       <c r="P1" t="s">
         <v>19</v>
@@ -6594,7 +6596,7 @@
         <v>22</v>
       </c>
       <c r="R1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="S1" t="s">
         <v>158</v>
@@ -6603,10 +6605,10 @@
         <v>106</v>
       </c>
       <c r="U1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="V1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="W1" t="s">
         <v>180</v>
@@ -6615,7 +6617,7 @@
         <v>181</v>
       </c>
       <c r="Y1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" spans="1:26" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6625,8 +6627,8 @@
       <c r="B2" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>277</v>
+      <c r="C2" s="9" t="s">
+        <v>541</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>105</v>
@@ -6641,7 +6643,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="49" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I2" s="24" t="s">
         <v>4</v>
@@ -6656,7 +6658,7 @@
         <v>14</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="N2" s="24" t="s">
         <v>7</v>
@@ -6695,7 +6697,7 @@
         <v>63</v>
       </c>
       <c r="Z2" s="24" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -6705,11 +6707,11 @@
       <c r="B3" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="47" t="s">
-        <v>148</v>
+      <c r="C3" t="b">
+        <v>1</v>
       </c>
       <c r="D3" s="47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E3" s="47" t="s">
         <v>160</v>
@@ -6746,8 +6748,8 @@
       <c r="B4" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C4" s="47" t="s">
-        <v>148</v>
+      <c r="C4" t="b">
+        <v>1</v>
       </c>
       <c r="D4" s="47" t="s">
         <v>249</v>
@@ -6777,14 +6779,14 @@
       <c r="B5" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C5" s="47" t="s">
-        <v>148</v>
+      <c r="C5" t="b">
+        <v>1</v>
       </c>
       <c r="D5" s="47" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E5" s="47" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F5" s="47"/>
       <c r="G5" s="47" t="s">
@@ -6803,28 +6805,28 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>141</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H6" s="47"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="C7" s="47" t="s">
-        <v>148</v>
+      <c r="C7" t="b">
+        <v>1</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E7" s="47" t="s">
         <v>160</v>
@@ -6886,19 +6888,19 @@
         <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F1" t="s">
         <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H1" t="s">
+        <v>354</v>
+      </c>
+      <c r="I1" t="s">
         <v>355</v>
-      </c>
-      <c r="I1" t="s">
-        <v>356</v>
       </c>
       <c r="J1" t="s">
         <v>19</v>
@@ -6907,7 +6909,7 @@
         <v>22</v>
       </c>
       <c r="L1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M1" t="s">
         <v>158</v>
@@ -6933,7 +6935,7 @@
         <v>13</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>7</v>
@@ -7294,10 +7296,10 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G1" t="s">
         <v>237</v>
@@ -7306,16 +7308,16 @@
         <v>236</v>
       </c>
       <c r="I1" t="s">
+        <v>473</v>
+      </c>
+      <c r="J1" t="s">
+        <v>356</v>
+      </c>
+      <c r="K1" t="s">
         <v>474</v>
       </c>
-      <c r="J1" t="s">
-        <v>357</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>475</v>
-      </c>
-      <c r="L1" t="s">
-        <v>476</v>
       </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -7332,13 +7334,13 @@
         <v>56</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>133</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>270</v>
@@ -7373,7 +7375,7 @@
         <v>140</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -7396,7 +7398,7 @@
         <v>138</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -7416,7 +7418,7 @@
         <v>149</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -7433,7 +7435,7 @@
         <v>139</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -7453,7 +7455,7 @@
         <v>138</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -7464,16 +7466,16 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>149</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -7481,16 +7483,16 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -7498,16 +7500,16 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>377</v>
-      </c>
       <c r="C10" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -7557,7 +7559,7 @@
         <v>161</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7583,10 +7585,10 @@
         <v>26</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>317</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -7826,7 +7828,7 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -7846,7 +7848,7 @@
         <v>256</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -8484,16 +8486,16 @@
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C4" s="18" t="s">
+        <v>382</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>384</v>
-      </c>
       <c r="E4" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -8549,13 +8551,13 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F1" t="s">
         <v>39</v>
@@ -8564,7 +8566,7 @@
         <v>35</v>
       </c>
       <c r="H1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I1" t="s">
         <v>41</v>
@@ -8573,7 +8575,7 @@
         <v>45</v>
       </c>
       <c r="K1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L1" t="s">
         <v>43</v>
@@ -8582,19 +8584,19 @@
         <v>53</v>
       </c>
       <c r="N1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="O1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="P1" t="s">
         <v>37</v>
       </c>
       <c r="Q1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="R1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="S1" t="s">
         <v>47</v>
@@ -8603,19 +8605,19 @@
         <v>51</v>
       </c>
       <c r="U1" t="s">
+        <v>321</v>
+      </c>
+      <c r="V1" t="s">
         <v>322</v>
       </c>
-      <c r="V1" t="s">
-        <v>323</v>
-      </c>
       <c r="W1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="X1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Y1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -8626,13 +8628,13 @@
         <v>55</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>518</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>519</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>520</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>38</v>
@@ -8641,7 +8643,7 @@
         <v>34</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>40</v>
@@ -8662,13 +8664,13 @@
         <v>273</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="P2" s="9" t="s">
         <v>36</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="R2" s="24" t="s">
         <v>11</v>
@@ -8680,19 +8682,19 @@
         <v>50</v>
       </c>
       <c r="U2" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="V2" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="V2" s="9" t="s">
-        <v>321</v>
-      </c>
       <c r="W2" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="X2" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="X2" s="9" t="s">
-        <v>338</v>
-      </c>
       <c r="Y2" s="9" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -8732,7 +8734,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>267</v>
@@ -8746,10 +8748,10 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="U6">
         <v>40</v>
@@ -8763,13 +8765,13 @@
         <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C7" t="s">
         <v>148</v>
       </c>
       <c r="Y7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -8802,7 +8804,7 @@
         <v>230</v>
       </c>
       <c r="B1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8811,42 +8813,42 @@
         <v>27</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>276</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>364</v>
-      </c>
       <c r="L2" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>27</v>
@@ -8887,94 +8889,94 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>276</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G4" t="s">
         <v>276</v>
       </c>
       <c r="H4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="J4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B5" s="14"/>
       <c r="G5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J5" t="s">
+        <v>362</v>
+      </c>
+      <c r="K5" t="s">
         <v>363</v>
       </c>
-      <c r="K5" t="s">
-        <v>364</v>
-      </c>
       <c r="L5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -9032,7 +9034,7 @@
         <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I1" t="s">
         <v>46</v>
@@ -9041,16 +9043,16 @@
         <v>49</v>
       </c>
       <c r="K1" t="s">
+        <v>321</v>
+      </c>
+      <c r="L1" t="s">
         <v>322</v>
       </c>
-      <c r="L1" t="s">
-        <v>323</v>
-      </c>
       <c r="M1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="N1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -9076,7 +9078,7 @@
         <v>36</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>9</v>
@@ -9085,16 +9087,16 @@
         <v>48</v>
       </c>
       <c r="K2" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>320</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>321</v>
-      </c>
       <c r="M2" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="N2" s="9" t="s">
         <v>337</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -9286,7 +9288,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>138</v>
@@ -9294,7 +9296,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>139</v>
@@ -9382,7 +9384,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>141</v>
@@ -9393,7 +9395,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>151</v>
@@ -9442,7 +9444,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G1" t="s">
         <v>132</v>
@@ -9497,7 +9499,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>269</v>
@@ -9558,16 +9560,16 @@
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F1" t="s">
         <v>129</v>
       </c>
       <c r="G1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -9610,7 +9612,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>269</v>
@@ -9861,7 +9863,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G1" t="s">
         <v>131</v>
@@ -9916,7 +9918,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>269</v>
@@ -9939,7 +9941,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>269</v>
@@ -9962,7 +9964,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>269</v>
@@ -9985,7 +9987,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>269</v>
@@ -10008,7 +10010,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>269</v>
@@ -10071,7 +10073,7 @@
         <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F1" t="s">
         <v>73</v>
@@ -10094,19 +10096,19 @@
         <v>190</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>187</v>
       </c>
       <c r="H2" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>503</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -10154,7 +10156,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
@@ -10174,7 +10176,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>32</v>
@@ -10194,7 +10196,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>152</v>
@@ -10214,7 +10216,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>33</v>
@@ -10234,7 +10236,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>33</v>
@@ -10254,7 +10256,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>183</v>
@@ -10288,98 +10290,109 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C017E3-B844-46CF-8B82-D76F5D9D7ACD}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
-    <col min="4" max="8" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="9" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>230</v>
       </c>
       <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" t="s">
+      <c r="C1" t="s">
         <v>147</v>
       </c>
-      <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="D4">
+      <c r="E4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="D5">
+        <v>430</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E5">
         <v>0</v>
       </c>
     </row>
@@ -10388,6 +10401,7 @@
     <hyperlink ref="A1" location="navigate!A1" display="navigate" xr:uid="{C203C3C8-4694-4AC0-9CF9-47EC8DF4B8CC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10422,7 +10436,7 @@
       <c r="D1" s="3"/>
       <c r="E1"/>
       <c r="F1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -10436,13 +10450,13 @@
         <v>56</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>134</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -10456,7 +10470,7 @@
         <v>140</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>164</v>
@@ -10476,7 +10490,7 @@
         <v>138</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>164</v>
@@ -10487,19 +10501,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>149</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -10507,19 +10521,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>376</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>377</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>138</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F6">
         <v>4</v>
@@ -10562,7 +10576,7 @@
       <c r="C1"/>
       <c r="D1"/>
       <c r="E1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10579,7 +10593,7 @@
         <v>134</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
   </sheetData>
@@ -10618,10 +10632,10 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
+        <v>395</v>
+      </c>
+      <c r="E1" t="s">
         <v>396</v>
-      </c>
-      <c r="E1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -10635,21 +10649,21 @@
         <v>134</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>398</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>255</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -10690,7 +10704,7 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10704,7 +10718,7 @@
         <v>134</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -10742,7 +10756,7 @@
       <c r="B1"/>
       <c r="C1"/>
       <c r="D1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -10756,18 +10770,18 @@
         <v>134</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>254</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D3">
         <v>-8</v>
@@ -10809,13 +10823,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C2" s="51" t="s">
+        <v>522</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>523</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -10823,10 +10837,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -10834,10 +10848,10 @@
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -10845,10 +10859,10 @@
         <v>27</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -10856,10 +10870,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D6" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -10867,10 +10881,10 @@
         <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -10878,13 +10892,13 @@
         <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>148</v>
       </c>
       <c r="D8" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -10926,28 +10940,28 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F1" t="s">
+        <v>464</v>
+      </c>
+      <c r="G1" t="s">
+        <v>442</v>
+      </c>
+      <c r="H1" t="s">
         <v>465</v>
       </c>
-      <c r="G1" t="s">
-        <v>443</v>
-      </c>
-      <c r="H1" t="s">
-        <v>466</v>
-      </c>
       <c r="I1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="J1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -10961,49 +10975,49 @@
         <v>156</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="G2" s="9" t="s">
-        <v>442</v>
-      </c>
       <c r="H2" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K2" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="M2" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="N2" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="M2" s="9" t="s">
-        <v>489</v>
-      </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>492</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>493</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>494</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -11014,158 +11028,158 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F3" t="s">
+        <v>443</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>445</v>
-      </c>
       <c r="H3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F4" t="s">
+        <v>443</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>445</v>
-      </c>
       <c r="H4" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>152</v>
       </c>
       <c r="C5" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F5" t="s">
+        <v>443</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>445</v>
-      </c>
       <c r="H5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F6" t="s">
+        <v>443</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>445</v>
-      </c>
       <c r="H6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>183</v>
       </c>
       <c r="C7" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F7" t="s">
+        <v>443</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>445</v>
-      </c>
       <c r="H7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>152</v>
       </c>
       <c r="E9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>183</v>
       </c>
       <c r="E11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G11" s="5"/>
     </row>
@@ -11205,13 +11219,13 @@
       </c>
       <c r="B1" s="3"/>
       <c r="C1" t="s">
+        <v>509</v>
+      </c>
+      <c r="D1" t="s">
         <v>510</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>511</v>
-      </c>
-      <c r="E1" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -11222,13 +11236,13 @@
         <v>74</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>513</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>514</v>
-      </c>
       <c r="E2" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
@@ -11268,7 +11282,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>32</v>
@@ -11282,7 +11296,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>152</v>
@@ -11296,7 +11310,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>33</v>
@@ -11310,7 +11324,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>183</v>
@@ -11324,7 +11338,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>32</v>
@@ -11333,7 +11347,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>152</v>
@@ -11342,7 +11356,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>33</v>
@@ -11351,7 +11365,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>183</v>
@@ -11412,7 +11426,7 @@
         <v>191</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -11493,7 +11507,7 @@
         <v>192</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>